<commit_message>
Update Master Gantt Chart
Updated my section of the Master Gantt chart. I need to make sure of something, so do not put anything in yet!
</commit_message>
<xml_diff>
--- a/383Game/Doc/Brain Stew Master Gantt Chart.xlsx
+++ b/383Game/Doc/Brain Stew Master Gantt Chart.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kayra\OneDrive\Masaüstü\Computer Science Courses\CS383 General Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/19db3ad368368567/Documents/GitHub/CS383BrainstewGame/383Game/Doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D882C50A-A854-46FC-B030-85083B1171DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="60" documentId="8_{D882C50A-A854-46FC-B030-85083B1171DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DBA05435-58E4-4E5E-956B-0E531A57CF06}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{6C77CEAA-6C20-4875-8E69-F182CEDC365C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{6C77CEAA-6C20-4875-8E69-F182CEDC365C}"/>
   </bookViews>
   <sheets>
     <sheet name="Gantt" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="33">
   <si>
     <t>Cory Clairmont</t>
   </si>
@@ -105,6 +105,39 @@
   </si>
   <si>
     <t>Deliverables should be on GitHub by midnight on Due Date and marked with a check (✓) mark under.</t>
+  </si>
+  <si>
+    <t>Begin the level design process</t>
+  </si>
+  <si>
+    <t>Create and set up backgrounds</t>
+  </si>
+  <si>
+    <t>Arrange tiles to form the map</t>
+  </si>
+  <si>
+    <t>Add physics component</t>
+  </si>
+  <si>
+    <t>Add interactive elements</t>
+  </si>
+  <si>
+    <t>Add objectives</t>
+  </si>
+  <si>
+    <t>Create cutscenes</t>
+  </si>
+  <si>
+    <t>Implement checkpoints</t>
+  </si>
+  <si>
+    <t>Documentation</t>
+  </si>
+  <si>
+    <t>Debugging and testing</t>
+  </si>
+  <si>
+    <t>Installation and finalize</t>
   </si>
 </sst>
 </file>
@@ -243,7 +276,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -267,8 +300,14 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -279,12 +318,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -300,10 +338,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -623,9 +657,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E50249A2-2F05-400B-B05E-0C14F827A1C5}">
-  <dimension ref="A1:BL47"/>
+  <dimension ref="A1:BL51"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -979,71 +1015,226 @@
       <c r="B32" s="2"/>
       <c r="D32" s="10"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="3"/>
-      <c r="B33" s="3"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" s="3"/>
-      <c r="B34" s="3"/>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" s="3"/>
-      <c r="B35" s="3"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" s="3"/>
-      <c r="B36" s="3"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" s="3"/>
-      <c r="B37" s="3"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38" s="3"/>
-      <c r="B38" s="3"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" s="3"/>
-      <c r="B39" s="3"/>
-    </row>
-    <row r="40" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="2" t="s">
+    <row r="33" spans="1:50" x14ac:dyDescent="0.3">
+      <c r="A33" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B33" s="21">
+        <v>7</v>
+      </c>
+      <c r="D33" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="E33" s="22"/>
+      <c r="F33" s="22"/>
+      <c r="G33" s="22"/>
+      <c r="H33" s="22"/>
+      <c r="I33" s="22"/>
+      <c r="J33" s="22"/>
+      <c r="K33" s="22"/>
+    </row>
+    <row r="34" spans="1:50" x14ac:dyDescent="0.3">
+      <c r="A34" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B34" s="21">
+        <v>7</v>
+      </c>
+      <c r="D34" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="L34" s="22"/>
+      <c r="M34" s="22"/>
+      <c r="N34" s="22"/>
+      <c r="O34" s="22"/>
+      <c r="P34" s="22"/>
+      <c r="Q34" s="22"/>
+      <c r="R34" s="22"/>
+    </row>
+    <row r="35" spans="1:50" x14ac:dyDescent="0.3">
+      <c r="A35" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B35" s="21">
+        <v>8</v>
+      </c>
+      <c r="D35" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="L35" s="22"/>
+      <c r="M35" s="22"/>
+      <c r="N35" s="22"/>
+      <c r="O35" s="22"/>
+      <c r="P35" s="22"/>
+      <c r="Q35" s="22"/>
+      <c r="R35" s="22"/>
+      <c r="S35" s="22"/>
+    </row>
+    <row r="36" spans="1:50" x14ac:dyDescent="0.3">
+      <c r="A36" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B36" s="21">
+        <v>4</v>
+      </c>
+      <c r="D36" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="S36" s="22"/>
+      <c r="T36" s="22"/>
+      <c r="U36" s="22"/>
+      <c r="V36" s="22"/>
+    </row>
+    <row r="37" spans="1:50" x14ac:dyDescent="0.3">
+      <c r="A37" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B37" s="21">
+        <v>6</v>
+      </c>
+      <c r="D37" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="W37" s="22"/>
+      <c r="X37" s="22"/>
+      <c r="Y37" s="22"/>
+      <c r="Z37" s="22"/>
+      <c r="AA37" s="22"/>
+      <c r="AB37" s="22"/>
+    </row>
+    <row r="38" spans="1:50" x14ac:dyDescent="0.3">
+      <c r="A38" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B38" s="21">
+        <v>6</v>
+      </c>
+      <c r="D38" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="W38" s="22"/>
+      <c r="X38" s="22"/>
+      <c r="Y38" s="22"/>
+      <c r="Z38" s="22"/>
+      <c r="AA38" s="22"/>
+      <c r="AB38" s="22"/>
+    </row>
+    <row r="39" spans="1:50" x14ac:dyDescent="0.3">
+      <c r="A39" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B39" s="21">
         <v>5</v>
       </c>
-      <c r="B40" s="2"/>
-      <c r="D40" s="10"/>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" s="3"/>
-      <c r="B41" s="3"/>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" s="3"/>
-      <c r="B42" s="3"/>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" s="3"/>
-      <c r="B43" s="3"/>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" s="3"/>
-      <c r="B44" s="3"/>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D39" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC39" s="22"/>
+      <c r="AD39" s="22"/>
+      <c r="AE39" s="22"/>
+      <c r="AF39" s="22"/>
+      <c r="AG39" s="22"/>
+    </row>
+    <row r="40" spans="1:50" x14ac:dyDescent="0.3">
+      <c r="A40" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B40" s="21">
+        <v>6</v>
+      </c>
+      <c r="D40" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="AH40" s="22"/>
+      <c r="AI40" s="22"/>
+      <c r="AJ40" s="22"/>
+      <c r="AK40" s="22"/>
+      <c r="AL40" s="22"/>
+      <c r="AM40" s="22"/>
+    </row>
+    <row r="41" spans="1:50" x14ac:dyDescent="0.3">
+      <c r="A41" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B41" s="21">
+        <v>4</v>
+      </c>
+      <c r="D41" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="AL41" s="22"/>
+      <c r="AM41" s="22"/>
+      <c r="AN41" s="22"/>
+      <c r="AO41" s="22"/>
+    </row>
+    <row r="42" spans="1:50" x14ac:dyDescent="0.3">
+      <c r="A42" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B42" s="21">
+        <v>6</v>
+      </c>
+      <c r="D42" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="AP42" s="22"/>
+      <c r="AQ42" s="22"/>
+      <c r="AR42" s="22"/>
+      <c r="AS42" s="22"/>
+      <c r="AT42" s="22"/>
+      <c r="AU42" s="22"/>
+    </row>
+    <row r="43" spans="1:50" x14ac:dyDescent="0.3">
+      <c r="A43" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B43" s="21">
+        <v>4</v>
+      </c>
+      <c r="D43" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="AV43" s="22"/>
+      <c r="AW43" s="22"/>
+      <c r="AX43" s="22"/>
+    </row>
+    <row r="44" spans="1:50" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B44" s="2"/>
+      <c r="D44" s="10"/>
+    </row>
+    <row r="45" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A45" s="3"/>
       <c r="B45" s="3"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A46" s="3"/>
       <c r="B46" s="3"/>
     </row>
-    <row r="47" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="2" t="s">
+    <row r="47" spans="1:50" x14ac:dyDescent="0.3">
+      <c r="A47" s="3"/>
+      <c r="B47" s="3"/>
+    </row>
+    <row r="48" spans="1:50" x14ac:dyDescent="0.3">
+      <c r="A48" s="3"/>
+      <c r="B48" s="3"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49" s="3"/>
+      <c r="B49" s="3"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50" s="3"/>
+      <c r="B50" s="3"/>
+    </row>
+    <row r="51" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B47" s="2"/>
-      <c r="D47" s="10"/>
+      <c r="B51" s="2"/>
+      <c r="D51" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1057,296 +1248,296 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00EB45AB-5FDF-4145-A8A6-9382A724B0A8}">
   <dimension ref="A2:S15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="2" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20" t="s">
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20" t="s">
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20" t="s">
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="L2" s="20"/>
-      <c r="M2" s="20"/>
-      <c r="N2" s="20" t="s">
+      <c r="L2" s="15"/>
+      <c r="M2" s="15"/>
+      <c r="N2" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="O2" s="20"/>
-      <c r="P2" s="20"/>
-      <c r="Q2" s="20" t="s">
+      <c r="O2" s="15"/>
+      <c r="P2" s="15"/>
+      <c r="Q2" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="R2" s="20"/>
-      <c r="S2" s="20"/>
+      <c r="R2" s="15"/>
+      <c r="S2" s="15"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15" t="s">
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15" t="s">
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="15"/>
-      <c r="J3" s="15"/>
-      <c r="K3" s="15" t="s">
+      <c r="I3" s="16"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="L3" s="15"/>
-      <c r="M3" s="15"/>
-      <c r="N3" s="15" t="s">
+      <c r="L3" s="16"/>
+      <c r="M3" s="16"/>
+      <c r="N3" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="O3" s="15"/>
-      <c r="P3" s="15"/>
-      <c r="Q3" s="15" t="s">
+      <c r="O3" s="16"/>
+      <c r="P3" s="16"/>
+      <c r="Q3" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="R3" s="15"/>
-      <c r="S3" s="15"/>
+      <c r="R3" s="16"/>
+      <c r="S3" s="16"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="B4" s="19"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="19"/>
-      <c r="I4" s="19"/>
-      <c r="J4" s="19"/>
-      <c r="K4" s="19"/>
-      <c r="L4" s="19"/>
-      <c r="M4" s="19"/>
-      <c r="N4" s="19"/>
-      <c r="O4" s="19"/>
-      <c r="P4" s="19"/>
-      <c r="Q4" s="19"/>
-      <c r="R4" s="19"/>
-      <c r="S4" s="19"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="17"/>
+      <c r="K4" s="17"/>
+      <c r="L4" s="17"/>
+      <c r="M4" s="17"/>
+      <c r="N4" s="17"/>
+      <c r="O4" s="17"/>
+      <c r="P4" s="17"/>
+      <c r="Q4" s="17"/>
+      <c r="R4" s="17"/>
+      <c r="S4" s="17"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="B5" s="19"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="19"/>
-      <c r="H5" s="19"/>
-      <c r="I5" s="19"/>
-      <c r="J5" s="19"/>
-      <c r="K5" s="19"/>
-      <c r="L5" s="19"/>
-      <c r="M5" s="19"/>
-      <c r="N5" s="19"/>
-      <c r="O5" s="19"/>
-      <c r="P5" s="19"/>
-      <c r="Q5" s="19"/>
-      <c r="R5" s="19"/>
-      <c r="S5" s="19"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="17"/>
+      <c r="K5" s="17"/>
+      <c r="L5" s="17"/>
+      <c r="M5" s="17"/>
+      <c r="N5" s="17"/>
+      <c r="O5" s="17"/>
+      <c r="P5" s="17"/>
+      <c r="Q5" s="17"/>
+      <c r="R5" s="17"/>
+      <c r="S5" s="17"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="B6" s="19"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="19"/>
-      <c r="I6" s="19"/>
-      <c r="J6" s="19"/>
-      <c r="K6" s="19"/>
-      <c r="L6" s="19"/>
-      <c r="M6" s="19"/>
-      <c r="N6" s="19"/>
-      <c r="O6" s="19"/>
-      <c r="P6" s="19"/>
-      <c r="Q6" s="19"/>
-      <c r="R6" s="19"/>
-      <c r="S6" s="19"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="17"/>
+      <c r="J6" s="17"/>
+      <c r="K6" s="17"/>
+      <c r="L6" s="17"/>
+      <c r="M6" s="17"/>
+      <c r="N6" s="17"/>
+      <c r="O6" s="17"/>
+      <c r="P6" s="17"/>
+      <c r="Q6" s="17"/>
+      <c r="R6" s="17"/>
+      <c r="S6" s="17"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="B7" s="19"/>
-      <c r="C7" s="19"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="19"/>
-      <c r="F7" s="19"/>
-      <c r="G7" s="19"/>
-      <c r="H7" s="19"/>
-      <c r="I7" s="19"/>
-      <c r="J7" s="19"/>
-      <c r="K7" s="19"/>
-      <c r="L7" s="19"/>
-      <c r="M7" s="19"/>
-      <c r="N7" s="19"/>
-      <c r="O7" s="19"/>
-      <c r="P7" s="19"/>
-      <c r="Q7" s="19"/>
-      <c r="R7" s="19"/>
-      <c r="S7" s="19"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="17"/>
+      <c r="J7" s="17"/>
+      <c r="K7" s="17"/>
+      <c r="L7" s="17"/>
+      <c r="M7" s="17"/>
+      <c r="N7" s="17"/>
+      <c r="O7" s="17"/>
+      <c r="P7" s="17"/>
+      <c r="Q7" s="17"/>
+      <c r="R7" s="17"/>
+      <c r="S7" s="17"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="B8" s="19"/>
-      <c r="C8" s="19"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="19"/>
-      <c r="F8" s="19"/>
-      <c r="G8" s="19"/>
-      <c r="H8" s="19"/>
-      <c r="I8" s="19"/>
-      <c r="J8" s="19"/>
-      <c r="K8" s="19"/>
-      <c r="L8" s="19"/>
-      <c r="M8" s="19"/>
-      <c r="N8" s="19"/>
-      <c r="O8" s="19"/>
-      <c r="P8" s="19"/>
-      <c r="Q8" s="19"/>
-      <c r="R8" s="19"/>
-      <c r="S8" s="19"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="17"/>
+      <c r="J8" s="17"/>
+      <c r="K8" s="17"/>
+      <c r="L8" s="17"/>
+      <c r="M8" s="17"/>
+      <c r="N8" s="17"/>
+      <c r="O8" s="17"/>
+      <c r="P8" s="17"/>
+      <c r="Q8" s="17"/>
+      <c r="R8" s="17"/>
+      <c r="S8" s="17"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="B9" s="19"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="19"/>
-      <c r="G9" s="19"/>
-      <c r="H9" s="19"/>
-      <c r="I9" s="19"/>
-      <c r="J9" s="19"/>
-      <c r="K9" s="19"/>
-      <c r="L9" s="19"/>
-      <c r="M9" s="19"/>
-      <c r="N9" s="19"/>
-      <c r="O9" s="19"/>
-      <c r="P9" s="19"/>
-      <c r="Q9" s="19"/>
-      <c r="R9" s="19"/>
-      <c r="S9" s="19"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="17"/>
+      <c r="K9" s="17"/>
+      <c r="L9" s="17"/>
+      <c r="M9" s="17"/>
+      <c r="N9" s="17"/>
+      <c r="O9" s="17"/>
+      <c r="P9" s="17"/>
+      <c r="Q9" s="17"/>
+      <c r="R9" s="17"/>
+      <c r="S9" s="17"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="B10" s="19"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="19"/>
-      <c r="I10" s="19"/>
-      <c r="J10" s="19"/>
-      <c r="K10" s="19"/>
-      <c r="L10" s="19"/>
-      <c r="M10" s="19"/>
-      <c r="N10" s="19"/>
-      <c r="O10" s="19"/>
-      <c r="P10" s="19"/>
-      <c r="Q10" s="19"/>
-      <c r="R10" s="19"/>
-      <c r="S10" s="19"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="17"/>
+      <c r="K10" s="17"/>
+      <c r="L10" s="17"/>
+      <c r="M10" s="17"/>
+      <c r="N10" s="17"/>
+      <c r="O10" s="17"/>
+      <c r="P10" s="17"/>
+      <c r="Q10" s="17"/>
+      <c r="R10" s="17"/>
+      <c r="S10" s="17"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="B11" s="19"/>
-      <c r="C11" s="19"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="19"/>
-      <c r="F11" s="19"/>
-      <c r="G11" s="19"/>
-      <c r="H11" s="19"/>
-      <c r="I11" s="19"/>
-      <c r="J11" s="19"/>
-      <c r="K11" s="19"/>
-      <c r="L11" s="19"/>
-      <c r="M11" s="19"/>
-      <c r="N11" s="19"/>
-      <c r="O11" s="19"/>
-      <c r="P11" s="19"/>
-      <c r="Q11" s="19"/>
-      <c r="R11" s="19"/>
-      <c r="S11" s="19"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="17"/>
+      <c r="J11" s="17"/>
+      <c r="K11" s="17"/>
+      <c r="L11" s="17"/>
+      <c r="M11" s="17"/>
+      <c r="N11" s="17"/>
+      <c r="O11" s="17"/>
+      <c r="P11" s="17"/>
+      <c r="Q11" s="17"/>
+      <c r="R11" s="17"/>
+      <c r="S11" s="17"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="B12" s="19"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="19"/>
-      <c r="G12" s="19"/>
-      <c r="H12" s="19"/>
-      <c r="I12" s="19"/>
-      <c r="J12" s="19"/>
-      <c r="K12" s="19"/>
-      <c r="L12" s="19"/>
-      <c r="M12" s="19"/>
-      <c r="N12" s="19"/>
-      <c r="O12" s="19"/>
-      <c r="P12" s="19"/>
-      <c r="Q12" s="19"/>
-      <c r="R12" s="19"/>
-      <c r="S12" s="19"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="17"/>
+      <c r="J12" s="17"/>
+      <c r="K12" s="17"/>
+      <c r="L12" s="17"/>
+      <c r="M12" s="17"/>
+      <c r="N12" s="17"/>
+      <c r="O12" s="17"/>
+      <c r="P12" s="17"/>
+      <c r="Q12" s="17"/>
+      <c r="R12" s="17"/>
+      <c r="S12" s="17"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="B13" s="19"/>
-      <c r="C13" s="19"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="19"/>
-      <c r="F13" s="19"/>
-      <c r="G13" s="19"/>
-      <c r="H13" s="19"/>
-      <c r="I13" s="19"/>
-      <c r="J13" s="19"/>
-      <c r="K13" s="19"/>
-      <c r="L13" s="19"/>
-      <c r="M13" s="19"/>
-      <c r="N13" s="19"/>
-      <c r="O13" s="19"/>
-      <c r="P13" s="19"/>
-      <c r="Q13" s="19"/>
-      <c r="R13" s="19"/>
-      <c r="S13" s="19"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="17"/>
+      <c r="J13" s="17"/>
+      <c r="K13" s="17"/>
+      <c r="L13" s="17"/>
+      <c r="M13" s="17"/>
+      <c r="N13" s="17"/>
+      <c r="O13" s="17"/>
+      <c r="P13" s="17"/>
+      <c r="Q13" s="17"/>
+      <c r="R13" s="17"/>
+      <c r="S13" s="17"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" s="9"/>
-      <c r="B14" s="16"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="18"/>
-      <c r="H14" s="16"/>
-      <c r="I14" s="17"/>
-      <c r="J14" s="18"/>
-      <c r="K14" s="15"/>
-      <c r="L14" s="15"/>
-      <c r="M14" s="15"/>
-      <c r="N14" s="15"/>
-      <c r="O14" s="15"/>
-      <c r="P14" s="15"/>
-      <c r="Q14" s="15"/>
-      <c r="R14" s="15"/>
-      <c r="S14" s="15"/>
+      <c r="B14" s="18"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="18"/>
+      <c r="I14" s="19"/>
+      <c r="J14" s="20"/>
+      <c r="K14" s="16"/>
+      <c r="L14" s="16"/>
+      <c r="M14" s="16"/>
+      <c r="N14" s="16"/>
+      <c r="O14" s="16"/>
+      <c r="P14" s="16"/>
+      <c r="Q14" s="16"/>
+      <c r="R14" s="16"/>
+      <c r="S14" s="16"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B15" s="12" t="s">
@@ -1363,12 +1554,12 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="Q2:S2"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="K2:M2"/>
-    <mergeCell ref="N2:P2"/>
+    <mergeCell ref="K14:M14"/>
+    <mergeCell ref="N14:P14"/>
+    <mergeCell ref="Q14:S14"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="H14:J14"/>
     <mergeCell ref="N3:P3"/>
     <mergeCell ref="Q3:S3"/>
     <mergeCell ref="B4:D13"/>
@@ -1381,12 +1572,12 @@
     <mergeCell ref="E3:G3"/>
     <mergeCell ref="H3:J3"/>
     <mergeCell ref="K3:M3"/>
-    <mergeCell ref="K14:M14"/>
-    <mergeCell ref="N14:P14"/>
-    <mergeCell ref="Q14:S14"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="H14:J14"/>
+    <mergeCell ref="Q2:S2"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="K2:M2"/>
+    <mergeCell ref="N2:P2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Brain Stew Master Gantt Chart.xlsx
</commit_message>
<xml_diff>
--- a/383Game/Doc/Brain Stew Master Gantt Chart.xlsx
+++ b/383Game/Doc/Brain Stew Master Gantt Chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aneeshashrestha/Documents/GitHub/CS383BrainstewGame/383Game/Doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{793C14F1-A52F-9746-91B6-723DB09700AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70A8E916-2475-7441-8076-219DB8BADA7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{6C77CEAA-6C20-4875-8E69-F182CEDC365C}"/>
   </bookViews>
@@ -704,7 +704,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -845,6 +845,13 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1338,8 +1345,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E50249A2-2F05-400B-B05E-0C14F827A1C5}">
   <dimension ref="A1:CRB103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L98" sqref="L98"/>
+    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I91" sqref="I91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -3004,7 +3011,7 @@
       <c r="C79" s="58">
         <v>0</v>
       </c>
-      <c r="D79" s="59"/>
+      <c r="D79" s="64"/>
       <c r="E79" s="59"/>
       <c r="F79" s="57"/>
       <c r="G79" s="57"/>
@@ -3054,7 +3061,7 @@
       <c r="C80" s="58">
         <v>1</v>
       </c>
-      <c r="D80" s="57"/>
+      <c r="D80" s="65"/>
       <c r="E80" s="57"/>
       <c r="F80" s="61"/>
       <c r="G80" s="61"/>
@@ -3104,7 +3111,7 @@
       <c r="C81" s="58">
         <v>1</v>
       </c>
-      <c r="D81" s="57"/>
+      <c r="D81" s="65"/>
       <c r="E81" s="57"/>
       <c r="F81" s="61"/>
       <c r="G81" s="61"/>
@@ -3154,7 +3161,7 @@
       <c r="C82" s="58">
         <v>1</v>
       </c>
-      <c r="D82" s="57"/>
+      <c r="D82" s="65"/>
       <c r="E82" s="57"/>
       <c r="F82" s="61"/>
       <c r="G82" s="61"/>
@@ -3204,7 +3211,7 @@
       <c r="C83" s="58" t="s">
         <v>136</v>
       </c>
-      <c r="D83" s="57"/>
+      <c r="D83" s="65"/>
       <c r="E83" s="57"/>
       <c r="F83" s="57"/>
       <c r="G83" s="57"/>
@@ -3254,7 +3261,7 @@
       <c r="C84" s="58" t="s">
         <v>137</v>
       </c>
-      <c r="D84" s="57"/>
+      <c r="D84" s="65"/>
       <c r="E84" s="57"/>
       <c r="F84" s="57"/>
       <c r="G84" s="57"/>
@@ -3304,7 +3311,7 @@
       <c r="C85" s="58" t="s">
         <v>71</v>
       </c>
-      <c r="D85" s="57"/>
+      <c r="D85" s="65"/>
       <c r="E85" s="57"/>
       <c r="F85" s="57"/>
       <c r="G85" s="57"/>
@@ -3354,7 +3361,7 @@
       <c r="C86" s="58">
         <v>7</v>
       </c>
-      <c r="D86" s="57"/>
+      <c r="D86" s="65"/>
       <c r="E86" s="57"/>
       <c r="F86" s="57"/>
       <c r="G86" s="57"/>
@@ -3404,7 +3411,7 @@
       <c r="C87" s="58">
         <v>8</v>
       </c>
-      <c r="D87" s="57"/>
+      <c r="D87" s="65"/>
       <c r="E87" s="57"/>
       <c r="F87" s="57"/>
       <c r="G87" s="57"/>
@@ -3454,7 +3461,7 @@
       <c r="C88" s="58" t="s">
         <v>138</v>
       </c>
-      <c r="D88" s="60"/>
+      <c r="D88" s="66"/>
       <c r="E88" s="60"/>
       <c r="F88" s="60"/>
       <c r="G88" s="60"/>
@@ -3504,7 +3511,7 @@
       <c r="C89" s="58">
         <v>10</v>
       </c>
-      <c r="D89" s="60"/>
+      <c r="D89" s="66"/>
       <c r="E89" s="60"/>
       <c r="F89" s="60"/>
       <c r="G89" s="60"/>
@@ -3554,7 +3561,7 @@
       <c r="C90" s="60">
         <v>11</v>
       </c>
-      <c r="D90" s="60"/>
+      <c r="D90" s="66"/>
       <c r="E90" s="60"/>
       <c r="F90" s="60"/>
       <c r="G90" s="60"/>
@@ -3604,7 +3611,7 @@
       <c r="C91" s="60">
         <v>12</v>
       </c>
-      <c r="D91" s="60"/>
+      <c r="D91" s="66"/>
       <c r="E91" s="60"/>
       <c r="F91" s="60"/>
       <c r="G91" s="60"/>
@@ -3654,7 +3661,7 @@
       <c r="C92" s="60">
         <v>13</v>
       </c>
-      <c r="D92" s="60"/>
+      <c r="D92" s="66"/>
       <c r="E92" s="60"/>
       <c r="F92" s="60"/>
       <c r="G92" s="60"/>

</xml_diff>

<commit_message>
Update Brain Stew Gantt
</commit_message>
<xml_diff>
--- a/383Game/Doc/Brain Stew Master Gantt Chart.xlsx
+++ b/383Game/Doc/Brain Stew Master Gantt Chart.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/252328c91043836d/Documents/GitHub/CS383BrainstewGame/383Game/Doc/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/19db3ad368368567/Documents/GitHub/CS383BrainstewGame/383Game/Doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="19" documentId="13_ncr:1_{F154A668-4499-40DB-9C61-ABFFA038B4BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{56F0B5A1-8E35-4465-8BC2-B174E7517F94}"/>
+  <xr:revisionPtr revIDLastSave="243" documentId="13_ncr:1_{F154A668-4499-40DB-9C61-ABFFA038B4BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{759806D6-E4D5-457B-97B8-7961D89361B6}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{6C77CEAA-6C20-4875-8E69-F182CEDC365C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12816" activeTab="3" xr2:uid="{6C77CEAA-6C20-4875-8E69-F182CEDC365C}"/>
   </bookViews>
   <sheets>
     <sheet name="Budget" sheetId="3" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="180">
   <si>
     <t>Cory Clairmont</t>
   </si>
@@ -543,17 +543,52 @@
   </si>
   <si>
     <t>6. UI Animations, Effects, Graphics</t>
+  </si>
+  <si>
+    <t>First Meeting</t>
+  </si>
+  <si>
+    <t>Hours</t>
+  </si>
+  <si>
+    <t>Andrew S</t>
+  </si>
+  <si>
+    <t>Nihat K</t>
+  </si>
+  <si>
+    <t>Jan. 24</t>
+  </si>
+  <si>
+    <t>Weekly Meeting</t>
+  </si>
+  <si>
+    <t>Jan. 27</t>
+  </si>
+  <si>
+    <t>Feb. 3</t>
+  </si>
+  <si>
+    <t>Feb. 10</t>
+  </si>
+  <si>
+    <t>SA Presentation Prep</t>
+  </si>
+  <si>
+    <t>Feb. 24</t>
+  </si>
+  <si>
+    <t>MVP Prep</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
-    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+  <numFmts count="1">
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -592,8 +627,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Wingdings"/>
+      <charset val="2"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -648,8 +695,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="13">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -789,11 +842,48 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -886,22 +976,31 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="8" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -922,16 +1021,13 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -940,23 +1036,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -967,16 +1060,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1313,8 +1424,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A562B3B-3013-4879-ABBB-AEB80198B717}">
   <dimension ref="B2:AF22"/>
   <sheetViews>
-    <sheetView zoomScale="35" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView zoomScale="92" zoomScaleNormal="92" workbookViewId="0">
+      <selection activeCell="S15" sqref="S15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1324,448 +1435,544 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:32" x14ac:dyDescent="0.3">
-      <c r="C2" s="60" t="s">
+      <c r="C2" s="63" t="s">
         <v>64</v>
       </c>
-      <c r="D2" s="61"/>
-      <c r="E2" s="61"/>
-      <c r="F2" s="61"/>
-      <c r="G2" s="61"/>
-      <c r="H2" s="62"/>
-      <c r="K2" s="60" t="s">
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="64"/>
+      <c r="H2" s="65"/>
+      <c r="K2" s="63" t="s">
         <v>163</v>
       </c>
-      <c r="L2" s="61"/>
-      <c r="M2" s="61"/>
-      <c r="N2" s="61"/>
-      <c r="O2" s="61"/>
-      <c r="P2" s="62"/>
-      <c r="S2" s="60" t="s">
+      <c r="L2" s="64"/>
+      <c r="M2" s="64"/>
+      <c r="N2" s="64"/>
+      <c r="O2" s="64"/>
+      <c r="P2" s="65"/>
+      <c r="S2" s="63" t="s">
         <v>164</v>
       </c>
-      <c r="T2" s="61"/>
-      <c r="U2" s="61"/>
-      <c r="V2" s="61"/>
-      <c r="W2" s="61"/>
-      <c r="X2" s="62"/>
-      <c r="AA2" s="60" t="s">
+      <c r="T2" s="64"/>
+      <c r="U2" s="64"/>
+      <c r="V2" s="64"/>
+      <c r="W2" s="64"/>
+      <c r="X2" s="65"/>
+      <c r="AA2" s="63" t="s">
         <v>165</v>
       </c>
-      <c r="AB2" s="61"/>
-      <c r="AC2" s="61"/>
-      <c r="AD2" s="61"/>
-      <c r="AE2" s="61"/>
-      <c r="AF2" s="62"/>
+      <c r="AB2" s="64"/>
+      <c r="AC2" s="64"/>
+      <c r="AD2" s="64"/>
+      <c r="AE2" s="64"/>
+      <c r="AF2" s="65"/>
     </row>
     <row r="3" spans="2:32" x14ac:dyDescent="0.3">
-      <c r="C3" s="63" t="s">
+      <c r="C3" s="66" t="s">
         <v>65</v>
       </c>
-      <c r="D3" s="64"/>
-      <c r="E3" s="64" t="s">
+      <c r="D3" s="67"/>
+      <c r="E3" s="67" t="s">
         <v>66</v>
       </c>
-      <c r="F3" s="64"/>
-      <c r="G3" s="64" t="s">
+      <c r="F3" s="67"/>
+      <c r="G3" s="67" t="s">
         <v>67</v>
       </c>
-      <c r="H3" s="65"/>
-      <c r="K3" s="63" t="s">
+      <c r="H3" s="68"/>
+      <c r="K3" s="66" t="s">
         <v>65</v>
       </c>
-      <c r="L3" s="64"/>
-      <c r="M3" s="64" t="s">
+      <c r="L3" s="67"/>
+      <c r="M3" s="67" t="s">
         <v>66</v>
       </c>
-      <c r="N3" s="64"/>
-      <c r="O3" s="64" t="s">
+      <c r="N3" s="67"/>
+      <c r="O3" s="67" t="s">
         <v>67</v>
       </c>
-      <c r="P3" s="65"/>
-      <c r="S3" s="63" t="s">
+      <c r="P3" s="68"/>
+      <c r="S3" s="66" t="s">
         <v>65</v>
       </c>
-      <c r="T3" s="64"/>
-      <c r="U3" s="64" t="s">
+      <c r="T3" s="67"/>
+      <c r="U3" s="67" t="s">
         <v>66</v>
       </c>
-      <c r="V3" s="64"/>
-      <c r="W3" s="64" t="s">
+      <c r="V3" s="67"/>
+      <c r="W3" s="67" t="s">
         <v>67</v>
       </c>
-      <c r="X3" s="65"/>
-      <c r="AA3" s="63" t="s">
+      <c r="X3" s="68"/>
+      <c r="AA3" s="66" t="s">
         <v>65</v>
       </c>
-      <c r="AB3" s="64"/>
-      <c r="AC3" s="64" t="s">
+      <c r="AB3" s="67"/>
+      <c r="AC3" s="67" t="s">
         <v>66</v>
       </c>
-      <c r="AD3" s="64"/>
-      <c r="AE3" s="64" t="s">
+      <c r="AD3" s="67"/>
+      <c r="AE3" s="67" t="s">
         <v>67</v>
       </c>
-      <c r="AF3" s="65"/>
+      <c r="AF3" s="68"/>
     </row>
     <row r="4" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B4" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="C4" s="75"/>
-      <c r="D4" s="66"/>
-      <c r="E4" s="66"/>
-      <c r="F4" s="66"/>
-      <c r="G4" s="66"/>
-      <c r="H4" s="67"/>
+      <c r="C4" s="69">
+        <v>8200</v>
+      </c>
+      <c r="D4" s="59"/>
+      <c r="E4" s="59" t="s">
+        <v>166</v>
+      </c>
+      <c r="F4" s="59"/>
+      <c r="G4" s="59" t="s">
+        <v>166</v>
+      </c>
+      <c r="H4" s="70"/>
       <c r="J4" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="K4" s="75">
+      <c r="K4" s="69">
         <v>5200</v>
       </c>
-      <c r="L4" s="66"/>
-      <c r="M4" s="66" t="s">
+      <c r="L4" s="59"/>
+      <c r="M4" s="59" t="s">
         <v>166</v>
       </c>
-      <c r="N4" s="66"/>
-      <c r="O4" s="66" t="s">
+      <c r="N4" s="59"/>
+      <c r="O4" s="59" t="s">
         <v>166</v>
       </c>
-      <c r="P4" s="67"/>
+      <c r="P4" s="70"/>
       <c r="R4" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="S4" s="72"/>
-      <c r="T4" s="66"/>
-      <c r="U4" s="66"/>
-      <c r="V4" s="66"/>
-      <c r="W4" s="66"/>
-      <c r="X4" s="67"/>
+      <c r="S4" s="69">
+        <v>3000</v>
+      </c>
+      <c r="T4" s="59"/>
+      <c r="U4" s="59" t="s">
+        <v>166</v>
+      </c>
+      <c r="V4" s="59"/>
+      <c r="W4" s="59" t="s">
+        <v>166</v>
+      </c>
+      <c r="X4" s="70"/>
       <c r="Z4" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="AA4" s="72"/>
-      <c r="AB4" s="66"/>
-      <c r="AC4" s="66"/>
-      <c r="AD4" s="66"/>
-      <c r="AE4" s="66"/>
-      <c r="AF4" s="67"/>
+      <c r="AA4" s="58"/>
+      <c r="AB4" s="59"/>
+      <c r="AC4" s="59"/>
+      <c r="AD4" s="59"/>
+      <c r="AE4" s="59"/>
+      <c r="AF4" s="70"/>
     </row>
     <row r="5" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B5" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="C5" s="73"/>
-      <c r="D5" s="55"/>
-      <c r="E5" s="55"/>
-      <c r="F5" s="55"/>
-      <c r="G5" s="55"/>
-      <c r="H5" s="56"/>
+      <c r="C5" s="69">
+        <v>10200</v>
+      </c>
+      <c r="D5" s="59"/>
+      <c r="E5" s="82" t="s">
+        <v>166</v>
+      </c>
+      <c r="F5" s="82"/>
+      <c r="G5" s="82" t="s">
+        <v>166</v>
+      </c>
+      <c r="H5" s="57"/>
       <c r="J5" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="K5" s="73">
+      <c r="K5" s="71">
         <v>7200</v>
       </c>
-      <c r="L5" s="55"/>
-      <c r="M5" s="55" t="s">
+      <c r="L5" s="56"/>
+      <c r="M5" s="56" t="s">
         <v>166</v>
       </c>
-      <c r="N5" s="55"/>
-      <c r="O5" s="55" t="s">
+      <c r="N5" s="56"/>
+      <c r="O5" s="56" t="s">
         <v>166</v>
       </c>
-      <c r="P5" s="56"/>
+      <c r="P5" s="57"/>
       <c r="R5" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="S5" s="59"/>
-      <c r="T5" s="55"/>
-      <c r="U5" s="55"/>
-      <c r="V5" s="55"/>
-      <c r="W5" s="55"/>
-      <c r="X5" s="56"/>
+      <c r="S5" s="69">
+        <v>3000</v>
+      </c>
+      <c r="T5" s="59"/>
+      <c r="U5" s="82" t="s">
+        <v>166</v>
+      </c>
+      <c r="V5" s="82"/>
+      <c r="W5" s="82" t="s">
+        <v>166</v>
+      </c>
+      <c r="X5" s="57"/>
       <c r="Z5" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="AA5" s="59"/>
-      <c r="AB5" s="55"/>
-      <c r="AC5" s="55"/>
-      <c r="AD5" s="55"/>
-      <c r="AE5" s="55"/>
-      <c r="AF5" s="56"/>
+      <c r="AA5" s="55"/>
+      <c r="AB5" s="56"/>
+      <c r="AC5" s="56"/>
+      <c r="AD5" s="56"/>
+      <c r="AE5" s="56"/>
+      <c r="AF5" s="57"/>
     </row>
     <row r="6" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B6" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="C6" s="59"/>
-      <c r="D6" s="55"/>
-      <c r="E6" s="55"/>
-      <c r="F6" s="55"/>
-      <c r="G6" s="55"/>
-      <c r="H6" s="56"/>
+      <c r="C6" s="69">
+        <v>8300</v>
+      </c>
+      <c r="D6" s="59"/>
+      <c r="E6" s="82" t="s">
+        <v>166</v>
+      </c>
+      <c r="F6" s="82"/>
+      <c r="G6" s="82" t="s">
+        <v>166</v>
+      </c>
+      <c r="H6" s="57"/>
       <c r="J6" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="K6" s="73">
+      <c r="K6" s="71">
         <v>5300</v>
       </c>
-      <c r="L6" s="55"/>
-      <c r="M6" s="55" t="s">
+      <c r="L6" s="56"/>
+      <c r="M6" s="56" t="s">
         <v>166</v>
       </c>
-      <c r="N6" s="55"/>
-      <c r="O6" s="55" t="s">
+      <c r="N6" s="56"/>
+      <c r="O6" s="56" t="s">
         <v>166</v>
       </c>
-      <c r="P6" s="56"/>
+      <c r="P6" s="57"/>
       <c r="R6" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="S6" s="59"/>
-      <c r="T6" s="55"/>
-      <c r="U6" s="55"/>
-      <c r="V6" s="55"/>
-      <c r="W6" s="55"/>
-      <c r="X6" s="56"/>
+      <c r="S6" s="69">
+        <v>3000</v>
+      </c>
+      <c r="T6" s="59"/>
+      <c r="U6" s="82" t="s">
+        <v>166</v>
+      </c>
+      <c r="V6" s="82"/>
+      <c r="W6" s="82" t="s">
+        <v>166</v>
+      </c>
+      <c r="X6" s="57"/>
       <c r="Z6" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="AA6" s="59"/>
-      <c r="AB6" s="55"/>
-      <c r="AC6" s="55"/>
-      <c r="AD6" s="55"/>
-      <c r="AE6" s="55"/>
-      <c r="AF6" s="56"/>
+      <c r="AA6" s="55"/>
+      <c r="AB6" s="56"/>
+      <c r="AC6" s="56"/>
+      <c r="AD6" s="56"/>
+      <c r="AE6" s="56"/>
+      <c r="AF6" s="57"/>
     </row>
     <row r="7" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B7" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="C7" s="59"/>
-      <c r="D7" s="55"/>
-      <c r="E7" s="55"/>
-      <c r="F7" s="55"/>
-      <c r="G7" s="55"/>
-      <c r="H7" s="56"/>
+      <c r="C7" s="69">
+        <v>9000</v>
+      </c>
+      <c r="D7" s="59"/>
+      <c r="E7" s="82" t="s">
+        <v>166</v>
+      </c>
+      <c r="F7" s="82"/>
+      <c r="G7" s="82" t="s">
+        <v>166</v>
+      </c>
+      <c r="H7" s="57"/>
       <c r="J7" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="K7" s="73">
+      <c r="K7" s="71">
         <v>6000</v>
       </c>
-      <c r="L7" s="55"/>
-      <c r="M7" s="55" t="s">
+      <c r="L7" s="56"/>
+      <c r="M7" s="56" t="s">
         <v>166</v>
       </c>
-      <c r="N7" s="55"/>
-      <c r="O7" s="55" t="s">
+      <c r="N7" s="56"/>
+      <c r="O7" s="56" t="s">
         <v>166</v>
       </c>
-      <c r="P7" s="56"/>
+      <c r="P7" s="57"/>
       <c r="R7" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="S7" s="59"/>
-      <c r="T7" s="55"/>
-      <c r="U7" s="55"/>
-      <c r="V7" s="55"/>
-      <c r="W7" s="55"/>
-      <c r="X7" s="56"/>
+      <c r="S7" s="69">
+        <v>3000</v>
+      </c>
+      <c r="T7" s="59"/>
+      <c r="U7" s="82" t="s">
+        <v>166</v>
+      </c>
+      <c r="V7" s="82"/>
+      <c r="W7" s="82" t="s">
+        <v>166</v>
+      </c>
+      <c r="X7" s="57"/>
       <c r="Z7" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="AA7" s="59"/>
-      <c r="AB7" s="55"/>
-      <c r="AC7" s="55"/>
-      <c r="AD7" s="55"/>
-      <c r="AE7" s="55"/>
-      <c r="AF7" s="56"/>
+      <c r="AA7" s="55"/>
+      <c r="AB7" s="56"/>
+      <c r="AC7" s="56"/>
+      <c r="AD7" s="56"/>
+      <c r="AE7" s="56"/>
+      <c r="AF7" s="57"/>
     </row>
     <row r="8" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B8" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="C8" s="59"/>
-      <c r="D8" s="55"/>
-      <c r="E8" s="55"/>
-      <c r="F8" s="55"/>
-      <c r="G8" s="55"/>
-      <c r="H8" s="56"/>
+      <c r="C8" s="69">
+        <v>9300</v>
+      </c>
+      <c r="D8" s="59"/>
+      <c r="E8" s="82" t="s">
+        <v>166</v>
+      </c>
+      <c r="F8" s="82"/>
+      <c r="G8" s="82" t="s">
+        <v>166</v>
+      </c>
+      <c r="H8" s="57"/>
       <c r="J8" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="K8" s="73">
+      <c r="K8" s="71">
         <v>6300</v>
       </c>
-      <c r="L8" s="55"/>
-      <c r="M8" s="55" t="s">
+      <c r="L8" s="56"/>
+      <c r="M8" s="56" t="s">
         <v>166</v>
       </c>
-      <c r="N8" s="55"/>
-      <c r="O8" s="55" t="s">
+      <c r="N8" s="56"/>
+      <c r="O8" s="56" t="s">
         <v>166</v>
       </c>
-      <c r="P8" s="56"/>
+      <c r="P8" s="57"/>
       <c r="R8" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="S8" s="59"/>
-      <c r="T8" s="55"/>
-      <c r="U8" s="55"/>
-      <c r="V8" s="55"/>
-      <c r="W8" s="55"/>
-      <c r="X8" s="56"/>
+      <c r="S8" s="69">
+        <v>3000</v>
+      </c>
+      <c r="T8" s="59"/>
+      <c r="U8" s="82" t="s">
+        <v>166</v>
+      </c>
+      <c r="V8" s="82"/>
+      <c r="W8" s="82" t="s">
+        <v>166</v>
+      </c>
+      <c r="X8" s="57"/>
       <c r="Z8" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="AA8" s="59"/>
-      <c r="AB8" s="55"/>
-      <c r="AC8" s="55"/>
-      <c r="AD8" s="55"/>
-      <c r="AE8" s="55"/>
-      <c r="AF8" s="56"/>
+      <c r="AA8" s="55"/>
+      <c r="AB8" s="56"/>
+      <c r="AC8" s="56"/>
+      <c r="AD8" s="56"/>
+      <c r="AE8" s="56"/>
+      <c r="AF8" s="57"/>
     </row>
     <row r="9" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B9" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="C9" s="59"/>
-      <c r="D9" s="55"/>
-      <c r="E9" s="55"/>
-      <c r="F9" s="55"/>
-      <c r="G9" s="55"/>
-      <c r="H9" s="56"/>
+      <c r="C9" s="69">
+        <v>8500</v>
+      </c>
+      <c r="D9" s="59"/>
+      <c r="E9" s="82" t="s">
+        <v>166</v>
+      </c>
+      <c r="F9" s="82"/>
+      <c r="G9" s="82" t="s">
+        <v>166</v>
+      </c>
+      <c r="H9" s="57"/>
       <c r="J9" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="K9" s="73">
+      <c r="K9" s="71">
         <v>5500</v>
       </c>
-      <c r="L9" s="55"/>
-      <c r="M9" s="55" t="s">
+      <c r="L9" s="56"/>
+      <c r="M9" s="56" t="s">
         <v>166</v>
       </c>
-      <c r="N9" s="55"/>
-      <c r="O9" s="55" t="s">
+      <c r="N9" s="56"/>
+      <c r="O9" s="56" t="s">
         <v>166</v>
       </c>
-      <c r="P9" s="56"/>
+      <c r="P9" s="57"/>
       <c r="R9" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="S9" s="59"/>
-      <c r="T9" s="55"/>
-      <c r="U9" s="55"/>
-      <c r="V9" s="55"/>
-      <c r="W9" s="55"/>
-      <c r="X9" s="56"/>
+      <c r="S9" s="69">
+        <v>3000</v>
+      </c>
+      <c r="T9" s="59"/>
+      <c r="U9" s="82" t="s">
+        <v>166</v>
+      </c>
+      <c r="V9" s="82"/>
+      <c r="W9" s="82" t="s">
+        <v>166</v>
+      </c>
+      <c r="X9" s="57"/>
       <c r="Z9" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="AA9" s="59"/>
-      <c r="AB9" s="55"/>
-      <c r="AC9" s="55"/>
-      <c r="AD9" s="55"/>
-      <c r="AE9" s="55"/>
-      <c r="AF9" s="56"/>
+      <c r="AA9" s="55"/>
+      <c r="AB9" s="56"/>
+      <c r="AC9" s="56"/>
+      <c r="AD9" s="56"/>
+      <c r="AE9" s="56"/>
+      <c r="AF9" s="57"/>
     </row>
     <row r="10" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B10" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="C10" s="68"/>
-      <c r="D10" s="57"/>
-      <c r="E10" s="57"/>
-      <c r="F10" s="57"/>
-      <c r="G10" s="57"/>
-      <c r="H10" s="58"/>
+      <c r="C10" s="69">
+        <v>7700</v>
+      </c>
+      <c r="D10" s="59"/>
+      <c r="E10" s="61" t="s">
+        <v>166</v>
+      </c>
+      <c r="F10" s="61"/>
+      <c r="G10" s="61" t="s">
+        <v>166</v>
+      </c>
+      <c r="H10" s="62"/>
       <c r="J10" s="24" t="s">
         <v>63</v>
       </c>
       <c r="K10" s="74">
         <v>4700</v>
       </c>
-      <c r="L10" s="57"/>
-      <c r="M10" s="57" t="s">
+      <c r="L10" s="61"/>
+      <c r="M10" s="61" t="s">
         <v>166</v>
       </c>
-      <c r="N10" s="57"/>
-      <c r="O10" s="57" t="s">
+      <c r="N10" s="61"/>
+      <c r="O10" s="61" t="s">
         <v>166</v>
       </c>
-      <c r="P10" s="58"/>
+      <c r="P10" s="62"/>
       <c r="R10" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="S10" s="68"/>
-      <c r="T10" s="57"/>
-      <c r="U10" s="57"/>
-      <c r="V10" s="57"/>
-      <c r="W10" s="57"/>
-      <c r="X10" s="58"/>
+      <c r="S10" s="69">
+        <v>3000</v>
+      </c>
+      <c r="T10" s="59"/>
+      <c r="U10" s="61" t="s">
+        <v>166</v>
+      </c>
+      <c r="V10" s="61"/>
+      <c r="W10" s="61" t="s">
+        <v>166</v>
+      </c>
+      <c r="X10" s="62"/>
       <c r="Z10" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="AA10" s="68"/>
-      <c r="AB10" s="57"/>
-      <c r="AC10" s="57"/>
-      <c r="AD10" s="57"/>
-      <c r="AE10" s="57"/>
-      <c r="AF10" s="58"/>
+      <c r="AA10" s="60"/>
+      <c r="AB10" s="61"/>
+      <c r="AC10" s="61"/>
+      <c r="AD10" s="61"/>
+      <c r="AE10" s="61"/>
+      <c r="AF10" s="62"/>
     </row>
     <row r="11" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B11" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="C11" s="68"/>
-      <c r="D11" s="57"/>
-      <c r="E11" s="57"/>
-      <c r="F11" s="57"/>
-      <c r="G11" s="57"/>
-      <c r="H11" s="58"/>
+      <c r="C11" s="69">
+        <v>5200</v>
+      </c>
+      <c r="D11" s="59"/>
+      <c r="E11" s="61" t="s">
+        <v>166</v>
+      </c>
+      <c r="F11" s="61"/>
+      <c r="G11" s="61" t="s">
+        <v>166</v>
+      </c>
+      <c r="H11" s="62"/>
       <c r="J11" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="K11" s="69">
-        <v>40200</v>
-      </c>
-      <c r="L11" s="70"/>
-      <c r="M11" s="70" t="s">
+      <c r="K11" s="74">
+        <v>42000</v>
+      </c>
+      <c r="L11" s="61"/>
+      <c r="M11" s="72" t="s">
         <v>166</v>
       </c>
-      <c r="N11" s="70"/>
-      <c r="O11" s="70" t="s">
+      <c r="N11" s="72"/>
+      <c r="O11" s="72" t="s">
         <v>166</v>
       </c>
-      <c r="P11" s="71"/>
+      <c r="P11" s="73"/>
       <c r="R11" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="S11" s="68"/>
-      <c r="T11" s="57"/>
-      <c r="U11" s="57"/>
-      <c r="V11" s="57"/>
-      <c r="W11" s="57"/>
-      <c r="X11" s="58"/>
+      <c r="S11" s="69">
+        <v>21000</v>
+      </c>
+      <c r="T11" s="59"/>
+      <c r="U11" s="61" t="s">
+        <v>166</v>
+      </c>
+      <c r="V11" s="61"/>
+      <c r="W11" s="61" t="s">
+        <v>166</v>
+      </c>
+      <c r="X11" s="62"/>
       <c r="Z11" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="AA11" s="68"/>
-      <c r="AB11" s="57"/>
-      <c r="AC11" s="57"/>
-      <c r="AD11" s="57"/>
-      <c r="AE11" s="57"/>
-      <c r="AF11" s="58"/>
+      <c r="AA11" s="60"/>
+      <c r="AB11" s="61"/>
+      <c r="AC11" s="61"/>
+      <c r="AD11" s="61"/>
+      <c r="AE11" s="61"/>
+      <c r="AF11" s="62"/>
     </row>
     <row r="12" spans="2:32" x14ac:dyDescent="0.3">
-      <c r="Y12" s="55"/>
-      <c r="Z12" s="55"/>
-      <c r="AA12" s="55"/>
-      <c r="AB12" s="55"/>
-      <c r="AC12" s="55"/>
-      <c r="AD12" s="55"/>
+      <c r="Y12" s="56"/>
+      <c r="Z12" s="56"/>
+      <c r="AA12" s="56"/>
+      <c r="AB12" s="56"/>
+      <c r="AC12" s="56"/>
+      <c r="AD12" s="56"/>
     </row>
     <row r="15" spans="2:32" x14ac:dyDescent="0.3">
       <c r="I15" s="52"/>
@@ -1793,73 +2000,30 @@
     </row>
   </sheetData>
   <mergeCells count="115">
-    <mergeCell ref="S9:T9"/>
-    <mergeCell ref="U9:V9"/>
-    <mergeCell ref="W9:X9"/>
-    <mergeCell ref="AA4:AB4"/>
-    <mergeCell ref="AC4:AD4"/>
-    <mergeCell ref="Y12:Z12"/>
-    <mergeCell ref="AA12:AB12"/>
-    <mergeCell ref="AC12:AD12"/>
-    <mergeCell ref="AA9:AB9"/>
-    <mergeCell ref="AA11:AB11"/>
-    <mergeCell ref="AC11:AD11"/>
-    <mergeCell ref="AA5:AB5"/>
-    <mergeCell ref="AA6:AB6"/>
-    <mergeCell ref="AA7:AB7"/>
-    <mergeCell ref="AA8:AB8"/>
-    <mergeCell ref="AA10:AB10"/>
-    <mergeCell ref="AC5:AD5"/>
-    <mergeCell ref="AC6:AD6"/>
-    <mergeCell ref="AC7:AD7"/>
-    <mergeCell ref="AC8:AD8"/>
-    <mergeCell ref="AC10:AD10"/>
-    <mergeCell ref="AC9:AD9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="C2:H2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="K2:P2"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="M3:N3"/>
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="M4:N4"/>
-    <mergeCell ref="O4:P4"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="O5:P5"/>
-    <mergeCell ref="M7:N7"/>
-    <mergeCell ref="O7:P7"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="O8:P8"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="AE9:AF9"/>
+    <mergeCell ref="AE10:AF10"/>
+    <mergeCell ref="AE11:AF11"/>
+    <mergeCell ref="S7:T7"/>
+    <mergeCell ref="U7:V7"/>
+    <mergeCell ref="W7:X7"/>
+    <mergeCell ref="S8:T8"/>
+    <mergeCell ref="AA2:AF2"/>
+    <mergeCell ref="AA3:AB3"/>
+    <mergeCell ref="AC3:AD3"/>
+    <mergeCell ref="AE3:AF3"/>
+    <mergeCell ref="AE4:AF4"/>
+    <mergeCell ref="AE5:AF5"/>
+    <mergeCell ref="AE6:AF6"/>
+    <mergeCell ref="AE7:AF7"/>
+    <mergeCell ref="AE8:AF8"/>
+    <mergeCell ref="S10:T10"/>
+    <mergeCell ref="U10:V10"/>
+    <mergeCell ref="W10:X10"/>
+    <mergeCell ref="S11:T11"/>
+    <mergeCell ref="U11:V11"/>
+    <mergeCell ref="W11:X11"/>
+    <mergeCell ref="U8:V8"/>
+    <mergeCell ref="W8:X8"/>
     <mergeCell ref="K11:L11"/>
     <mergeCell ref="M11:N11"/>
     <mergeCell ref="O11:P11"/>
@@ -1884,30 +2048,73 @@
     <mergeCell ref="O10:P10"/>
     <mergeCell ref="O6:P6"/>
     <mergeCell ref="K7:L7"/>
-    <mergeCell ref="AE9:AF9"/>
-    <mergeCell ref="AE10:AF10"/>
-    <mergeCell ref="AE11:AF11"/>
-    <mergeCell ref="S7:T7"/>
-    <mergeCell ref="U7:V7"/>
-    <mergeCell ref="W7:X7"/>
-    <mergeCell ref="S8:T8"/>
-    <mergeCell ref="AA2:AF2"/>
-    <mergeCell ref="AA3:AB3"/>
-    <mergeCell ref="AC3:AD3"/>
-    <mergeCell ref="AE3:AF3"/>
-    <mergeCell ref="AE4:AF4"/>
-    <mergeCell ref="AE5:AF5"/>
-    <mergeCell ref="AE6:AF6"/>
-    <mergeCell ref="AE7:AF7"/>
-    <mergeCell ref="AE8:AF8"/>
-    <mergeCell ref="S10:T10"/>
-    <mergeCell ref="U10:V10"/>
-    <mergeCell ref="W10:X10"/>
-    <mergeCell ref="S11:T11"/>
-    <mergeCell ref="U11:V11"/>
-    <mergeCell ref="W11:X11"/>
-    <mergeCell ref="U8:V8"/>
-    <mergeCell ref="W8:X8"/>
+    <mergeCell ref="M7:N7"/>
+    <mergeCell ref="O7:P7"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="O8:P8"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="K2:P2"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="O4:P4"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="O5:P5"/>
+    <mergeCell ref="C2:H2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="S9:T9"/>
+    <mergeCell ref="U9:V9"/>
+    <mergeCell ref="W9:X9"/>
+    <mergeCell ref="AA4:AB4"/>
+    <mergeCell ref="AC4:AD4"/>
+    <mergeCell ref="Y12:Z12"/>
+    <mergeCell ref="AA12:AB12"/>
+    <mergeCell ref="AC12:AD12"/>
+    <mergeCell ref="AA9:AB9"/>
+    <mergeCell ref="AA11:AB11"/>
+    <mergeCell ref="AC11:AD11"/>
+    <mergeCell ref="AA5:AB5"/>
+    <mergeCell ref="AA6:AB6"/>
+    <mergeCell ref="AA7:AB7"/>
+    <mergeCell ref="AA8:AB8"/>
+    <mergeCell ref="AA10:AB10"/>
+    <mergeCell ref="AC5:AD5"/>
+    <mergeCell ref="AC6:AD6"/>
+    <mergeCell ref="AC7:AD7"/>
+    <mergeCell ref="AC8:AD8"/>
+    <mergeCell ref="AC10:AD10"/>
+    <mergeCell ref="AC9:AD9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1917,7 +2124,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E50249A2-2F05-400B-B05E-0C14F827A1C5}">
   <dimension ref="A1:CRB111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="55" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A8" zoomScale="55" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="AG111" sqref="AG111:AJ111"/>
     </sheetView>
   </sheetViews>
@@ -1956,10 +2163,10 @@
       </c>
     </row>
     <row r="2" spans="1:64" s="33" customFormat="1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A2" s="76" t="s">
+      <c r="A2" s="75" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="76"/>
+      <c r="B2" s="75"/>
       <c r="D2" s="34"/>
       <c r="E2" s="33">
         <v>1</v>
@@ -7130,11 +7337,6 @@
         <v>50</v>
       </c>
       <c r="D107" s="14"/>
-      <c r="M107" s="85"/>
-      <c r="N107" s="85"/>
-      <c r="O107" s="85"/>
-      <c r="P107" s="85"/>
-      <c r="Q107" s="85"/>
       <c r="T107" s="15"/>
       <c r="U107" s="15"/>
       <c r="V107" s="15"/>
@@ -7152,16 +7354,6 @@
         <v>6</v>
       </c>
       <c r="D108" s="14"/>
-      <c r="M108" s="86"/>
-      <c r="N108" s="86"/>
-      <c r="O108" s="86"/>
-      <c r="P108" s="86"/>
-      <c r="Q108" s="86"/>
-      <c r="R108" s="84"/>
-      <c r="S108" s="84"/>
-      <c r="T108" s="84"/>
-      <c r="U108" s="84"/>
-      <c r="V108" s="84"/>
       <c r="Y108" s="15"/>
       <c r="Z108" s="15"/>
       <c r="AA108" s="15"/>
@@ -7179,10 +7371,6 @@
         <v>6</v>
       </c>
       <c r="D109" s="14"/>
-      <c r="W109" s="84"/>
-      <c r="X109" s="84"/>
-      <c r="Y109" s="84"/>
-      <c r="Z109" s="84"/>
       <c r="AD109" s="15"/>
       <c r="AE109" s="15"/>
       <c r="AF109" s="15"/>
@@ -7201,12 +7389,6 @@
         <v>51</v>
       </c>
       <c r="D110" s="14"/>
-      <c r="AA110" s="84"/>
-      <c r="AB110" s="84"/>
-      <c r="AC110" s="84"/>
-      <c r="AD110" s="84"/>
-      <c r="AE110" s="84"/>
-      <c r="AF110" s="84"/>
       <c r="AJ110" s="15"/>
       <c r="AK110" s="15"/>
       <c r="AL110" s="15"/>
@@ -7225,10 +7407,6 @@
         <v>9</v>
       </c>
       <c r="D111" s="49"/>
-      <c r="AG111" s="83"/>
-      <c r="AH111" s="83"/>
-      <c r="AI111" s="83"/>
-      <c r="AJ111" s="83"/>
       <c r="AP111" s="50"/>
       <c r="AQ111" s="50"/>
       <c r="AR111" s="50"/>
@@ -7254,36 +7432,36 @@
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="2" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="B2" s="82" t="s">
+      <c r="B2" s="76" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="82"/>
-      <c r="D2" s="82"/>
-      <c r="E2" s="82" t="s">
+      <c r="C2" s="76"/>
+      <c r="D2" s="76"/>
+      <c r="E2" s="76" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="82"/>
-      <c r="G2" s="82"/>
-      <c r="H2" s="82" t="s">
+      <c r="F2" s="76"/>
+      <c r="G2" s="76"/>
+      <c r="H2" s="76" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="82"/>
-      <c r="J2" s="82"/>
-      <c r="K2" s="82" t="s">
+      <c r="I2" s="76"/>
+      <c r="J2" s="76"/>
+      <c r="K2" s="76" t="s">
         <v>15</v>
       </c>
-      <c r="L2" s="82"/>
-      <c r="M2" s="82"/>
-      <c r="N2" s="82" t="s">
+      <c r="L2" s="76"/>
+      <c r="M2" s="76"/>
+      <c r="N2" s="76" t="s">
         <v>16</v>
       </c>
-      <c r="O2" s="82"/>
-      <c r="P2" s="82"/>
-      <c r="Q2" s="82" t="s">
+      <c r="O2" s="76"/>
+      <c r="P2" s="76"/>
+      <c r="Q2" s="76" t="s">
         <v>17</v>
       </c>
-      <c r="R2" s="82"/>
-      <c r="S2" s="82"/>
+      <c r="R2" s="76"/>
+      <c r="S2" s="76"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B3" s="77" t="s">
@@ -7318,216 +7496,216 @@
       <c r="S3" s="77"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="B4" s="81"/>
-      <c r="C4" s="81"/>
-      <c r="D4" s="81"/>
-      <c r="E4" s="81"/>
-      <c r="F4" s="81"/>
-      <c r="G4" s="81"/>
-      <c r="H4" s="81"/>
-      <c r="I4" s="81"/>
-      <c r="J4" s="81"/>
-      <c r="K4" s="81"/>
-      <c r="L4" s="81"/>
-      <c r="M4" s="81"/>
-      <c r="N4" s="81"/>
-      <c r="O4" s="81"/>
-      <c r="P4" s="81"/>
-      <c r="Q4" s="81"/>
-      <c r="R4" s="81"/>
-      <c r="S4" s="81"/>
+      <c r="B4" s="78"/>
+      <c r="C4" s="78"/>
+      <c r="D4" s="78"/>
+      <c r="E4" s="78"/>
+      <c r="F4" s="78"/>
+      <c r="G4" s="78"/>
+      <c r="H4" s="78"/>
+      <c r="I4" s="78"/>
+      <c r="J4" s="78"/>
+      <c r="K4" s="78"/>
+      <c r="L4" s="78"/>
+      <c r="M4" s="78"/>
+      <c r="N4" s="78"/>
+      <c r="O4" s="78"/>
+      <c r="P4" s="78"/>
+      <c r="Q4" s="78"/>
+      <c r="R4" s="78"/>
+      <c r="S4" s="78"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="B5" s="81"/>
-      <c r="C5" s="81"/>
-      <c r="D5" s="81"/>
-      <c r="E5" s="81"/>
-      <c r="F5" s="81"/>
-      <c r="G5" s="81"/>
-      <c r="H5" s="81"/>
-      <c r="I5" s="81"/>
-      <c r="J5" s="81"/>
-      <c r="K5" s="81"/>
-      <c r="L5" s="81"/>
-      <c r="M5" s="81"/>
-      <c r="N5" s="81"/>
-      <c r="O5" s="81"/>
-      <c r="P5" s="81"/>
-      <c r="Q5" s="81"/>
-      <c r="R5" s="81"/>
-      <c r="S5" s="81"/>
+      <c r="B5" s="78"/>
+      <c r="C5" s="78"/>
+      <c r="D5" s="78"/>
+      <c r="E5" s="78"/>
+      <c r="F5" s="78"/>
+      <c r="G5" s="78"/>
+      <c r="H5" s="78"/>
+      <c r="I5" s="78"/>
+      <c r="J5" s="78"/>
+      <c r="K5" s="78"/>
+      <c r="L5" s="78"/>
+      <c r="M5" s="78"/>
+      <c r="N5" s="78"/>
+      <c r="O5" s="78"/>
+      <c r="P5" s="78"/>
+      <c r="Q5" s="78"/>
+      <c r="R5" s="78"/>
+      <c r="S5" s="78"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="B6" s="81"/>
-      <c r="C6" s="81"/>
-      <c r="D6" s="81"/>
-      <c r="E6" s="81"/>
-      <c r="F6" s="81"/>
-      <c r="G6" s="81"/>
-      <c r="H6" s="81"/>
-      <c r="I6" s="81"/>
-      <c r="J6" s="81"/>
-      <c r="K6" s="81"/>
-      <c r="L6" s="81"/>
-      <c r="M6" s="81"/>
-      <c r="N6" s="81"/>
-      <c r="O6" s="81"/>
-      <c r="P6" s="81"/>
-      <c r="Q6" s="81"/>
-      <c r="R6" s="81"/>
-      <c r="S6" s="81"/>
+      <c r="B6" s="78"/>
+      <c r="C6" s="78"/>
+      <c r="D6" s="78"/>
+      <c r="E6" s="78"/>
+      <c r="F6" s="78"/>
+      <c r="G6" s="78"/>
+      <c r="H6" s="78"/>
+      <c r="I6" s="78"/>
+      <c r="J6" s="78"/>
+      <c r="K6" s="78"/>
+      <c r="L6" s="78"/>
+      <c r="M6" s="78"/>
+      <c r="N6" s="78"/>
+      <c r="O6" s="78"/>
+      <c r="P6" s="78"/>
+      <c r="Q6" s="78"/>
+      <c r="R6" s="78"/>
+      <c r="S6" s="78"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="B7" s="81"/>
-      <c r="C7" s="81"/>
-      <c r="D7" s="81"/>
-      <c r="E7" s="81"/>
-      <c r="F7" s="81"/>
-      <c r="G7" s="81"/>
-      <c r="H7" s="81"/>
-      <c r="I7" s="81"/>
-      <c r="J7" s="81"/>
-      <c r="K7" s="81"/>
-      <c r="L7" s="81"/>
-      <c r="M7" s="81"/>
-      <c r="N7" s="81"/>
-      <c r="O7" s="81"/>
-      <c r="P7" s="81"/>
-      <c r="Q7" s="81"/>
-      <c r="R7" s="81"/>
-      <c r="S7" s="81"/>
+      <c r="B7" s="78"/>
+      <c r="C7" s="78"/>
+      <c r="D7" s="78"/>
+      <c r="E7" s="78"/>
+      <c r="F7" s="78"/>
+      <c r="G7" s="78"/>
+      <c r="H7" s="78"/>
+      <c r="I7" s="78"/>
+      <c r="J7" s="78"/>
+      <c r="K7" s="78"/>
+      <c r="L7" s="78"/>
+      <c r="M7" s="78"/>
+      <c r="N7" s="78"/>
+      <c r="O7" s="78"/>
+      <c r="P7" s="78"/>
+      <c r="Q7" s="78"/>
+      <c r="R7" s="78"/>
+      <c r="S7" s="78"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="B8" s="81"/>
-      <c r="C8" s="81"/>
-      <c r="D8" s="81"/>
-      <c r="E8" s="81"/>
-      <c r="F8" s="81"/>
-      <c r="G8" s="81"/>
-      <c r="H8" s="81"/>
-      <c r="I8" s="81"/>
-      <c r="J8" s="81"/>
-      <c r="K8" s="81"/>
-      <c r="L8" s="81"/>
-      <c r="M8" s="81"/>
-      <c r="N8" s="81"/>
-      <c r="O8" s="81"/>
-      <c r="P8" s="81"/>
-      <c r="Q8" s="81"/>
-      <c r="R8" s="81"/>
-      <c r="S8" s="81"/>
+      <c r="B8" s="78"/>
+      <c r="C8" s="78"/>
+      <c r="D8" s="78"/>
+      <c r="E8" s="78"/>
+      <c r="F8" s="78"/>
+      <c r="G8" s="78"/>
+      <c r="H8" s="78"/>
+      <c r="I8" s="78"/>
+      <c r="J8" s="78"/>
+      <c r="K8" s="78"/>
+      <c r="L8" s="78"/>
+      <c r="M8" s="78"/>
+      <c r="N8" s="78"/>
+      <c r="O8" s="78"/>
+      <c r="P8" s="78"/>
+      <c r="Q8" s="78"/>
+      <c r="R8" s="78"/>
+      <c r="S8" s="78"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="B9" s="81"/>
-      <c r="C9" s="81"/>
-      <c r="D9" s="81"/>
-      <c r="E9" s="81"/>
-      <c r="F9" s="81"/>
-      <c r="G9" s="81"/>
-      <c r="H9" s="81"/>
-      <c r="I9" s="81"/>
-      <c r="J9" s="81"/>
-      <c r="K9" s="81"/>
-      <c r="L9" s="81"/>
-      <c r="M9" s="81"/>
-      <c r="N9" s="81"/>
-      <c r="O9" s="81"/>
-      <c r="P9" s="81"/>
-      <c r="Q9" s="81"/>
-      <c r="R9" s="81"/>
-      <c r="S9" s="81"/>
+      <c r="B9" s="78"/>
+      <c r="C9" s="78"/>
+      <c r="D9" s="78"/>
+      <c r="E9" s="78"/>
+      <c r="F9" s="78"/>
+      <c r="G9" s="78"/>
+      <c r="H9" s="78"/>
+      <c r="I9" s="78"/>
+      <c r="J9" s="78"/>
+      <c r="K9" s="78"/>
+      <c r="L9" s="78"/>
+      <c r="M9" s="78"/>
+      <c r="N9" s="78"/>
+      <c r="O9" s="78"/>
+      <c r="P9" s="78"/>
+      <c r="Q9" s="78"/>
+      <c r="R9" s="78"/>
+      <c r="S9" s="78"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="B10" s="81"/>
-      <c r="C10" s="81"/>
-      <c r="D10" s="81"/>
-      <c r="E10" s="81"/>
-      <c r="F10" s="81"/>
-      <c r="G10" s="81"/>
-      <c r="H10" s="81"/>
-      <c r="I10" s="81"/>
-      <c r="J10" s="81"/>
-      <c r="K10" s="81"/>
-      <c r="L10" s="81"/>
-      <c r="M10" s="81"/>
-      <c r="N10" s="81"/>
-      <c r="O10" s="81"/>
-      <c r="P10" s="81"/>
-      <c r="Q10" s="81"/>
-      <c r="R10" s="81"/>
-      <c r="S10" s="81"/>
+      <c r="B10" s="78"/>
+      <c r="C10" s="78"/>
+      <c r="D10" s="78"/>
+      <c r="E10" s="78"/>
+      <c r="F10" s="78"/>
+      <c r="G10" s="78"/>
+      <c r="H10" s="78"/>
+      <c r="I10" s="78"/>
+      <c r="J10" s="78"/>
+      <c r="K10" s="78"/>
+      <c r="L10" s="78"/>
+      <c r="M10" s="78"/>
+      <c r="N10" s="78"/>
+      <c r="O10" s="78"/>
+      <c r="P10" s="78"/>
+      <c r="Q10" s="78"/>
+      <c r="R10" s="78"/>
+      <c r="S10" s="78"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="B11" s="81"/>
-      <c r="C11" s="81"/>
-      <c r="D11" s="81"/>
-      <c r="E11" s="81"/>
-      <c r="F11" s="81"/>
-      <c r="G11" s="81"/>
-      <c r="H11" s="81"/>
-      <c r="I11" s="81"/>
-      <c r="J11" s="81"/>
-      <c r="K11" s="81"/>
-      <c r="L11" s="81"/>
-      <c r="M11" s="81"/>
-      <c r="N11" s="81"/>
-      <c r="O11" s="81"/>
-      <c r="P11" s="81"/>
-      <c r="Q11" s="81"/>
-      <c r="R11" s="81"/>
-      <c r="S11" s="81"/>
+      <c r="B11" s="78"/>
+      <c r="C11" s="78"/>
+      <c r="D11" s="78"/>
+      <c r="E11" s="78"/>
+      <c r="F11" s="78"/>
+      <c r="G11" s="78"/>
+      <c r="H11" s="78"/>
+      <c r="I11" s="78"/>
+      <c r="J11" s="78"/>
+      <c r="K11" s="78"/>
+      <c r="L11" s="78"/>
+      <c r="M11" s="78"/>
+      <c r="N11" s="78"/>
+      <c r="O11" s="78"/>
+      <c r="P11" s="78"/>
+      <c r="Q11" s="78"/>
+      <c r="R11" s="78"/>
+      <c r="S11" s="78"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="B12" s="81"/>
-      <c r="C12" s="81"/>
-      <c r="D12" s="81"/>
-      <c r="E12" s="81"/>
-      <c r="F12" s="81"/>
-      <c r="G12" s="81"/>
-      <c r="H12" s="81"/>
-      <c r="I12" s="81"/>
-      <c r="J12" s="81"/>
-      <c r="K12" s="81"/>
-      <c r="L12" s="81"/>
-      <c r="M12" s="81"/>
-      <c r="N12" s="81"/>
-      <c r="O12" s="81"/>
-      <c r="P12" s="81"/>
-      <c r="Q12" s="81"/>
-      <c r="R12" s="81"/>
-      <c r="S12" s="81"/>
+      <c r="B12" s="78"/>
+      <c r="C12" s="78"/>
+      <c r="D12" s="78"/>
+      <c r="E12" s="78"/>
+      <c r="F12" s="78"/>
+      <c r="G12" s="78"/>
+      <c r="H12" s="78"/>
+      <c r="I12" s="78"/>
+      <c r="J12" s="78"/>
+      <c r="K12" s="78"/>
+      <c r="L12" s="78"/>
+      <c r="M12" s="78"/>
+      <c r="N12" s="78"/>
+      <c r="O12" s="78"/>
+      <c r="P12" s="78"/>
+      <c r="Q12" s="78"/>
+      <c r="R12" s="78"/>
+      <c r="S12" s="78"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="B13" s="81"/>
-      <c r="C13" s="81"/>
-      <c r="D13" s="81"/>
-      <c r="E13" s="81"/>
-      <c r="F13" s="81"/>
-      <c r="G13" s="81"/>
-      <c r="H13" s="81"/>
-      <c r="I13" s="81"/>
-      <c r="J13" s="81"/>
-      <c r="K13" s="81"/>
-      <c r="L13" s="81"/>
-      <c r="M13" s="81"/>
-      <c r="N13" s="81"/>
-      <c r="O13" s="81"/>
-      <c r="P13" s="81"/>
-      <c r="Q13" s="81"/>
-      <c r="R13" s="81"/>
-      <c r="S13" s="81"/>
+      <c r="B13" s="78"/>
+      <c r="C13" s="78"/>
+      <c r="D13" s="78"/>
+      <c r="E13" s="78"/>
+      <c r="F13" s="78"/>
+      <c r="G13" s="78"/>
+      <c r="H13" s="78"/>
+      <c r="I13" s="78"/>
+      <c r="J13" s="78"/>
+      <c r="K13" s="78"/>
+      <c r="L13" s="78"/>
+      <c r="M13" s="78"/>
+      <c r="N13" s="78"/>
+      <c r="O13" s="78"/>
+      <c r="P13" s="78"/>
+      <c r="Q13" s="78"/>
+      <c r="R13" s="78"/>
+      <c r="S13" s="78"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
-      <c r="B14" s="78"/>
-      <c r="C14" s="79"/>
-      <c r="D14" s="80"/>
-      <c r="E14" s="78"/>
-      <c r="F14" s="79"/>
-      <c r="G14" s="80"/>
-      <c r="H14" s="78"/>
-      <c r="I14" s="79"/>
-      <c r="J14" s="80"/>
+      <c r="B14" s="79"/>
+      <c r="C14" s="80"/>
+      <c r="D14" s="81"/>
+      <c r="E14" s="79"/>
+      <c r="F14" s="80"/>
+      <c r="G14" s="81"/>
+      <c r="H14" s="79"/>
+      <c r="I14" s="80"/>
+      <c r="J14" s="81"/>
       <c r="K14" s="77"/>
       <c r="L14" s="77"/>
       <c r="M14" s="77"/>
@@ -7553,12 +7731,12 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="Q2:S2"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="K2:M2"/>
-    <mergeCell ref="N2:P2"/>
+    <mergeCell ref="K14:M14"/>
+    <mergeCell ref="N14:P14"/>
+    <mergeCell ref="Q14:S14"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="H14:J14"/>
     <mergeCell ref="N3:P3"/>
     <mergeCell ref="Q3:S3"/>
     <mergeCell ref="B4:D13"/>
@@ -7571,12 +7749,12 @@
     <mergeCell ref="E3:G3"/>
     <mergeCell ref="H3:J3"/>
     <mergeCell ref="K3:M3"/>
-    <mergeCell ref="K14:M14"/>
-    <mergeCell ref="N14:P14"/>
-    <mergeCell ref="Q14:S14"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="H14:J14"/>
+    <mergeCell ref="Q2:S2"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="K2:M2"/>
+    <mergeCell ref="N2:P2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7584,12 +7762,301 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B51242B0-8199-4649-98A5-8BB48574D175}">
-  <dimension ref="A1"/>
+  <dimension ref="B2:O12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12:L12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="6" max="6" width="11.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B2" s="83"/>
+      <c r="C2" s="89" t="s">
+        <v>172</v>
+      </c>
+      <c r="D2" s="90" t="s">
+        <v>174</v>
+      </c>
+      <c r="E2" s="90" t="s">
+        <v>175</v>
+      </c>
+      <c r="F2" s="90" t="s">
+        <v>176</v>
+      </c>
+      <c r="G2" s="90" t="s">
+        <v>178</v>
+      </c>
+      <c r="H2" s="90"/>
+      <c r="I2" s="90"/>
+      <c r="J2" s="90"/>
+      <c r="K2" s="90"/>
+      <c r="L2" s="91"/>
+    </row>
+    <row r="3" spans="2:15" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B3" s="83"/>
+      <c r="C3" s="92" t="s">
+        <v>168</v>
+      </c>
+      <c r="D3" s="93" t="s">
+        <v>173</v>
+      </c>
+      <c r="E3" s="93" t="s">
+        <v>173</v>
+      </c>
+      <c r="F3" s="93" t="s">
+        <v>177</v>
+      </c>
+      <c r="G3" s="93" t="s">
+        <v>179</v>
+      </c>
+      <c r="H3" s="93"/>
+      <c r="I3" s="93"/>
+      <c r="J3" s="93"/>
+      <c r="K3" s="93"/>
+      <c r="L3" s="94"/>
+    </row>
+    <row r="4" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B4" s="83" t="s">
+        <v>169</v>
+      </c>
+      <c r="C4" s="95">
+        <v>1</v>
+      </c>
+      <c r="D4" s="96">
+        <v>2</v>
+      </c>
+      <c r="E4" s="96">
+        <v>2</v>
+      </c>
+      <c r="F4" s="96">
+        <v>3</v>
+      </c>
+      <c r="G4" s="96">
+        <v>4</v>
+      </c>
+      <c r="H4" s="96"/>
+      <c r="I4" s="96"/>
+      <c r="J4" s="96"/>
+      <c r="K4" s="96"/>
+      <c r="L4" s="97"/>
+    </row>
+    <row r="5" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B5" s="86" t="s">
+        <v>57</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5">
+        <v>3</v>
+      </c>
+      <c r="G5">
+        <v>2</v>
+      </c>
+      <c r="H5" s="84"/>
+      <c r="I5" s="84"/>
+      <c r="J5" s="84"/>
+      <c r="K5" s="84"/>
+      <c r="L5" s="84"/>
+    </row>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B6" s="87" t="s">
+        <v>58</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="F6">
+        <v>3</v>
+      </c>
+      <c r="G6">
+        <v>4</v>
+      </c>
+      <c r="H6" s="83"/>
+      <c r="I6" s="83"/>
+      <c r="J6" s="84"/>
+      <c r="K6" s="84"/>
+      <c r="L6" s="84"/>
+      <c r="O6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B7" s="87" t="s">
+        <v>170</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="F7">
+        <v>3</v>
+      </c>
+      <c r="G7">
+        <v>2</v>
+      </c>
+      <c r="H7" s="84"/>
+      <c r="I7" s="84"/>
+      <c r="J7" s="84"/>
+      <c r="K7" s="84"/>
+      <c r="L7" s="84"/>
+      <c r="O7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B8" s="87" t="s">
+        <v>60</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+      <c r="F8">
+        <v>3</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8" s="84"/>
+      <c r="I8" s="84"/>
+      <c r="J8" s="84"/>
+      <c r="K8" s="84"/>
+      <c r="L8" s="84"/>
+      <c r="O8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B9" s="87" t="s">
+        <v>171</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+      <c r="F9">
+        <v>3</v>
+      </c>
+      <c r="G9">
+        <v>4</v>
+      </c>
+      <c r="H9" s="84"/>
+      <c r="I9" s="84"/>
+      <c r="J9" s="84"/>
+      <c r="K9" s="84"/>
+      <c r="L9" s="84"/>
+      <c r="O9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B10" s="87" t="s">
+        <v>62</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="E10">
+        <v>2</v>
+      </c>
+      <c r="F10">
+        <v>3</v>
+      </c>
+      <c r="G10">
+        <v>3</v>
+      </c>
+      <c r="H10" s="84"/>
+      <c r="I10" s="84"/>
+      <c r="J10" s="84"/>
+      <c r="K10" s="84"/>
+      <c r="L10" s="84"/>
+    </row>
+    <row r="11" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B11" s="88" t="s">
+        <v>63</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+      <c r="E11">
+        <v>2</v>
+      </c>
+      <c r="F11">
+        <v>3</v>
+      </c>
+      <c r="G11">
+        <v>4</v>
+      </c>
+      <c r="H11" s="85"/>
+      <c r="I11" s="85"/>
+      <c r="J11" s="85"/>
+      <c r="K11" s="85"/>
+      <c r="L11" s="85"/>
+    </row>
+    <row r="12" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B12" s="98" t="s">
+        <v>64</v>
+      </c>
+      <c r="C12" s="99">
+        <v>7</v>
+      </c>
+      <c r="D12" s="100">
+        <v>14</v>
+      </c>
+      <c r="E12" s="100">
+        <v>14</v>
+      </c>
+      <c r="F12" s="100">
+        <v>35</v>
+      </c>
+      <c r="G12" s="100">
+        <v>4</v>
+      </c>
+      <c r="H12" s="100"/>
+      <c r="I12" s="100"/>
+      <c r="J12" s="100"/>
+      <c r="K12" s="100"/>
+      <c r="L12" s="101"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added Player to Amazoon
</commit_message>
<xml_diff>
--- a/383Game/Doc/Brain Stew Master Gantt Chart.xlsx
+++ b/383Game/Doc/Brain Stew Master Gantt Chart.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/19db3ad368368567/Documents/GitHub/CS383BrainstewGame/383Game/Doc/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jcjab\Documents\GitHub\CS383BrainstewGame\383Game\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="86" documentId="13_ncr:1_{B97EFEB6-BC69-234F-B622-F5F1D74BC570}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7D4DD9EC-19B7-44CE-A9A1-CFA09F2FF91A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76FEBAE3-2AD1-4360-8558-1A30AAB88F6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3087" yWindow="3093" windowWidth="19200" windowHeight="10074" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Budget" sheetId="1" r:id="rId1"/>
@@ -916,7 +916,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="116">
+  <cellXfs count="114">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1042,40 +1042,25 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="5" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1096,61 +1081,70 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="5" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1418,597 +1412,650 @@
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.64453125" defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="9" max="9" width="10.6640625" customWidth="1"/>
-    <col min="17" max="17" width="10.33203125" customWidth="1"/>
+    <col min="9" max="9" width="10.64453125" customWidth="1"/>
+    <col min="17" max="17" width="10.3515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C2" s="89" t="s">
+    <row r="2" spans="2:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="C2" s="88" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="89"/>
-      <c r="E2" s="89"/>
-      <c r="F2" s="89"/>
-      <c r="G2" s="89"/>
-      <c r="H2" s="89"/>
-      <c r="K2" s="89" t="s">
+      <c r="D2" s="88"/>
+      <c r="E2" s="88"/>
+      <c r="F2" s="88"/>
+      <c r="G2" s="88"/>
+      <c r="H2" s="88"/>
+      <c r="K2" s="88" t="s">
         <v>1</v>
       </c>
-      <c r="L2" s="89"/>
-      <c r="M2" s="89"/>
-      <c r="N2" s="89"/>
-      <c r="O2" s="89"/>
-      <c r="P2" s="89"/>
-      <c r="S2" s="89" t="s">
+      <c r="L2" s="88"/>
+      <c r="M2" s="88"/>
+      <c r="N2" s="88"/>
+      <c r="O2" s="88"/>
+      <c r="P2" s="88"/>
+      <c r="S2" s="88" t="s">
         <v>2</v>
       </c>
-      <c r="T2" s="89"/>
-      <c r="U2" s="89"/>
-      <c r="V2" s="89"/>
-      <c r="W2" s="89"/>
-      <c r="X2" s="89"/>
-      <c r="AA2" s="89" t="s">
+      <c r="T2" s="88"/>
+      <c r="U2" s="88"/>
+      <c r="V2" s="88"/>
+      <c r="W2" s="88"/>
+      <c r="X2" s="88"/>
+      <c r="AA2" s="88" t="s">
         <v>3</v>
       </c>
-      <c r="AB2" s="89"/>
-      <c r="AC2" s="89"/>
-      <c r="AD2" s="89"/>
-      <c r="AE2" s="89"/>
-      <c r="AF2" s="89"/>
-    </row>
-    <row r="3" spans="2:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="90" t="s">
+      <c r="AB2" s="88"/>
+      <c r="AC2" s="88"/>
+      <c r="AD2" s="88"/>
+      <c r="AE2" s="88"/>
+      <c r="AF2" s="88"/>
+    </row>
+    <row r="3" spans="2:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="C3" s="89" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="90"/>
-      <c r="E3" s="91" t="s">
+      <c r="D3" s="89"/>
+      <c r="E3" s="90" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="91"/>
-      <c r="G3" s="92" t="s">
+      <c r="F3" s="90"/>
+      <c r="G3" s="91" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="92"/>
-      <c r="K3" s="90" t="s">
+      <c r="H3" s="91"/>
+      <c r="K3" s="89" t="s">
         <v>4</v>
       </c>
-      <c r="L3" s="90"/>
-      <c r="M3" s="91" t="s">
+      <c r="L3" s="89"/>
+      <c r="M3" s="90" t="s">
         <v>5</v>
       </c>
-      <c r="N3" s="91"/>
-      <c r="O3" s="92" t="s">
+      <c r="N3" s="90"/>
+      <c r="O3" s="91" t="s">
         <v>6</v>
       </c>
-      <c r="P3" s="92"/>
-      <c r="S3" s="90" t="s">
+      <c r="P3" s="91"/>
+      <c r="S3" s="89" t="s">
         <v>4</v>
       </c>
-      <c r="T3" s="90"/>
-      <c r="U3" s="91" t="s">
+      <c r="T3" s="89"/>
+      <c r="U3" s="90" t="s">
         <v>5</v>
       </c>
-      <c r="V3" s="91"/>
-      <c r="W3" s="92" t="s">
+      <c r="V3" s="90"/>
+      <c r="W3" s="91" t="s">
         <v>6</v>
       </c>
-      <c r="X3" s="92"/>
-      <c r="AA3" s="90" t="s">
+      <c r="X3" s="91"/>
+      <c r="AA3" s="89" t="s">
         <v>4</v>
       </c>
-      <c r="AB3" s="90"/>
-      <c r="AC3" s="91" t="s">
+      <c r="AB3" s="89"/>
+      <c r="AC3" s="90" t="s">
         <v>5</v>
       </c>
-      <c r="AD3" s="91"/>
-      <c r="AE3" s="92" t="s">
+      <c r="AD3" s="90"/>
+      <c r="AE3" s="91" t="s">
         <v>6</v>
       </c>
-      <c r="AF3" s="92"/>
-    </row>
-    <row r="4" spans="2:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AF3" s="91"/>
+    </row>
+    <row r="4" spans="2:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="108">
+      <c r="C4" s="84">
         <v>8200</v>
       </c>
-      <c r="D4" s="108"/>
-      <c r="E4" s="102">
+      <c r="D4" s="84"/>
+      <c r="E4" s="85">
         <v>2500</v>
       </c>
-      <c r="F4" s="87"/>
-      <c r="G4" s="88" t="s">
+      <c r="F4" s="86"/>
+      <c r="G4" s="87" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="88"/>
+      <c r="H4" s="87"/>
       <c r="J4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K4" s="79">
+      <c r="K4" s="98">
         <v>5200</v>
       </c>
-      <c r="L4" s="79"/>
-      <c r="M4" s="102">
+      <c r="L4" s="98"/>
+      <c r="M4" s="85">
         <v>1400</v>
       </c>
-      <c r="N4" s="87"/>
-      <c r="O4" s="88" t="s">
+      <c r="N4" s="86"/>
+      <c r="O4" s="87" t="s">
         <v>8</v>
       </c>
-      <c r="P4" s="88"/>
+      <c r="P4" s="87"/>
       <c r="R4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="S4" s="108">
+      <c r="S4" s="84">
         <v>3000</v>
       </c>
-      <c r="T4" s="108"/>
-      <c r="U4" s="102">
+      <c r="T4" s="84"/>
+      <c r="U4" s="85">
         <v>1100</v>
       </c>
-      <c r="V4" s="87"/>
-      <c r="W4" s="88" t="s">
+      <c r="V4" s="86"/>
+      <c r="W4" s="87" t="s">
         <v>8</v>
       </c>
-      <c r="X4" s="88"/>
+      <c r="X4" s="87"/>
       <c r="Z4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="AA4" s="86"/>
-      <c r="AB4" s="86"/>
-      <c r="AC4" s="87"/>
-      <c r="AD4" s="87"/>
-      <c r="AE4" s="88"/>
-      <c r="AF4" s="88"/>
-    </row>
-    <row r="5" spans="2:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AA4" s="95"/>
+      <c r="AB4" s="95"/>
+      <c r="AC4" s="86"/>
+      <c r="AD4" s="86"/>
+      <c r="AE4" s="87"/>
+      <c r="AF4" s="87"/>
+    </row>
+    <row r="5" spans="2:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="108">
+      <c r="C5" s="84">
         <v>10200</v>
       </c>
-      <c r="D5" s="108"/>
-      <c r="E5" s="112">
+      <c r="D5" s="84"/>
+      <c r="E5" s="92">
         <v>3100</v>
       </c>
-      <c r="F5" s="106"/>
-      <c r="G5" s="84" t="s">
+      <c r="F5" s="93"/>
+      <c r="G5" s="94" t="s">
         <v>8</v>
       </c>
-      <c r="H5" s="84"/>
+      <c r="H5" s="94"/>
       <c r="J5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K5" s="85">
+      <c r="K5" s="96">
         <v>7200</v>
       </c>
-      <c r="L5" s="85"/>
-      <c r="M5" s="103">
+      <c r="L5" s="96"/>
+      <c r="M5" s="92">
         <v>1900</v>
       </c>
-      <c r="N5" s="75"/>
-      <c r="O5" s="84" t="s">
+      <c r="N5" s="93"/>
+      <c r="O5" s="94" t="s">
         <v>8</v>
       </c>
-      <c r="P5" s="84"/>
+      <c r="P5" s="94"/>
       <c r="R5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="S5" s="108">
+      <c r="S5" s="84">
         <v>3000</v>
       </c>
-      <c r="T5" s="108"/>
-      <c r="U5" s="103">
+      <c r="T5" s="84"/>
+      <c r="U5" s="92">
         <v>1200</v>
       </c>
-      <c r="V5" s="75"/>
-      <c r="W5" s="84" t="s">
+      <c r="V5" s="93"/>
+      <c r="W5" s="94" t="s">
         <v>8</v>
       </c>
-      <c r="X5" s="84"/>
+      <c r="X5" s="94"/>
       <c r="Z5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="AA5" s="83"/>
-      <c r="AB5" s="83"/>
-      <c r="AC5" s="75"/>
-      <c r="AD5" s="75"/>
-      <c r="AE5" s="84"/>
-      <c r="AF5" s="84"/>
-    </row>
-    <row r="6" spans="2:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AA5" s="97"/>
+      <c r="AB5" s="97"/>
+      <c r="AC5" s="93"/>
+      <c r="AD5" s="93"/>
+      <c r="AE5" s="94"/>
+      <c r="AF5" s="94"/>
+    </row>
+    <row r="6" spans="2:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="108">
+      <c r="C6" s="84">
         <v>8300</v>
       </c>
-      <c r="D6" s="108"/>
-      <c r="E6" s="112">
+      <c r="D6" s="84"/>
+      <c r="E6" s="92">
         <v>1600</v>
       </c>
-      <c r="F6" s="106"/>
-      <c r="G6" s="84" t="s">
+      <c r="F6" s="93"/>
+      <c r="G6" s="94" t="s">
         <v>8</v>
       </c>
-      <c r="H6" s="84"/>
+      <c r="H6" s="94"/>
       <c r="J6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="K6" s="85">
+      <c r="K6" s="96">
         <v>5300</v>
       </c>
-      <c r="L6" s="85"/>
-      <c r="M6" s="103">
+      <c r="L6" s="96"/>
+      <c r="M6" s="92">
         <v>600</v>
       </c>
-      <c r="N6" s="75"/>
-      <c r="O6" s="84" t="s">
+      <c r="N6" s="93"/>
+      <c r="O6" s="94" t="s">
         <v>8</v>
       </c>
-      <c r="P6" s="84"/>
+      <c r="P6" s="94"/>
       <c r="R6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="S6" s="108">
+      <c r="S6" s="84">
         <v>3000</v>
       </c>
-      <c r="T6" s="108"/>
-      <c r="U6" s="103">
+      <c r="T6" s="84"/>
+      <c r="U6" s="92">
         <v>1000</v>
       </c>
-      <c r="V6" s="75"/>
-      <c r="W6" s="84" t="s">
+      <c r="V6" s="93"/>
+      <c r="W6" s="94" t="s">
         <v>8</v>
       </c>
-      <c r="X6" s="84"/>
+      <c r="X6" s="94"/>
       <c r="Z6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="AA6" s="83"/>
-      <c r="AB6" s="83"/>
-      <c r="AC6" s="75"/>
-      <c r="AD6" s="75"/>
-      <c r="AE6" s="84"/>
-      <c r="AF6" s="84"/>
-    </row>
-    <row r="7" spans="2:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AA6" s="97"/>
+      <c r="AB6" s="97"/>
+      <c r="AC6" s="93"/>
+      <c r="AD6" s="93"/>
+      <c r="AE6" s="94"/>
+      <c r="AF6" s="94"/>
+    </row>
+    <row r="7" spans="2:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="108">
+      <c r="C7" s="84">
         <v>9000</v>
       </c>
-      <c r="D7" s="108"/>
-      <c r="E7" s="112">
+      <c r="D7" s="84"/>
+      <c r="E7" s="92">
         <v>1300</v>
       </c>
-      <c r="F7" s="106"/>
-      <c r="G7" s="84" t="s">
+      <c r="F7" s="93"/>
+      <c r="G7" s="94" t="s">
         <v>8</v>
       </c>
-      <c r="H7" s="84"/>
+      <c r="H7" s="94"/>
       <c r="J7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="K7" s="85">
+      <c r="K7" s="96">
         <v>6000</v>
       </c>
-      <c r="L7" s="85"/>
-      <c r="M7" s="103">
+      <c r="L7" s="96"/>
+      <c r="M7" s="92">
         <v>400</v>
       </c>
-      <c r="N7" s="75"/>
-      <c r="O7" s="84" t="s">
+      <c r="N7" s="93"/>
+      <c r="O7" s="94" t="s">
         <v>8</v>
       </c>
-      <c r="P7" s="84"/>
+      <c r="P7" s="94"/>
       <c r="R7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="S7" s="108">
+      <c r="S7" s="84">
         <v>3000</v>
       </c>
-      <c r="T7" s="108"/>
-      <c r="U7" s="103">
+      <c r="T7" s="84"/>
+      <c r="U7" s="92">
         <v>900</v>
       </c>
-      <c r="V7" s="75"/>
-      <c r="W7" s="84" t="s">
+      <c r="V7" s="93"/>
+      <c r="W7" s="94" t="s">
         <v>8</v>
       </c>
-      <c r="X7" s="84"/>
+      <c r="X7" s="94"/>
       <c r="Z7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="AA7" s="83"/>
-      <c r="AB7" s="83"/>
-      <c r="AC7" s="75"/>
-      <c r="AD7" s="75"/>
-      <c r="AE7" s="84"/>
-      <c r="AF7" s="84"/>
-    </row>
-    <row r="8" spans="2:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AA7" s="97"/>
+      <c r="AB7" s="97"/>
+      <c r="AC7" s="93"/>
+      <c r="AD7" s="93"/>
+      <c r="AE7" s="94"/>
+      <c r="AF7" s="94"/>
+    </row>
+    <row r="8" spans="2:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="108">
+      <c r="C8" s="84">
         <v>9300</v>
       </c>
-      <c r="D8" s="108"/>
-      <c r="E8" s="112">
+      <c r="D8" s="84"/>
+      <c r="E8" s="92">
         <v>1900</v>
       </c>
-      <c r="F8" s="106"/>
-      <c r="G8" s="84" t="s">
+      <c r="F8" s="93"/>
+      <c r="G8" s="94" t="s">
         <v>8</v>
       </c>
-      <c r="H8" s="84"/>
+      <c r="H8" s="94"/>
       <c r="J8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="K8" s="85">
+      <c r="K8" s="96">
         <v>6300</v>
       </c>
-      <c r="L8" s="85"/>
-      <c r="M8" s="103">
+      <c r="L8" s="96"/>
+      <c r="M8" s="92">
         <v>600</v>
       </c>
-      <c r="N8" s="75"/>
-      <c r="O8" s="84" t="s">
+      <c r="N8" s="93"/>
+      <c r="O8" s="94" t="s">
         <v>8</v>
       </c>
-      <c r="P8" s="84"/>
+      <c r="P8" s="94"/>
       <c r="R8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="S8" s="108">
+      <c r="S8" s="84">
         <v>3000</v>
       </c>
-      <c r="T8" s="108"/>
-      <c r="U8" s="103">
+      <c r="T8" s="84"/>
+      <c r="U8" s="92">
         <v>1300</v>
       </c>
-      <c r="V8" s="75"/>
-      <c r="W8" s="84" t="s">
+      <c r="V8" s="93"/>
+      <c r="W8" s="94" t="s">
         <v>8</v>
       </c>
-      <c r="X8" s="84"/>
+      <c r="X8" s="94"/>
       <c r="Z8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="AA8" s="83"/>
-      <c r="AB8" s="83"/>
-      <c r="AC8" s="75"/>
-      <c r="AD8" s="75"/>
-      <c r="AE8" s="84"/>
-      <c r="AF8" s="84"/>
-    </row>
-    <row r="9" spans="2:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AA8" s="97"/>
+      <c r="AB8" s="97"/>
+      <c r="AC8" s="93"/>
+      <c r="AD8" s="93"/>
+      <c r="AE8" s="94"/>
+      <c r="AF8" s="94"/>
+    </row>
+    <row r="9" spans="2:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="108">
+      <c r="C9" s="84">
         <v>8500</v>
       </c>
-      <c r="D9" s="108"/>
-      <c r="E9" s="112">
+      <c r="D9" s="84"/>
+      <c r="E9" s="92">
         <v>4400</v>
       </c>
-      <c r="F9" s="106"/>
-      <c r="G9" s="84" t="s">
+      <c r="F9" s="93"/>
+      <c r="G9" s="94" t="s">
         <v>8</v>
       </c>
-      <c r="H9" s="84"/>
+      <c r="H9" s="94"/>
       <c r="J9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="K9" s="85">
+      <c r="K9" s="96">
         <v>5500</v>
       </c>
-      <c r="L9" s="85"/>
-      <c r="M9" s="103">
+      <c r="L9" s="96"/>
+      <c r="M9" s="92">
         <v>2200</v>
       </c>
-      <c r="N9" s="75"/>
-      <c r="O9" s="84" t="s">
+      <c r="N9" s="93"/>
+      <c r="O9" s="94" t="s">
         <v>8</v>
       </c>
-      <c r="P9" s="84"/>
+      <c r="P9" s="94"/>
       <c r="R9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="S9" s="108">
+      <c r="S9" s="84">
         <v>3000</v>
       </c>
-      <c r="T9" s="108"/>
-      <c r="U9" s="103">
+      <c r="T9" s="84"/>
+      <c r="U9" s="92">
         <v>1200</v>
       </c>
-      <c r="V9" s="75"/>
-      <c r="W9" s="84" t="s">
+      <c r="V9" s="93"/>
+      <c r="W9" s="94" t="s">
         <v>8</v>
       </c>
-      <c r="X9" s="84"/>
+      <c r="X9" s="94"/>
       <c r="Z9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="AA9" s="83"/>
-      <c r="AB9" s="83"/>
-      <c r="AC9" s="75"/>
-      <c r="AD9" s="75"/>
-      <c r="AE9" s="84"/>
-      <c r="AF9" s="84"/>
-    </row>
-    <row r="10" spans="2:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AA9" s="97"/>
+      <c r="AB9" s="97"/>
+      <c r="AC9" s="93"/>
+      <c r="AD9" s="93"/>
+      <c r="AE9" s="94"/>
+      <c r="AF9" s="94"/>
+    </row>
+    <row r="10" spans="2:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B10" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="108">
+      <c r="C10" s="84">
         <v>8800</v>
       </c>
-      <c r="D10" s="108"/>
-      <c r="E10" s="112">
+      <c r="D10" s="84"/>
+      <c r="E10" s="92">
         <v>3600</v>
       </c>
-      <c r="F10" s="106"/>
-      <c r="G10" s="84" t="s">
+      <c r="F10" s="93"/>
+      <c r="G10" s="94" t="s">
         <v>8</v>
       </c>
-      <c r="H10" s="84"/>
+      <c r="H10" s="94"/>
       <c r="J10" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="K10" s="80">
+      <c r="K10" s="106">
         <v>5800</v>
       </c>
-      <c r="L10" s="80"/>
-      <c r="M10" s="104">
+      <c r="L10" s="106"/>
+      <c r="M10" s="107">
         <v>2300</v>
       </c>
-      <c r="N10" s="77"/>
-      <c r="O10" s="78" t="s">
+      <c r="N10" s="100"/>
+      <c r="O10" s="101" t="s">
         <v>8</v>
       </c>
-      <c r="P10" s="78"/>
+      <c r="P10" s="101"/>
       <c r="R10" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="S10" s="108">
+      <c r="S10" s="84">
         <v>3000</v>
       </c>
-      <c r="T10" s="108"/>
-      <c r="U10" s="112">
+      <c r="T10" s="84"/>
+      <c r="U10" s="92">
         <v>1300</v>
       </c>
-      <c r="V10" s="106"/>
-      <c r="W10" s="84" t="s">
+      <c r="V10" s="93"/>
+      <c r="W10" s="94" t="s">
         <v>8</v>
       </c>
-      <c r="X10" s="84"/>
+      <c r="X10" s="94"/>
       <c r="Z10" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="AA10" s="76"/>
-      <c r="AB10" s="76"/>
-      <c r="AC10" s="77"/>
-      <c r="AD10" s="77"/>
-      <c r="AE10" s="78"/>
-      <c r="AF10" s="78"/>
-    </row>
-    <row r="11" spans="2:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AA10" s="99"/>
+      <c r="AB10" s="99"/>
+      <c r="AC10" s="100"/>
+      <c r="AD10" s="100"/>
+      <c r="AE10" s="101"/>
+      <c r="AF10" s="101"/>
+    </row>
+    <row r="11" spans="2:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B11" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C11" s="107">
+      <c r="C11" s="102">
         <v>62300</v>
       </c>
-      <c r="D11" s="107"/>
-      <c r="E11" s="105">
+      <c r="D11" s="102"/>
+      <c r="E11" s="103">
         <v>17400</v>
       </c>
-      <c r="F11" s="81"/>
-      <c r="G11" s="82" t="s">
+      <c r="F11" s="104"/>
+      <c r="G11" s="105" t="s">
         <v>8</v>
       </c>
-      <c r="H11" s="82"/>
+      <c r="H11" s="105"/>
       <c r="J11" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="K11" s="80">
+      <c r="K11" s="106">
         <v>43100</v>
       </c>
-      <c r="L11" s="80"/>
-      <c r="M11" s="105">
+      <c r="L11" s="106"/>
+      <c r="M11" s="103">
         <v>9400</v>
       </c>
-      <c r="N11" s="81"/>
-      <c r="O11" s="82" t="s">
+      <c r="N11" s="104"/>
+      <c r="O11" s="105" t="s">
         <v>8</v>
       </c>
-      <c r="P11" s="82"/>
+      <c r="P11" s="105"/>
       <c r="R11" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="S11" s="107">
+      <c r="S11" s="102">
         <v>21000</v>
       </c>
-      <c r="T11" s="107"/>
-      <c r="U11" s="105">
+      <c r="T11" s="102"/>
+      <c r="U11" s="103">
         <v>8000</v>
       </c>
-      <c r="V11" s="81"/>
-      <c r="W11" s="82" t="s">
+      <c r="V11" s="104"/>
+      <c r="W11" s="105" t="s">
         <v>8</v>
       </c>
-      <c r="X11" s="82"/>
+      <c r="X11" s="105"/>
       <c r="Z11" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="AA11" s="76"/>
-      <c r="AB11" s="76"/>
-      <c r="AC11" s="77"/>
-      <c r="AD11" s="77"/>
-      <c r="AE11" s="78"/>
-      <c r="AF11" s="78"/>
-    </row>
-    <row r="12" spans="2:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="Y12" s="75"/>
-      <c r="Z12" s="75"/>
-      <c r="AA12" s="75"/>
-      <c r="AB12" s="75"/>
-      <c r="AC12" s="75"/>
-      <c r="AD12" s="75"/>
-    </row>
-    <row r="15" spans="2:32" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="AA11" s="99"/>
+      <c r="AB11" s="99"/>
+      <c r="AC11" s="100"/>
+      <c r="AD11" s="100"/>
+      <c r="AE11" s="101"/>
+      <c r="AF11" s="101"/>
+    </row>
+    <row r="12" spans="2:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="Y12" s="93"/>
+      <c r="Z12" s="93"/>
+      <c r="AA12" s="93"/>
+      <c r="AB12" s="93"/>
+      <c r="AC12" s="93"/>
+      <c r="AD12" s="93"/>
+    </row>
+    <row r="15" spans="2:32" ht="14.35" x14ac:dyDescent="0.5">
       <c r="I15" s="5"/>
     </row>
-    <row r="16" spans="2:32" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:32" ht="14.35" x14ac:dyDescent="0.5">
       <c r="I16" s="5"/>
     </row>
-    <row r="17" spans="9:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="17" spans="9:9" ht="14.35" x14ac:dyDescent="0.5">
       <c r="I17" s="5"/>
     </row>
-    <row r="18" spans="9:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="18" spans="9:9" ht="14.35" x14ac:dyDescent="0.5">
       <c r="I18" s="5"/>
     </row>
-    <row r="19" spans="9:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="19" spans="9:9" ht="14.35" x14ac:dyDescent="0.5">
       <c r="I19" s="5"/>
     </row>
-    <row r="20" spans="9:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="20" spans="9:9" ht="14.35" x14ac:dyDescent="0.5">
       <c r="I20" s="5"/>
     </row>
-    <row r="21" spans="9:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="21" spans="9:9" ht="14.35" x14ac:dyDescent="0.5">
       <c r="I21" s="5"/>
     </row>
-    <row r="22" spans="9:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="22" spans="9:9" ht="14.35" x14ac:dyDescent="0.5">
       <c r="I22" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="115">
-    <mergeCell ref="S4:T4"/>
-    <mergeCell ref="U4:V4"/>
-    <mergeCell ref="W4:X4"/>
-    <mergeCell ref="C2:H2"/>
-    <mergeCell ref="K2:P2"/>
-    <mergeCell ref="S2:X2"/>
-    <mergeCell ref="AA2:AF2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="M3:N3"/>
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="S3:T3"/>
-    <mergeCell ref="U3:V3"/>
-    <mergeCell ref="W3:X3"/>
-    <mergeCell ref="AA3:AB3"/>
-    <mergeCell ref="AC3:AD3"/>
-    <mergeCell ref="AE3:AF3"/>
+    <mergeCell ref="Y12:Z12"/>
+    <mergeCell ref="AA12:AB12"/>
+    <mergeCell ref="AC12:AD12"/>
+    <mergeCell ref="AA10:AB10"/>
+    <mergeCell ref="AC10:AD10"/>
+    <mergeCell ref="AE10:AF10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="M11:N11"/>
+    <mergeCell ref="O11:P11"/>
+    <mergeCell ref="S11:T11"/>
+    <mergeCell ref="U11:V11"/>
+    <mergeCell ref="W11:X11"/>
+    <mergeCell ref="AA11:AB11"/>
+    <mergeCell ref="AC11:AD11"/>
+    <mergeCell ref="AE11:AF11"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="S10:T10"/>
+    <mergeCell ref="U10:V10"/>
+    <mergeCell ref="W10:X10"/>
+    <mergeCell ref="AA8:AB8"/>
+    <mergeCell ref="AC8:AD8"/>
+    <mergeCell ref="AE8:AF8"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="O9:P9"/>
+    <mergeCell ref="S9:T9"/>
+    <mergeCell ref="U9:V9"/>
+    <mergeCell ref="W9:X9"/>
+    <mergeCell ref="AA9:AB9"/>
+    <mergeCell ref="AC9:AD9"/>
+    <mergeCell ref="AE9:AF9"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="O8:P8"/>
+    <mergeCell ref="S8:T8"/>
+    <mergeCell ref="U8:V8"/>
+    <mergeCell ref="W8:X8"/>
+    <mergeCell ref="AA6:AB6"/>
+    <mergeCell ref="AC6:AD6"/>
+    <mergeCell ref="AE6:AF6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="M7:N7"/>
+    <mergeCell ref="O7:P7"/>
+    <mergeCell ref="S7:T7"/>
+    <mergeCell ref="U7:V7"/>
+    <mergeCell ref="W7:X7"/>
+    <mergeCell ref="AA7:AB7"/>
+    <mergeCell ref="AC7:AD7"/>
+    <mergeCell ref="AE7:AF7"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="O6:P6"/>
     <mergeCell ref="S6:T6"/>
     <mergeCell ref="U6:V6"/>
     <mergeCell ref="W6:X6"/>
@@ -2033,78 +2080,25 @@
     <mergeCell ref="K4:L4"/>
     <mergeCell ref="M4:N4"/>
     <mergeCell ref="O4:P4"/>
-    <mergeCell ref="S8:T8"/>
-    <mergeCell ref="U8:V8"/>
-    <mergeCell ref="W8:X8"/>
-    <mergeCell ref="AA6:AB6"/>
-    <mergeCell ref="AC6:AD6"/>
-    <mergeCell ref="AE6:AF6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="M7:N7"/>
-    <mergeCell ref="O7:P7"/>
-    <mergeCell ref="S7:T7"/>
-    <mergeCell ref="U7:V7"/>
-    <mergeCell ref="W7:X7"/>
-    <mergeCell ref="AA7:AB7"/>
-    <mergeCell ref="AC7:AD7"/>
-    <mergeCell ref="AE7:AF7"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="S10:T10"/>
-    <mergeCell ref="U10:V10"/>
-    <mergeCell ref="W10:X10"/>
-    <mergeCell ref="AA8:AB8"/>
-    <mergeCell ref="AC8:AD8"/>
-    <mergeCell ref="AE8:AF8"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="M9:N9"/>
-    <mergeCell ref="O9:P9"/>
-    <mergeCell ref="S9:T9"/>
-    <mergeCell ref="U9:V9"/>
-    <mergeCell ref="W9:X9"/>
-    <mergeCell ref="AA9:AB9"/>
-    <mergeCell ref="AC9:AD9"/>
-    <mergeCell ref="AE9:AF9"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="O8:P8"/>
-    <mergeCell ref="Y12:Z12"/>
-    <mergeCell ref="AA12:AB12"/>
-    <mergeCell ref="AC12:AD12"/>
-    <mergeCell ref="AA10:AB10"/>
-    <mergeCell ref="AC10:AD10"/>
-    <mergeCell ref="AE10:AF10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="M11:N11"/>
-    <mergeCell ref="O11:P11"/>
-    <mergeCell ref="S11:T11"/>
-    <mergeCell ref="U11:V11"/>
-    <mergeCell ref="W11:X11"/>
-    <mergeCell ref="AA11:AB11"/>
-    <mergeCell ref="AC11:AD11"/>
-    <mergeCell ref="AE11:AF11"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="M10:N10"/>
-    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="S4:T4"/>
+    <mergeCell ref="U4:V4"/>
+    <mergeCell ref="W4:X4"/>
+    <mergeCell ref="C2:H2"/>
+    <mergeCell ref="K2:P2"/>
+    <mergeCell ref="S2:X2"/>
+    <mergeCell ref="AA2:AF2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="S3:T3"/>
+    <mergeCell ref="U3:V3"/>
+    <mergeCell ref="W3:X3"/>
+    <mergeCell ref="AA3:AB3"/>
+    <mergeCell ref="AC3:AD3"/>
+    <mergeCell ref="AE3:AF3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -2115,21 +2109,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:CRB111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="AU101" sqref="AU101"/>
+    <sheetView tabSelected="1" topLeftCell="C13" zoomScale="39" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="M34" sqref="M34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.64453125" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.65"/>
   <cols>
-    <col min="1" max="1" width="45.44140625" style="7" customWidth="1"/>
-    <col min="2" max="3" width="17.6640625" style="7" customWidth="1"/>
-    <col min="4" max="4" width="17.6640625" style="8" customWidth="1"/>
-    <col min="5" max="6" width="8.6640625" style="7"/>
-    <col min="7" max="7" width="12.6640625" style="7" customWidth="1"/>
-    <col min="8" max="16384" width="8.6640625" style="7"/>
+    <col min="1" max="1" width="45.41015625" style="7" customWidth="1"/>
+    <col min="2" max="3" width="17.64453125" style="7" customWidth="1"/>
+    <col min="4" max="4" width="17.64453125" style="8" customWidth="1"/>
+    <col min="5" max="6" width="8.64453125" style="7"/>
+    <col min="7" max="7" width="12.64453125" style="7" customWidth="1"/>
+    <col min="8" max="16384" width="8.64453125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:64" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:64" s="9" customFormat="1" ht="18.350000000000001" x14ac:dyDescent="0.65">
       <c r="B1" s="9" t="s">
         <v>15</v>
       </c>
@@ -2152,11 +2146,11 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:64" s="14" customFormat="1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A2" s="93" t="s">
+    <row r="2" spans="1:64" s="14" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
+      <c r="A2" s="108" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="93"/>
+      <c r="B2" s="108"/>
       <c r="D2" s="15"/>
       <c r="E2" s="14">
         <v>1</v>
@@ -2339,7 +2333,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:64" ht="18.350000000000001" x14ac:dyDescent="0.65">
       <c r="A3" s="16" t="s">
         <v>23</v>
       </c>
@@ -2355,7 +2349,7 @@
       <c r="G3" s="20"/>
       <c r="H3" s="20"/>
     </row>
-    <row r="4" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:64" ht="18.350000000000001" x14ac:dyDescent="0.65">
       <c r="A4" s="16" t="s">
         <v>25</v>
       </c>
@@ -2369,7 +2363,7 @@
       <c r="G4" s="19"/>
       <c r="H4" s="19"/>
     </row>
-    <row r="5" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:64" ht="18.350000000000001" x14ac:dyDescent="0.65">
       <c r="A5" s="16" t="s">
         <v>26</v>
       </c>
@@ -2385,7 +2379,7 @@
       <c r="I5" s="22"/>
       <c r="J5" s="22"/>
     </row>
-    <row r="6" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:64" ht="18.350000000000001" x14ac:dyDescent="0.65">
       <c r="A6" s="16" t="s">
         <v>27</v>
       </c>
@@ -2398,7 +2392,7 @@
       <c r="D6" s="18"/>
       <c r="I6" s="19"/>
     </row>
-    <row r="7" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:64" ht="18.350000000000001" x14ac:dyDescent="0.65">
       <c r="A7" s="16" t="s">
         <v>29</v>
       </c>
@@ -2412,7 +2406,7 @@
       <c r="I7" s="19"/>
       <c r="J7" s="19"/>
     </row>
-    <row r="8" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:64" ht="18.350000000000001" x14ac:dyDescent="0.65">
       <c r="A8" s="16" t="s">
         <v>30</v>
       </c>
@@ -2426,7 +2420,7 @@
       <c r="K8" s="19"/>
       <c r="L8" s="19"/>
     </row>
-    <row r="9" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:64" ht="18.350000000000001" x14ac:dyDescent="0.65">
       <c r="A9" s="16" t="s">
         <v>32</v>
       </c>
@@ -2440,7 +2434,7 @@
       <c r="M9" s="19"/>
       <c r="N9" s="19"/>
     </row>
-    <row r="10" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:64" ht="18.350000000000001" x14ac:dyDescent="0.65">
       <c r="A10" s="16" t="s">
         <v>34</v>
       </c>
@@ -2454,7 +2448,7 @@
       <c r="J10" s="19"/>
       <c r="K10" s="19"/>
     </row>
-    <row r="11" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:64" ht="18.350000000000001" x14ac:dyDescent="0.65">
       <c r="A11" s="16" t="s">
         <v>35</v>
       </c>
@@ -2470,7 +2464,7 @@
       <c r="M11" s="22"/>
       <c r="N11" s="22"/>
     </row>
-    <row r="12" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:64" ht="18.350000000000001" x14ac:dyDescent="0.65">
       <c r="A12" s="16" t="s">
         <v>36</v>
       </c>
@@ -2488,7 +2482,7 @@
       <c r="Q12" s="24"/>
       <c r="R12" s="24"/>
     </row>
-    <row r="13" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:64" ht="18.350000000000001" x14ac:dyDescent="0.65">
       <c r="A13" s="16" t="s">
         <v>37</v>
       </c>
@@ -2503,7 +2497,7 @@
       <c r="T13" s="22"/>
       <c r="U13" s="22"/>
     </row>
-    <row r="14" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:64" ht="18.350000000000001" x14ac:dyDescent="0.65">
       <c r="A14" s="16" t="s">
         <v>39</v>
       </c>
@@ -2517,7 +2511,7 @@
       <c r="L14" s="22"/>
       <c r="M14" s="22"/>
     </row>
-    <row r="15" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:64" ht="18.350000000000001" x14ac:dyDescent="0.65">
       <c r="A15" s="16" t="s">
         <v>40</v>
       </c>
@@ -2531,7 +2525,7 @@
       <c r="O15" s="19"/>
       <c r="P15" s="22"/>
     </row>
-    <row r="16" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:64" ht="18.350000000000001" x14ac:dyDescent="0.65">
       <c r="A16" s="16" t="s">
         <v>42</v>
       </c>
@@ -2545,7 +2539,7 @@
       <c r="N16" s="24"/>
       <c r="O16" s="24"/>
     </row>
-    <row r="17" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:38" ht="18.350000000000001" x14ac:dyDescent="0.65">
       <c r="A17" s="16" t="s">
         <v>43</v>
       </c>
@@ -2560,7 +2554,7 @@
       <c r="W17" s="24"/>
       <c r="X17" s="24"/>
     </row>
-    <row r="18" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:38" ht="18.350000000000001" x14ac:dyDescent="0.65">
       <c r="A18" s="16" t="s">
         <v>45</v>
       </c>
@@ -2577,7 +2571,7 @@
       <c r="Y18" s="24"/>
       <c r="Z18" s="24"/>
     </row>
-    <row r="19" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:38" ht="18.350000000000001" x14ac:dyDescent="0.65">
       <c r="A19" s="16" t="s">
         <v>46</v>
       </c>
@@ -2593,7 +2587,7 @@
       <c r="AC19" s="24"/>
       <c r="AD19" s="24"/>
     </row>
-    <row r="20" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:38" ht="18.350000000000001" x14ac:dyDescent="0.65">
       <c r="A20" s="16" t="s">
         <v>48</v>
       </c>
@@ -2608,7 +2602,7 @@
       <c r="AF20" s="24"/>
       <c r="AG20" s="24"/>
     </row>
-    <row r="21" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:38" ht="18.350000000000001" x14ac:dyDescent="0.65">
       <c r="A21" s="16" t="s">
         <v>49</v>
       </c>
@@ -2622,14 +2616,14 @@
       <c r="AH21" s="24"/>
       <c r="AI21" s="24"/>
     </row>
-    <row r="22" spans="1:38" s="27" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:38" s="27" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
       <c r="A22" s="25" t="s">
         <v>50</v>
       </c>
       <c r="B22" s="26"/>
       <c r="D22" s="28"/>
     </row>
-    <row r="23" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:38" ht="18.350000000000001" x14ac:dyDescent="0.65">
       <c r="A23" s="16" t="s">
         <v>51</v>
       </c>
@@ -2643,7 +2637,7 @@
       <c r="E23" s="19"/>
       <c r="F23" s="19"/>
     </row>
-    <row r="24" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:38" ht="18.350000000000001" x14ac:dyDescent="0.65">
       <c r="A24" s="16" t="s">
         <v>52</v>
       </c>
@@ -2658,7 +2652,7 @@
       <c r="H24" s="19"/>
       <c r="I24" s="19"/>
     </row>
-    <row r="25" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:38" ht="18.350000000000001" x14ac:dyDescent="0.65">
       <c r="A25" s="16" t="s">
         <v>53</v>
       </c>
@@ -2674,7 +2668,7 @@
       <c r="L25" s="19"/>
       <c r="M25" s="19"/>
     </row>
-    <row r="26" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:38" ht="18.350000000000001" x14ac:dyDescent="0.65">
       <c r="A26" s="16" t="s">
         <v>54</v>
       </c>
@@ -2692,7 +2686,7 @@
       <c r="R26" s="19"/>
       <c r="S26" s="19"/>
     </row>
-    <row r="27" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:38" ht="18.350000000000001" x14ac:dyDescent="0.65">
       <c r="A27" s="16" t="s">
         <v>55</v>
       </c>
@@ -2707,7 +2701,7 @@
       <c r="U27" s="19"/>
       <c r="V27" s="19"/>
     </row>
-    <row r="28" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:38" ht="18.350000000000001" x14ac:dyDescent="0.65">
       <c r="A28" s="16" t="s">
         <v>57</v>
       </c>
@@ -2720,7 +2714,7 @@
       <c r="D28" s="18"/>
       <c r="W28" s="19"/>
     </row>
-    <row r="29" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:38" ht="18.350000000000001" x14ac:dyDescent="0.65">
       <c r="A29" s="16" t="s">
         <v>58</v>
       </c>
@@ -2737,7 +2731,7 @@
       <c r="Z29" s="22"/>
       <c r="AA29" s="22"/>
     </row>
-    <row r="30" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:38" ht="18.350000000000001" x14ac:dyDescent="0.65">
       <c r="A30" s="16" t="s">
         <v>59</v>
       </c>
@@ -2752,7 +2746,7 @@
       <c r="AC30" s="24"/>
       <c r="AD30" s="24"/>
     </row>
-    <row r="31" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:38" ht="18.350000000000001" x14ac:dyDescent="0.65">
       <c r="A31" s="16" t="s">
         <v>60</v>
       </c>
@@ -2763,14 +2757,14 @@
         <v>8</v>
       </c>
       <c r="D31" s="21"/>
-      <c r="AE31" s="24"/>
-      <c r="AF31" s="24"/>
-      <c r="AG31" s="24"/>
-      <c r="AH31" s="24"/>
-      <c r="AI31" s="24"/>
-      <c r="AJ31" s="24"/>
-    </row>
-    <row r="32" spans="1:38" x14ac:dyDescent="0.35">
+      <c r="AE31" s="113"/>
+      <c r="AF31" s="113"/>
+      <c r="AG31" s="113"/>
+      <c r="AH31" s="113"/>
+      <c r="AI31" s="113"/>
+      <c r="AJ31" s="113"/>
+    </row>
+    <row r="32" spans="1:38" ht="18.350000000000001" x14ac:dyDescent="0.65">
       <c r="A32" s="16" t="s">
         <v>61</v>
       </c>
@@ -2781,10 +2775,10 @@
         <v>9</v>
       </c>
       <c r="D32" s="21"/>
-      <c r="AK32" s="24"/>
-      <c r="AL32" s="24"/>
-    </row>
-    <row r="33" spans="1:61" x14ac:dyDescent="0.35">
+      <c r="AK32" s="113"/>
+      <c r="AL32" s="113"/>
+    </row>
+    <row r="33" spans="1:61" ht="18.350000000000001" x14ac:dyDescent="0.65">
       <c r="A33" s="16" t="s">
         <v>62</v>
       </c>
@@ -2795,11 +2789,11 @@
         <v>63</v>
       </c>
       <c r="D33" s="21"/>
-      <c r="AB33" s="24"/>
-      <c r="AC33" s="24"/>
-      <c r="AD33" s="24"/>
-    </row>
-    <row r="34" spans="1:61" x14ac:dyDescent="0.35">
+      <c r="AB33" s="113"/>
+      <c r="AC33" s="113"/>
+      <c r="AD33" s="113"/>
+    </row>
+    <row r="34" spans="1:61" ht="18.350000000000001" x14ac:dyDescent="0.65">
       <c r="A34" s="16" t="s">
         <v>64</v>
       </c>
@@ -2810,12 +2804,12 @@
         <v>11</v>
       </c>
       <c r="D34" s="21"/>
-      <c r="AE34" s="24"/>
-      <c r="AF34" s="24"/>
-      <c r="AG34" s="24"/>
-      <c r="AH34" s="24"/>
-    </row>
-    <row r="35" spans="1:61" x14ac:dyDescent="0.35">
+      <c r="AE34" s="113"/>
+      <c r="AF34" s="113"/>
+      <c r="AG34" s="113"/>
+      <c r="AH34" s="113"/>
+    </row>
+    <row r="35" spans="1:61" ht="18.350000000000001" x14ac:dyDescent="0.65">
       <c r="A35" s="16" t="s">
         <v>65</v>
       </c>
@@ -2825,16 +2819,16 @@
       <c r="C35" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="D35" s="23"/>
-      <c r="AM35" s="24"/>
-      <c r="AN35" s="24"/>
-      <c r="AO35" s="24"/>
-      <c r="AP35" s="24"/>
-      <c r="AQ35" s="24"/>
-      <c r="AR35" s="24"/>
-      <c r="AS35" s="24"/>
-    </row>
-    <row r="36" spans="1:61" x14ac:dyDescent="0.35">
+      <c r="D35" s="112"/>
+      <c r="AM35" s="113"/>
+      <c r="AN35" s="113"/>
+      <c r="AO35" s="113"/>
+      <c r="AP35" s="113"/>
+      <c r="AQ35" s="113"/>
+      <c r="AR35" s="113"/>
+      <c r="AS35" s="113"/>
+    </row>
+    <row r="36" spans="1:61" ht="18.350000000000001" x14ac:dyDescent="0.65">
       <c r="A36" s="16" t="s">
         <v>67</v>
       </c>
@@ -2848,7 +2842,7 @@
       <c r="AT36" s="24"/>
       <c r="AU36" s="24"/>
     </row>
-    <row r="37" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:61" ht="18.350000000000001" x14ac:dyDescent="0.65">
       <c r="A37" s="16" t="s">
         <v>68</v>
       </c>
@@ -2867,7 +2861,7 @@
       <c r="AJ37" s="24"/>
       <c r="AK37" s="24"/>
     </row>
-    <row r="38" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:61" ht="18.350000000000001" x14ac:dyDescent="0.65">
       <c r="A38" s="16" t="s">
         <v>69</v>
       </c>
@@ -2887,7 +2881,7 @@
       <c r="BB38" s="24"/>
       <c r="BC38" s="24"/>
     </row>
-    <row r="39" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:61" ht="18.350000000000001" x14ac:dyDescent="0.65">
       <c r="A39" s="16" t="s">
         <v>70</v>
       </c>
@@ -2905,14 +2899,14 @@
       <c r="BH39" s="24"/>
       <c r="BI39" s="24"/>
     </row>
-    <row r="40" spans="1:61" s="27" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:61" s="27" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A40" s="25" t="s">
         <v>71</v>
       </c>
       <c r="B40" s="26"/>
       <c r="D40" s="28"/>
     </row>
-    <row r="41" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:61" ht="18.350000000000001" x14ac:dyDescent="0.65">
       <c r="A41" s="16" t="s">
         <v>72</v>
       </c>
@@ -2926,7 +2920,7 @@
       <c r="E41" s="19"/>
       <c r="F41" s="19"/>
     </row>
-    <row r="42" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:61" ht="18.350000000000001" x14ac:dyDescent="0.65">
       <c r="A42" s="16" t="s">
         <v>73</v>
       </c>
@@ -2940,7 +2934,7 @@
       <c r="G42" s="19"/>
       <c r="H42" s="19"/>
     </row>
-    <row r="43" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:61" ht="18.350000000000001" x14ac:dyDescent="0.65">
       <c r="A43" s="16" t="s">
         <v>74</v>
       </c>
@@ -2953,7 +2947,7 @@
       <c r="D43" s="30"/>
       <c r="I43" s="22"/>
     </row>
-    <row r="44" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:61" ht="18.350000000000001" x14ac:dyDescent="0.65">
       <c r="A44" s="16" t="s">
         <v>75</v>
       </c>
@@ -2969,7 +2963,7 @@
       <c r="K44" s="22"/>
       <c r="L44" s="22"/>
     </row>
-    <row r="45" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:61" ht="18.350000000000001" x14ac:dyDescent="0.65">
       <c r="A45" s="16" t="s">
         <v>76</v>
       </c>
@@ -2985,7 +2979,7 @@
       <c r="O45" s="22"/>
       <c r="P45" s="22"/>
     </row>
-    <row r="46" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:61" ht="18.350000000000001" x14ac:dyDescent="0.65">
       <c r="A46" s="16" t="s">
         <v>78</v>
       </c>
@@ -2999,7 +2993,7 @@
       <c r="Q46" s="24"/>
       <c r="R46" s="24"/>
     </row>
-    <row r="47" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:61" ht="18.350000000000001" x14ac:dyDescent="0.65">
       <c r="A47" s="16" t="s">
         <v>80</v>
       </c>
@@ -3015,7 +3009,7 @@
       <c r="S47" s="24"/>
       <c r="T47" s="24"/>
     </row>
-    <row r="48" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:61" ht="18.350000000000001" x14ac:dyDescent="0.65">
       <c r="A48" s="16" t="s">
         <v>81</v>
       </c>
@@ -3029,7 +3023,7 @@
       <c r="U48" s="24"/>
       <c r="V48" s="24"/>
     </row>
-    <row r="49" spans="1:49" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:49" ht="18.350000000000001" x14ac:dyDescent="0.65">
       <c r="A49" s="16" t="s">
         <v>82</v>
       </c>
@@ -3043,7 +3037,7 @@
       <c r="W49" s="24"/>
       <c r="X49" s="24"/>
     </row>
-    <row r="50" spans="1:49" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:49" ht="18.350000000000001" x14ac:dyDescent="0.65">
       <c r="A50" s="16" t="s">
         <v>83</v>
       </c>
@@ -3056,7 +3050,7 @@
       <c r="D50" s="31"/>
       <c r="Y50" s="24"/>
     </row>
-    <row r="51" spans="1:49" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:49" ht="18.350000000000001" x14ac:dyDescent="0.65">
       <c r="A51" s="16" t="s">
         <v>84</v>
       </c>
@@ -3072,7 +3066,7 @@
       <c r="AA51" s="24"/>
       <c r="AB51" s="24"/>
     </row>
-    <row r="52" spans="1:49" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:49" ht="18.350000000000001" x14ac:dyDescent="0.65">
       <c r="A52" s="16" t="s">
         <v>85</v>
       </c>
@@ -3088,7 +3082,7 @@
       <c r="AE52" s="24"/>
       <c r="AF52" s="24"/>
     </row>
-    <row r="53" spans="1:49" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:49" ht="18.350000000000001" x14ac:dyDescent="0.65">
       <c r="A53" s="16" t="s">
         <v>87</v>
       </c>
@@ -3102,7 +3096,7 @@
       <c r="AG53" s="24"/>
       <c r="AH53" s="24"/>
     </row>
-    <row r="54" spans="1:49" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:49" ht="18.350000000000001" x14ac:dyDescent="0.65">
       <c r="A54" s="16" t="s">
         <v>89</v>
       </c>
@@ -3118,7 +3112,7 @@
       <c r="AI54" s="24"/>
       <c r="AJ54" s="24"/>
     </row>
-    <row r="55" spans="1:49" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:49" ht="18.350000000000001" x14ac:dyDescent="0.65">
       <c r="A55" s="16" t="s">
         <v>90</v>
       </c>
@@ -3132,7 +3126,7 @@
       <c r="AK55" s="24"/>
       <c r="AL55" s="24"/>
     </row>
-    <row r="56" spans="1:49" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:49" ht="18.350000000000001" x14ac:dyDescent="0.65">
       <c r="A56" s="16" t="s">
         <v>91</v>
       </c>
@@ -3146,7 +3140,7 @@
       <c r="AM56" s="24"/>
       <c r="AN56" s="24"/>
     </row>
-    <row r="57" spans="1:49" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:49" ht="18.350000000000001" x14ac:dyDescent="0.65">
       <c r="A57" s="16" t="s">
         <v>92</v>
       </c>
@@ -3159,7 +3153,7 @@
       <c r="D57" s="31"/>
       <c r="AO57" s="24"/>
     </row>
-    <row r="58" spans="1:49" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:49" ht="18.350000000000001" x14ac:dyDescent="0.65">
       <c r="A58" s="16" t="s">
         <v>93</v>
       </c>
@@ -3175,7 +3169,7 @@
       <c r="AR58" s="24"/>
       <c r="AS58" s="24"/>
     </row>
-    <row r="59" spans="1:49" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:49" ht="18.350000000000001" x14ac:dyDescent="0.65">
       <c r="A59" s="16" t="s">
         <v>95</v>
       </c>
@@ -3189,7 +3183,7 @@
       <c r="AT59" s="24"/>
       <c r="AU59" s="24"/>
     </row>
-    <row r="60" spans="1:49" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:49" ht="18.350000000000001" x14ac:dyDescent="0.65">
       <c r="A60" s="16" t="s">
         <v>97</v>
       </c>
@@ -3205,14 +3199,14 @@
       <c r="AV60" s="24"/>
       <c r="AW60" s="24"/>
     </row>
-    <row r="61" spans="1:49" s="27" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:49" s="27" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
       <c r="A61" s="25" t="s">
         <v>98</v>
       </c>
       <c r="B61" s="26"/>
       <c r="D61" s="28"/>
     </row>
-    <row r="62" spans="1:49" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:49" ht="18.350000000000001" x14ac:dyDescent="0.65">
       <c r="A62" s="7" t="s">
         <v>99</v>
       </c>
@@ -3228,7 +3222,7 @@
       <c r="G62" s="32"/>
       <c r="H62" s="32"/>
     </row>
-    <row r="63" spans="1:49" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:49" ht="18.350000000000001" x14ac:dyDescent="0.65">
       <c r="A63" s="7" t="s">
         <v>100</v>
       </c>
@@ -3246,7 +3240,7 @@
       <c r="M63" s="33"/>
       <c r="N63" s="33"/>
     </row>
-    <row r="64" spans="1:49" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:49" ht="18.350000000000001" x14ac:dyDescent="0.65">
       <c r="A64" s="7" t="s">
         <v>101</v>
       </c>
@@ -3266,7 +3260,7 @@
       <c r="O64" s="33"/>
       <c r="P64" s="33"/>
     </row>
-    <row r="65" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:42" ht="18.350000000000001" x14ac:dyDescent="0.65">
       <c r="A65" s="7" t="s">
         <v>102</v>
       </c>
@@ -3286,7 +3280,7 @@
       <c r="W65" s="34"/>
       <c r="X65" s="34"/>
     </row>
-    <row r="66" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:42" ht="18.350000000000001" x14ac:dyDescent="0.65">
       <c r="A66" s="7" t="s">
         <v>103</v>
       </c>
@@ -3302,7 +3296,7 @@
       <c r="S66" s="34"/>
       <c r="T66" s="34"/>
     </row>
-    <row r="67" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:42" ht="18.350000000000001" x14ac:dyDescent="0.65">
       <c r="A67" s="7" t="s">
         <v>105</v>
       </c>
@@ -3322,7 +3316,7 @@
       <c r="W67" s="34"/>
       <c r="X67" s="34"/>
     </row>
-    <row r="68" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:42" ht="18.350000000000001" x14ac:dyDescent="0.65">
       <c r="A68" s="7" t="s">
         <v>106</v>
       </c>
@@ -3338,7 +3332,7 @@
       <c r="AA68" s="34"/>
       <c r="AB68" s="34"/>
     </row>
-    <row r="69" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:42" ht="18.350000000000001" x14ac:dyDescent="0.65">
       <c r="A69" s="7" t="s">
         <v>108</v>
       </c>
@@ -3354,7 +3348,7 @@
       <c r="AA69" s="34"/>
       <c r="AB69" s="34"/>
     </row>
-    <row r="70" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:42" ht="18.350000000000001" x14ac:dyDescent="0.65">
       <c r="A70" s="7" t="s">
         <v>109</v>
       </c>
@@ -3369,7 +3363,7 @@
       <c r="AD70" s="34"/>
       <c r="AE70" s="34"/>
     </row>
-    <row r="71" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:42" ht="18.350000000000001" x14ac:dyDescent="0.65">
       <c r="A71" s="7" t="s">
         <v>110</v>
       </c>
@@ -3384,7 +3378,7 @@
       <c r="AG71" s="34"/>
       <c r="AH71" s="34"/>
     </row>
-    <row r="72" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:42" ht="18.350000000000001" x14ac:dyDescent="0.65">
       <c r="A72" s="7" t="s">
         <v>112</v>
       </c>
@@ -3400,7 +3394,7 @@
       <c r="AK72" s="34"/>
       <c r="AL72" s="34"/>
     </row>
-    <row r="73" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:42" ht="18.350000000000001" x14ac:dyDescent="0.65">
       <c r="A73" s="7" t="s">
         <v>113</v>
       </c>
@@ -3416,14 +3410,14 @@
       <c r="AO73" s="34"/>
       <c r="AP73" s="34"/>
     </row>
-    <row r="74" spans="1:42" s="27" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+    <row r="74" spans="1:42" s="27" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
       <c r="A74" s="25" t="s">
         <v>114</v>
       </c>
       <c r="B74" s="35"/>
       <c r="D74" s="28"/>
     </row>
-    <row r="75" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:42" ht="18.350000000000001" x14ac:dyDescent="0.65">
       <c r="A75" s="16" t="s">
         <v>115</v>
       </c>
@@ -3442,7 +3436,7 @@
       <c r="J75" s="22"/>
       <c r="K75" s="22"/>
     </row>
-    <row r="76" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:42" ht="18.350000000000001" x14ac:dyDescent="0.65">
       <c r="A76" s="16" t="s">
         <v>116</v>
       </c>
@@ -3461,7 +3455,7 @@
       <c r="Q76" s="22"/>
       <c r="R76" s="22"/>
     </row>
-    <row r="77" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:42" ht="18.350000000000001" x14ac:dyDescent="0.65">
       <c r="A77" s="16" t="s">
         <v>117</v>
       </c>
@@ -3481,7 +3475,7 @@
       <c r="R77" s="22"/>
       <c r="S77" s="24"/>
     </row>
-    <row r="78" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:42" ht="18.350000000000001" x14ac:dyDescent="0.65">
       <c r="A78" s="16" t="s">
         <v>118</v>
       </c>
@@ -3497,7 +3491,7 @@
       <c r="U78" s="24"/>
       <c r="V78" s="24"/>
     </row>
-    <row r="79" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:42" ht="18.350000000000001" x14ac:dyDescent="0.65">
       <c r="A79" s="16" t="s">
         <v>120</v>
       </c>
@@ -3515,7 +3509,7 @@
       <c r="AA79" s="24"/>
       <c r="AB79" s="24"/>
     </row>
-    <row r="80" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:42" ht="18.350000000000001" x14ac:dyDescent="0.65">
       <c r="A80" s="16" t="s">
         <v>121</v>
       </c>
@@ -3533,7 +3527,7 @@
       <c r="AA80" s="24"/>
       <c r="AB80" s="24"/>
     </row>
-    <row r="81" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:44" ht="18.350000000000001" x14ac:dyDescent="0.65">
       <c r="A81" s="16" t="s">
         <v>122</v>
       </c>
@@ -3550,7 +3544,7 @@
       <c r="AF81" s="24"/>
       <c r="AG81" s="24"/>
     </row>
-    <row r="82" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:44" ht="18.350000000000001" x14ac:dyDescent="0.65">
       <c r="A82" s="16" t="s">
         <v>124</v>
       </c>
@@ -3568,7 +3562,7 @@
       <c r="AL82" s="24"/>
       <c r="AM82" s="24"/>
     </row>
-    <row r="83" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:44" ht="18.350000000000001" x14ac:dyDescent="0.65">
       <c r="A83" s="16" t="s">
         <v>125</v>
       </c>
@@ -3584,7 +3578,7 @@
       <c r="AN83" s="24"/>
       <c r="AO83" s="24"/>
     </row>
-    <row r="84" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:44" ht="18.350000000000001" x14ac:dyDescent="0.65">
       <c r="A84" s="16" t="s">
         <v>126</v>
       </c>
@@ -3595,51 +3589,45 @@
         <v>24</v>
       </c>
       <c r="D84" s="31"/>
-      <c r="E84" s="98"/>
-      <c r="F84" s="98"/>
-      <c r="G84" s="98"/>
-      <c r="H84" s="97"/>
-      <c r="I84" s="97"/>
-      <c r="J84" s="97"/>
-      <c r="K84" s="97"/>
-      <c r="L84" s="97"/>
-      <c r="M84" s="97"/>
-      <c r="N84" s="97"/>
-      <c r="O84" s="97"/>
-      <c r="P84" s="97"/>
-      <c r="Q84" s="97"/>
-      <c r="R84" s="97"/>
-      <c r="S84" s="101"/>
-      <c r="T84" s="101"/>
-      <c r="U84" s="101"/>
-      <c r="V84" s="101"/>
-      <c r="W84" s="101"/>
-      <c r="X84" s="101"/>
-      <c r="Y84" s="101"/>
-      <c r="Z84" s="101"/>
-      <c r="AA84" s="101"/>
-      <c r="AB84" s="101"/>
-      <c r="AC84" s="101"/>
-      <c r="AD84" s="101"/>
-      <c r="AE84" s="101"/>
-      <c r="AF84" s="101"/>
-      <c r="AG84" s="101"/>
-      <c r="AH84" s="101"/>
-      <c r="AI84" s="101"/>
-      <c r="AJ84" s="101"/>
-      <c r="AK84" s="101"/>
-      <c r="AL84" s="101"/>
-      <c r="AM84" s="101"/>
-      <c r="AN84" s="101"/>
-      <c r="AO84" s="101"/>
-      <c r="AP84" s="99"/>
-      <c r="AQ84" s="99"/>
-      <c r="AR84" s="99"/>
-      <c r="AS84" s="99"/>
-      <c r="AT84" s="99"/>
-      <c r="AU84" s="99"/>
-    </row>
-    <row r="85" spans="1:50" x14ac:dyDescent="0.35">
+      <c r="E84" s="76"/>
+      <c r="F84" s="76"/>
+      <c r="G84" s="76"/>
+      <c r="H84" s="75"/>
+      <c r="I84" s="75"/>
+      <c r="J84" s="75"/>
+      <c r="K84" s="75"/>
+      <c r="L84" s="75"/>
+      <c r="M84" s="75"/>
+      <c r="N84" s="75"/>
+      <c r="O84" s="75"/>
+      <c r="P84" s="75"/>
+      <c r="Q84" s="75"/>
+      <c r="R84" s="75"/>
+      <c r="S84" s="78"/>
+      <c r="T84" s="78"/>
+      <c r="U84" s="78"/>
+      <c r="V84" s="78"/>
+      <c r="W84" s="78"/>
+      <c r="X84" s="78"/>
+      <c r="Y84" s="78"/>
+      <c r="Z84" s="78"/>
+      <c r="AA84" s="78"/>
+      <c r="AB84" s="78"/>
+      <c r="AC84" s="78"/>
+      <c r="AD84" s="78"/>
+      <c r="AE84" s="78"/>
+      <c r="AF84" s="78"/>
+      <c r="AG84" s="78"/>
+      <c r="AH84" s="78"/>
+      <c r="AI84" s="78"/>
+      <c r="AJ84" s="78"/>
+      <c r="AK84" s="78"/>
+      <c r="AL84" s="78"/>
+      <c r="AM84" s="78"/>
+      <c r="AN84" s="78"/>
+      <c r="AO84" s="78"/>
+    </row>
+    <row r="85" spans="1:44" ht="18.350000000000001" x14ac:dyDescent="0.65">
       <c r="A85" s="16" t="s">
         <v>127</v>
       </c>
@@ -3650,32 +3638,18 @@
         <v>179</v>
       </c>
       <c r="D85" s="31"/>
-      <c r="H85" s="99"/>
-      <c r="I85" s="99"/>
-      <c r="J85" s="99"/>
-      <c r="K85" s="99"/>
-      <c r="L85" s="99"/>
-      <c r="M85" s="99"/>
-      <c r="N85" s="99"/>
-      <c r="O85" s="99"/>
-      <c r="P85" s="99"/>
-      <c r="Q85" s="99"/>
-      <c r="R85" s="99"/>
-      <c r="AP85" s="100"/>
-      <c r="AQ85" s="100"/>
-      <c r="AR85" s="100"/>
-      <c r="AV85" s="99"/>
-      <c r="AW85" s="99"/>
-      <c r="AX85" s="99"/>
-    </row>
-    <row r="86" spans="1:50" s="27" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+      <c r="AP85" s="77"/>
+      <c r="AQ85" s="77"/>
+      <c r="AR85" s="77"/>
+    </row>
+    <row r="86" spans="1:44" s="27" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
       <c r="A86" s="25" t="s">
         <v>128</v>
       </c>
       <c r="B86" s="26"/>
       <c r="D86" s="28"/>
     </row>
-    <row r="87" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:44" ht="18.350000000000001" x14ac:dyDescent="0.65">
       <c r="A87" s="16" t="s">
         <v>129</v>
       </c>
@@ -3710,7 +3684,7 @@
       <c r="Z87" s="38"/>
       <c r="AA87" s="38"/>
     </row>
-    <row r="88" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:44" ht="18.350000000000001" x14ac:dyDescent="0.65">
       <c r="A88" s="16" t="s">
         <v>130</v>
       </c>
@@ -3745,7 +3719,7 @@
       <c r="Z88" s="38"/>
       <c r="AA88" s="38"/>
     </row>
-    <row r="89" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:44" ht="18.350000000000001" x14ac:dyDescent="0.65">
       <c r="A89" s="16" t="s">
         <v>131</v>
       </c>
@@ -3780,7 +3754,7 @@
       <c r="Z89" s="38"/>
       <c r="AA89" s="38"/>
     </row>
-    <row r="90" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:44" ht="18.350000000000001" x14ac:dyDescent="0.65">
       <c r="A90" s="16" t="s">
         <v>132</v>
       </c>
@@ -3815,7 +3789,7 @@
       <c r="Z90" s="38"/>
       <c r="AA90" s="38"/>
     </row>
-    <row r="91" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:44" ht="18.350000000000001" x14ac:dyDescent="0.65">
       <c r="A91" s="16" t="s">
         <v>133</v>
       </c>
@@ -3850,7 +3824,7 @@
       <c r="Z91" s="38"/>
       <c r="AA91" s="38"/>
     </row>
-    <row r="92" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:44" ht="18.350000000000001" x14ac:dyDescent="0.65">
       <c r="A92" s="16" t="s">
         <v>135</v>
       </c>
@@ -3883,7 +3857,7 @@
       <c r="Z92" s="38"/>
       <c r="AA92" s="38"/>
     </row>
-    <row r="93" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:44" ht="18.350000000000001" x14ac:dyDescent="0.65">
       <c r="A93" s="16" t="s">
         <v>137</v>
       </c>
@@ -3916,7 +3890,7 @@
       <c r="Z93" s="38"/>
       <c r="AA93" s="38"/>
     </row>
-    <row r="94" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:44" ht="18.350000000000001" x14ac:dyDescent="0.65">
       <c r="A94" s="16" t="s">
         <v>138</v>
       </c>
@@ -3951,7 +3925,7 @@
       <c r="Z94" s="38"/>
       <c r="AA94" s="38"/>
     </row>
-    <row r="95" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:44" ht="18.350000000000001" x14ac:dyDescent="0.65">
       <c r="A95" s="16" t="s">
         <v>140</v>
       </c>
@@ -3986,7 +3960,7 @@
       <c r="X95" s="41"/>
       <c r="Y95" s="41"/>
     </row>
-    <row r="96" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:44" ht="18.350000000000001" x14ac:dyDescent="0.65">
       <c r="A96" s="16" t="s">
         <v>141</v>
       </c>
@@ -4000,7 +3974,7 @@
       <c r="X96" s="34"/>
       <c r="Y96" s="34"/>
     </row>
-    <row r="97" spans="1:2498" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:2498" ht="18.350000000000001" x14ac:dyDescent="0.65">
       <c r="A97" s="16" t="s">
         <v>142</v>
       </c>
@@ -4022,7 +3996,7 @@
       <c r="AH97" s="34"/>
       <c r="AI97" s="34"/>
     </row>
-    <row r="98" spans="1:2498" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:2498" ht="18.350000000000001" x14ac:dyDescent="0.65">
       <c r="A98" s="7" t="s">
         <v>143</v>
       </c>
@@ -4035,7 +4009,7 @@
       <c r="D98" s="42"/>
       <c r="AI98" s="34"/>
     </row>
-    <row r="99" spans="1:2498" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:2498" ht="18.350000000000001" x14ac:dyDescent="0.65">
       <c r="A99" s="7" t="s">
         <v>144</v>
       </c>
@@ -4052,21 +4026,21 @@
       <c r="AM99" s="34"/>
       <c r="AN99" s="34"/>
     </row>
-    <row r="100" spans="1:2498" s="99" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A100" s="99" t="s">
+    <row r="100" spans="1:2498" ht="18.350000000000001" x14ac:dyDescent="0.65">
+      <c r="A100" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="B100" s="113">
+      <c r="B100" s="17">
         <v>2</v>
       </c>
-      <c r="C100" s="113">
+      <c r="C100" s="17">
         <v>13</v>
       </c>
-      <c r="D100" s="114"/>
-      <c r="AO100" s="115"/>
-      <c r="AP100" s="115"/>
-    </row>
-    <row r="101" spans="1:2498" s="43" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+      <c r="D100" s="82"/>
+      <c r="AO100" s="83"/>
+      <c r="AP100" s="83"/>
+    </row>
+    <row r="101" spans="1:2498" s="43" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
       <c r="A101" s="25" t="s">
         <v>146</v>
       </c>
@@ -6568,7 +6542,7 @@
       <c r="CRA101" s="27"/>
       <c r="CRB101" s="27"/>
     </row>
-    <row r="102" spans="1:2498" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:2498" ht="18.350000000000001" x14ac:dyDescent="0.65">
       <c r="A102" s="44" t="s">
         <v>147</v>
       </c>
@@ -6582,7 +6556,7 @@
       <c r="E102" s="19"/>
       <c r="F102" s="19"/>
     </row>
-    <row r="103" spans="1:2498" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:2498" ht="18.350000000000001" x14ac:dyDescent="0.65">
       <c r="A103" s="44" t="s">
         <v>148</v>
       </c>
@@ -6599,7 +6573,7 @@
       <c r="J103" s="19"/>
       <c r="K103" s="19"/>
     </row>
-    <row r="104" spans="1:2498" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:2498" ht="18.350000000000001" x14ac:dyDescent="0.65">
       <c r="A104" s="44" t="s">
         <v>149</v>
       </c>
@@ -6616,7 +6590,7 @@
       <c r="J104" s="19"/>
       <c r="K104" s="19"/>
     </row>
-    <row r="105" spans="1:2498" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:2498" ht="18.350000000000001" x14ac:dyDescent="0.65">
       <c r="A105" s="44" t="s">
         <v>150</v>
       </c>
@@ -6633,7 +6607,7 @@
       <c r="J105" s="19"/>
       <c r="K105" s="19"/>
     </row>
-    <row r="106" spans="1:2498" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:2498" ht="18.350000000000001" x14ac:dyDescent="0.65">
       <c r="A106" s="44" t="s">
         <v>151</v>
       </c>
@@ -6658,7 +6632,7 @@
       <c r="R106" s="22"/>
       <c r="S106" s="22"/>
     </row>
-    <row r="107" spans="1:2498" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:2498" ht="18.350000000000001" x14ac:dyDescent="0.65">
       <c r="A107" s="44" t="s">
         <v>152</v>
       </c>
@@ -6675,7 +6649,7 @@
       <c r="W107" s="24"/>
       <c r="X107" s="24"/>
     </row>
-    <row r="108" spans="1:2498" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:2498" ht="18.350000000000001" x14ac:dyDescent="0.65">
       <c r="A108" s="44" t="s">
         <v>154</v>
       </c>
@@ -6692,7 +6666,7 @@
       <c r="AB108" s="24"/>
       <c r="AC108" s="24"/>
     </row>
-    <row r="109" spans="1:2498" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:2498" ht="18.350000000000001" x14ac:dyDescent="0.65">
       <c r="A109" s="44" t="s">
         <v>155</v>
       </c>
@@ -6710,7 +6684,7 @@
       <c r="AH109" s="24"/>
       <c r="AI109" s="24"/>
     </row>
-    <row r="110" spans="1:2498" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:2498" ht="18.350000000000001" x14ac:dyDescent="0.65">
       <c r="A110" s="44" t="s">
         <v>156</v>
       </c>
@@ -6728,7 +6702,7 @@
       <c r="AN110" s="24"/>
       <c r="AO110" s="24"/>
     </row>
-    <row r="111" spans="1:2498" s="43" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:2498" s="43" customFormat="1" ht="18.350000000000001" x14ac:dyDescent="0.65">
       <c r="A111" s="46" t="s">
         <v>158</v>
       </c>
@@ -6761,294 +6735,294 @@
       <selection activeCell="E2" sqref="E2:G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.64453125" defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.5"/>
   <sheetData>
-    <row r="2" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="96" t="s">
+    <row r="2" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B2" s="109" t="s">
         <v>159</v>
       </c>
-      <c r="C2" s="96"/>
-      <c r="D2" s="96"/>
-      <c r="E2" s="96" t="s">
+      <c r="C2" s="109"/>
+      <c r="D2" s="109"/>
+      <c r="E2" s="109" t="s">
         <v>160</v>
       </c>
-      <c r="F2" s="96"/>
-      <c r="G2" s="96"/>
-      <c r="H2" s="96" t="s">
+      <c r="F2" s="109"/>
+      <c r="G2" s="109"/>
+      <c r="H2" s="109" t="s">
         <v>161</v>
       </c>
-      <c r="I2" s="96"/>
-      <c r="J2" s="96"/>
-      <c r="K2" s="96" t="s">
+      <c r="I2" s="109"/>
+      <c r="J2" s="109"/>
+      <c r="K2" s="109" t="s">
         <v>162</v>
       </c>
-      <c r="L2" s="96"/>
-      <c r="M2" s="96"/>
-      <c r="N2" s="96" t="s">
+      <c r="L2" s="109"/>
+      <c r="M2" s="109"/>
+      <c r="N2" s="109" t="s">
         <v>163</v>
       </c>
-      <c r="O2" s="96"/>
-      <c r="P2" s="96"/>
-      <c r="Q2" s="96" t="s">
+      <c r="O2" s="109"/>
+      <c r="P2" s="109"/>
+      <c r="Q2" s="109" t="s">
         <v>164</v>
       </c>
-      <c r="R2" s="96"/>
-      <c r="S2" s="96"/>
-    </row>
-    <row r="3" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="95" t="s">
+      <c r="R2" s="109"/>
+      <c r="S2" s="109"/>
+    </row>
+    <row r="3" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B3" s="110" t="s">
         <v>165</v>
       </c>
-      <c r="C3" s="95"/>
-      <c r="D3" s="95"/>
-      <c r="E3" s="95" t="s">
+      <c r="C3" s="110"/>
+      <c r="D3" s="110"/>
+      <c r="E3" s="110" t="s">
         <v>165</v>
       </c>
-      <c r="F3" s="95"/>
-      <c r="G3" s="95"/>
-      <c r="H3" s="95" t="s">
+      <c r="F3" s="110"/>
+      <c r="G3" s="110"/>
+      <c r="H3" s="110" t="s">
         <v>165</v>
       </c>
-      <c r="I3" s="95"/>
-      <c r="J3" s="95"/>
-      <c r="K3" s="95" t="s">
+      <c r="I3" s="110"/>
+      <c r="J3" s="110"/>
+      <c r="K3" s="110" t="s">
         <v>165</v>
       </c>
-      <c r="L3" s="95"/>
-      <c r="M3" s="95"/>
-      <c r="N3" s="95" t="s">
+      <c r="L3" s="110"/>
+      <c r="M3" s="110"/>
+      <c r="N3" s="110" t="s">
         <v>165</v>
       </c>
-      <c r="O3" s="95"/>
-      <c r="P3" s="95"/>
-      <c r="Q3" s="95" t="s">
+      <c r="O3" s="110"/>
+      <c r="P3" s="110"/>
+      <c r="Q3" s="110" t="s">
         <v>165</v>
       </c>
-      <c r="R3" s="95"/>
-      <c r="S3" s="95"/>
-    </row>
-    <row r="4" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="94"/>
-      <c r="C4" s="94"/>
-      <c r="D4" s="94"/>
-      <c r="E4" s="94"/>
-      <c r="F4" s="94"/>
-      <c r="G4" s="94"/>
-      <c r="H4" s="94"/>
-      <c r="I4" s="94"/>
-      <c r="J4" s="94"/>
-      <c r="K4" s="94"/>
-      <c r="L4" s="94"/>
-      <c r="M4" s="94"/>
-      <c r="N4" s="94"/>
-      <c r="O4" s="94"/>
-      <c r="P4" s="94"/>
-      <c r="Q4" s="94"/>
-      <c r="R4" s="94"/>
-      <c r="S4" s="94"/>
-    </row>
-    <row r="5" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="94"/>
-      <c r="C5" s="94"/>
-      <c r="D5" s="94"/>
-      <c r="E5" s="94"/>
-      <c r="F5" s="94"/>
-      <c r="G5" s="94"/>
-      <c r="H5" s="94"/>
-      <c r="I5" s="94"/>
-      <c r="J5" s="94"/>
-      <c r="K5" s="94"/>
-      <c r="L5" s="94"/>
-      <c r="M5" s="94"/>
-      <c r="N5" s="94"/>
-      <c r="O5" s="94"/>
-      <c r="P5" s="94"/>
-      <c r="Q5" s="94"/>
-      <c r="R5" s="94"/>
-      <c r="S5" s="94"/>
-    </row>
-    <row r="6" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="94"/>
-      <c r="C6" s="94"/>
-      <c r="D6" s="94"/>
-      <c r="E6" s="94"/>
-      <c r="F6" s="94"/>
-      <c r="G6" s="94"/>
-      <c r="H6" s="94"/>
-      <c r="I6" s="94"/>
-      <c r="J6" s="94"/>
-      <c r="K6" s="94"/>
-      <c r="L6" s="94"/>
-      <c r="M6" s="94"/>
-      <c r="N6" s="94"/>
-      <c r="O6" s="94"/>
-      <c r="P6" s="94"/>
-      <c r="Q6" s="94"/>
-      <c r="R6" s="94"/>
-      <c r="S6" s="94"/>
-    </row>
-    <row r="7" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="94"/>
-      <c r="C7" s="94"/>
-      <c r="D7" s="94"/>
-      <c r="E7" s="94"/>
-      <c r="F7" s="94"/>
-      <c r="G7" s="94"/>
-      <c r="H7" s="94"/>
-      <c r="I7" s="94"/>
-      <c r="J7" s="94"/>
-      <c r="K7" s="94"/>
-      <c r="L7" s="94"/>
-      <c r="M7" s="94"/>
-      <c r="N7" s="94"/>
-      <c r="O7" s="94"/>
-      <c r="P7" s="94"/>
-      <c r="Q7" s="94"/>
-      <c r="R7" s="94"/>
-      <c r="S7" s="94"/>
-    </row>
-    <row r="8" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="94"/>
-      <c r="C8" s="94"/>
-      <c r="D8" s="94"/>
-      <c r="E8" s="94"/>
-      <c r="F8" s="94"/>
-      <c r="G8" s="94"/>
-      <c r="H8" s="94"/>
-      <c r="I8" s="94"/>
-      <c r="J8" s="94"/>
-      <c r="K8" s="94"/>
-      <c r="L8" s="94"/>
-      <c r="M8" s="94"/>
-      <c r="N8" s="94"/>
-      <c r="O8" s="94"/>
-      <c r="P8" s="94"/>
-      <c r="Q8" s="94"/>
-      <c r="R8" s="94"/>
-      <c r="S8" s="94"/>
-    </row>
-    <row r="9" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="94"/>
-      <c r="C9" s="94"/>
-      <c r="D9" s="94"/>
-      <c r="E9" s="94"/>
-      <c r="F9" s="94"/>
-      <c r="G9" s="94"/>
-      <c r="H9" s="94"/>
-      <c r="I9" s="94"/>
-      <c r="J9" s="94"/>
-      <c r="K9" s="94"/>
-      <c r="L9" s="94"/>
-      <c r="M9" s="94"/>
-      <c r="N9" s="94"/>
-      <c r="O9" s="94"/>
-      <c r="P9" s="94"/>
-      <c r="Q9" s="94"/>
-      <c r="R9" s="94"/>
-      <c r="S9" s="94"/>
-    </row>
-    <row r="10" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="94"/>
-      <c r="C10" s="94"/>
-      <c r="D10" s="94"/>
-      <c r="E10" s="94"/>
-      <c r="F10" s="94"/>
-      <c r="G10" s="94"/>
-      <c r="H10" s="94"/>
-      <c r="I10" s="94"/>
-      <c r="J10" s="94"/>
-      <c r="K10" s="94"/>
-      <c r="L10" s="94"/>
-      <c r="M10" s="94"/>
-      <c r="N10" s="94"/>
-      <c r="O10" s="94"/>
-      <c r="P10" s="94"/>
-      <c r="Q10" s="94"/>
-      <c r="R10" s="94"/>
-      <c r="S10" s="94"/>
-    </row>
-    <row r="11" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="94"/>
-      <c r="C11" s="94"/>
-      <c r="D11" s="94"/>
-      <c r="E11" s="94"/>
-      <c r="F11" s="94"/>
-      <c r="G11" s="94"/>
-      <c r="H11" s="94"/>
-      <c r="I11" s="94"/>
-      <c r="J11" s="94"/>
-      <c r="K11" s="94"/>
-      <c r="L11" s="94"/>
-      <c r="M11" s="94"/>
-      <c r="N11" s="94"/>
-      <c r="O11" s="94"/>
-      <c r="P11" s="94"/>
-      <c r="Q11" s="94"/>
-      <c r="R11" s="94"/>
-      <c r="S11" s="94"/>
-    </row>
-    <row r="12" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="94"/>
-      <c r="C12" s="94"/>
-      <c r="D12" s="94"/>
-      <c r="E12" s="94"/>
-      <c r="F12" s="94"/>
-      <c r="G12" s="94"/>
-      <c r="H12" s="94"/>
-      <c r="I12" s="94"/>
-      <c r="J12" s="94"/>
-      <c r="K12" s="94"/>
-      <c r="L12" s="94"/>
-      <c r="M12" s="94"/>
-      <c r="N12" s="94"/>
-      <c r="O12" s="94"/>
-      <c r="P12" s="94"/>
-      <c r="Q12" s="94"/>
-      <c r="R12" s="94"/>
-      <c r="S12" s="94"/>
-    </row>
-    <row r="13" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B13" s="94"/>
-      <c r="C13" s="94"/>
-      <c r="D13" s="94"/>
-      <c r="E13" s="94"/>
-      <c r="F13" s="94"/>
-      <c r="G13" s="94"/>
-      <c r="H13" s="94"/>
-      <c r="I13" s="94"/>
-      <c r="J13" s="94"/>
-      <c r="K13" s="94"/>
-      <c r="L13" s="94"/>
-      <c r="M13" s="94"/>
-      <c r="N13" s="94"/>
-      <c r="O13" s="94"/>
-      <c r="P13" s="94"/>
-      <c r="Q13" s="94"/>
-      <c r="R13" s="94"/>
-      <c r="S13" s="94"/>
-    </row>
-    <row r="14" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="R3" s="110"/>
+      <c r="S3" s="110"/>
+    </row>
+    <row r="4" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B4" s="111"/>
+      <c r="C4" s="111"/>
+      <c r="D4" s="111"/>
+      <c r="E4" s="111"/>
+      <c r="F4" s="111"/>
+      <c r="G4" s="111"/>
+      <c r="H4" s="111"/>
+      <c r="I4" s="111"/>
+      <c r="J4" s="111"/>
+      <c r="K4" s="111"/>
+      <c r="L4" s="111"/>
+      <c r="M4" s="111"/>
+      <c r="N4" s="111"/>
+      <c r="O4" s="111"/>
+      <c r="P4" s="111"/>
+      <c r="Q4" s="111"/>
+      <c r="R4" s="111"/>
+      <c r="S4" s="111"/>
+    </row>
+    <row r="5" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B5" s="111"/>
+      <c r="C5" s="111"/>
+      <c r="D5" s="111"/>
+      <c r="E5" s="111"/>
+      <c r="F5" s="111"/>
+      <c r="G5" s="111"/>
+      <c r="H5" s="111"/>
+      <c r="I5" s="111"/>
+      <c r="J5" s="111"/>
+      <c r="K5" s="111"/>
+      <c r="L5" s="111"/>
+      <c r="M5" s="111"/>
+      <c r="N5" s="111"/>
+      <c r="O5" s="111"/>
+      <c r="P5" s="111"/>
+      <c r="Q5" s="111"/>
+      <c r="R5" s="111"/>
+      <c r="S5" s="111"/>
+    </row>
+    <row r="6" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B6" s="111"/>
+      <c r="C6" s="111"/>
+      <c r="D6" s="111"/>
+      <c r="E6" s="111"/>
+      <c r="F6" s="111"/>
+      <c r="G6" s="111"/>
+      <c r="H6" s="111"/>
+      <c r="I6" s="111"/>
+      <c r="J6" s="111"/>
+      <c r="K6" s="111"/>
+      <c r="L6" s="111"/>
+      <c r="M6" s="111"/>
+      <c r="N6" s="111"/>
+      <c r="O6" s="111"/>
+      <c r="P6" s="111"/>
+      <c r="Q6" s="111"/>
+      <c r="R6" s="111"/>
+      <c r="S6" s="111"/>
+    </row>
+    <row r="7" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B7" s="111"/>
+      <c r="C7" s="111"/>
+      <c r="D7" s="111"/>
+      <c r="E7" s="111"/>
+      <c r="F7" s="111"/>
+      <c r="G7" s="111"/>
+      <c r="H7" s="111"/>
+      <c r="I7" s="111"/>
+      <c r="J7" s="111"/>
+      <c r="K7" s="111"/>
+      <c r="L7" s="111"/>
+      <c r="M7" s="111"/>
+      <c r="N7" s="111"/>
+      <c r="O7" s="111"/>
+      <c r="P7" s="111"/>
+      <c r="Q7" s="111"/>
+      <c r="R7" s="111"/>
+      <c r="S7" s="111"/>
+    </row>
+    <row r="8" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B8" s="111"/>
+      <c r="C8" s="111"/>
+      <c r="D8" s="111"/>
+      <c r="E8" s="111"/>
+      <c r="F8" s="111"/>
+      <c r="G8" s="111"/>
+      <c r="H8" s="111"/>
+      <c r="I8" s="111"/>
+      <c r="J8" s="111"/>
+      <c r="K8" s="111"/>
+      <c r="L8" s="111"/>
+      <c r="M8" s="111"/>
+      <c r="N8" s="111"/>
+      <c r="O8" s="111"/>
+      <c r="P8" s="111"/>
+      <c r="Q8" s="111"/>
+      <c r="R8" s="111"/>
+      <c r="S8" s="111"/>
+    </row>
+    <row r="9" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B9" s="111"/>
+      <c r="C9" s="111"/>
+      <c r="D9" s="111"/>
+      <c r="E9" s="111"/>
+      <c r="F9" s="111"/>
+      <c r="G9" s="111"/>
+      <c r="H9" s="111"/>
+      <c r="I9" s="111"/>
+      <c r="J9" s="111"/>
+      <c r="K9" s="111"/>
+      <c r="L9" s="111"/>
+      <c r="M9" s="111"/>
+      <c r="N9" s="111"/>
+      <c r="O9" s="111"/>
+      <c r="P9" s="111"/>
+      <c r="Q9" s="111"/>
+      <c r="R9" s="111"/>
+      <c r="S9" s="111"/>
+    </row>
+    <row r="10" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B10" s="111"/>
+      <c r="C10" s="111"/>
+      <c r="D10" s="111"/>
+      <c r="E10" s="111"/>
+      <c r="F10" s="111"/>
+      <c r="G10" s="111"/>
+      <c r="H10" s="111"/>
+      <c r="I10" s="111"/>
+      <c r="J10" s="111"/>
+      <c r="K10" s="111"/>
+      <c r="L10" s="111"/>
+      <c r="M10" s="111"/>
+      <c r="N10" s="111"/>
+      <c r="O10" s="111"/>
+      <c r="P10" s="111"/>
+      <c r="Q10" s="111"/>
+      <c r="R10" s="111"/>
+      <c r="S10" s="111"/>
+    </row>
+    <row r="11" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B11" s="111"/>
+      <c r="C11" s="111"/>
+      <c r="D11" s="111"/>
+      <c r="E11" s="111"/>
+      <c r="F11" s="111"/>
+      <c r="G11" s="111"/>
+      <c r="H11" s="111"/>
+      <c r="I11" s="111"/>
+      <c r="J11" s="111"/>
+      <c r="K11" s="111"/>
+      <c r="L11" s="111"/>
+      <c r="M11" s="111"/>
+      <c r="N11" s="111"/>
+      <c r="O11" s="111"/>
+      <c r="P11" s="111"/>
+      <c r="Q11" s="111"/>
+      <c r="R11" s="111"/>
+      <c r="S11" s="111"/>
+    </row>
+    <row r="12" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B12" s="111"/>
+      <c r="C12" s="111"/>
+      <c r="D12" s="111"/>
+      <c r="E12" s="111"/>
+      <c r="F12" s="111"/>
+      <c r="G12" s="111"/>
+      <c r="H12" s="111"/>
+      <c r="I12" s="111"/>
+      <c r="J12" s="111"/>
+      <c r="K12" s="111"/>
+      <c r="L12" s="111"/>
+      <c r="M12" s="111"/>
+      <c r="N12" s="111"/>
+      <c r="O12" s="111"/>
+      <c r="P12" s="111"/>
+      <c r="Q12" s="111"/>
+      <c r="R12" s="111"/>
+      <c r="S12" s="111"/>
+    </row>
+    <row r="13" spans="1:19" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="B13" s="111"/>
+      <c r="C13" s="111"/>
+      <c r="D13" s="111"/>
+      <c r="E13" s="111"/>
+      <c r="F13" s="111"/>
+      <c r="G13" s="111"/>
+      <c r="H13" s="111"/>
+      <c r="I13" s="111"/>
+      <c r="J13" s="111"/>
+      <c r="K13" s="111"/>
+      <c r="L13" s="111"/>
+      <c r="M13" s="111"/>
+      <c r="N13" s="111"/>
+      <c r="O13" s="111"/>
+      <c r="P13" s="111"/>
+      <c r="Q13" s="111"/>
+      <c r="R13" s="111"/>
+      <c r="S13" s="111"/>
+    </row>
+    <row r="14" spans="1:19" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A14" s="50"/>
-      <c r="B14" s="95"/>
-      <c r="C14" s="95"/>
-      <c r="D14" s="95"/>
-      <c r="E14" s="95"/>
-      <c r="F14" s="95"/>
-      <c r="G14" s="95"/>
-      <c r="H14" s="95"/>
-      <c r="I14" s="95"/>
-      <c r="J14" s="95"/>
-      <c r="K14" s="95"/>
-      <c r="L14" s="95"/>
-      <c r="M14" s="95"/>
-      <c r="N14" s="95"/>
-      <c r="O14" s="95"/>
-      <c r="P14" s="95"/>
-      <c r="Q14" s="95"/>
-      <c r="R14" s="95"/>
-      <c r="S14" s="95"/>
-    </row>
-    <row r="15" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="B14" s="110"/>
+      <c r="C14" s="110"/>
+      <c r="D14" s="110"/>
+      <c r="E14" s="110"/>
+      <c r="F14" s="110"/>
+      <c r="G14" s="110"/>
+      <c r="H14" s="110"/>
+      <c r="I14" s="110"/>
+      <c r="J14" s="110"/>
+      <c r="K14" s="110"/>
+      <c r="L14" s="110"/>
+      <c r="M14" s="110"/>
+      <c r="N14" s="110"/>
+      <c r="O14" s="110"/>
+      <c r="P14" s="110"/>
+      <c r="Q14" s="110"/>
+      <c r="R14" s="110"/>
+      <c r="S14" s="110"/>
+    </row>
+    <row r="15" spans="1:19" ht="14.35" x14ac:dyDescent="0.5">
       <c r="B15" s="51" t="s">
         <v>166</v>
       </c>
@@ -7063,6 +7037,18 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="Q4:S13"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="H14:J14"/>
+    <mergeCell ref="K14:M14"/>
+    <mergeCell ref="N14:P14"/>
+    <mergeCell ref="Q14:S14"/>
+    <mergeCell ref="B4:D13"/>
+    <mergeCell ref="E4:G13"/>
+    <mergeCell ref="H4:J13"/>
+    <mergeCell ref="K4:M13"/>
+    <mergeCell ref="N4:P13"/>
     <mergeCell ref="Q2:S2"/>
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="E3:G3"/>
@@ -7075,18 +7061,6 @@
     <mergeCell ref="H2:J2"/>
     <mergeCell ref="K2:M2"/>
     <mergeCell ref="N2:P2"/>
-    <mergeCell ref="Q4:S13"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="H14:J14"/>
-    <mergeCell ref="K14:M14"/>
-    <mergeCell ref="N14:P14"/>
-    <mergeCell ref="Q14:S14"/>
-    <mergeCell ref="B4:D13"/>
-    <mergeCell ref="E4:G13"/>
-    <mergeCell ref="H4:J13"/>
-    <mergeCell ref="K4:M13"/>
-    <mergeCell ref="N4:P13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -7101,12 +7075,12 @@
       <selection activeCell="C11" sqref="C11:H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.64453125" defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="6" max="6" width="11.77734375" customWidth="1"/>
+    <col min="6" max="6" width="11.76171875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:15" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:15" ht="14.35" x14ac:dyDescent="0.5">
       <c r="B2" s="53"/>
       <c r="C2" s="54" t="s">
         <v>167</v>
@@ -7120,10 +7094,10 @@
       <c r="F2" s="55" t="s">
         <v>170</v>
       </c>
-      <c r="G2" s="110" t="s">
+      <c r="G2" s="80" t="s">
         <v>171</v>
       </c>
-      <c r="H2" s="111" t="s">
+      <c r="H2" s="81" t="s">
         <v>181</v>
       </c>
       <c r="I2" s="55"/>
@@ -7131,7 +7105,7 @@
       <c r="K2" s="55"/>
       <c r="L2" s="56"/>
     </row>
-    <row r="3" spans="2:15" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:15" ht="43" x14ac:dyDescent="0.5">
       <c r="B3" s="53"/>
       <c r="C3" s="57" t="s">
         <v>172</v>
@@ -7156,7 +7130,7 @@
       <c r="K3" s="58"/>
       <c r="L3" s="59"/>
     </row>
-    <row r="4" spans="2:15" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:15" ht="14.35" x14ac:dyDescent="0.5">
       <c r="B4" s="53" t="s">
         <v>176</v>
       </c>
@@ -7183,7 +7157,7 @@
       <c r="K4" s="61"/>
       <c r="L4" s="62"/>
     </row>
-    <row r="5" spans="2:15" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:15" ht="14.35" x14ac:dyDescent="0.5">
       <c r="B5" s="63" t="s">
         <v>7</v>
       </c>
@@ -7210,7 +7184,7 @@
       <c r="K5" s="64"/>
       <c r="L5" s="64"/>
     </row>
-    <row r="6" spans="2:15" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:15" ht="14.35" x14ac:dyDescent="0.5">
       <c r="B6" s="65" t="s">
         <v>9</v>
       </c>
@@ -7229,7 +7203,7 @@
       <c r="G6">
         <v>4</v>
       </c>
-      <c r="H6" s="109" t="s">
+      <c r="H6" s="79" t="s">
         <v>180</v>
       </c>
       <c r="I6" s="53"/>
@@ -7240,7 +7214,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="2:15" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:15" ht="14.35" x14ac:dyDescent="0.5">
       <c r="B7" s="65" t="s">
         <v>177</v>
       </c>
@@ -7259,7 +7233,7 @@
       <c r="G7">
         <v>2</v>
       </c>
-      <c r="H7" s="109" t="s">
+      <c r="H7" s="79" t="s">
         <v>180</v>
       </c>
       <c r="I7" s="64"/>
@@ -7270,7 +7244,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="2:15" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:15" ht="14.35" x14ac:dyDescent="0.5">
       <c r="B8" s="65" t="s">
         <v>11</v>
       </c>
@@ -7289,7 +7263,7 @@
       <c r="G8">
         <v>1</v>
       </c>
-      <c r="H8" s="109" t="s">
+      <c r="H8" s="79" t="s">
         <v>180</v>
       </c>
       <c r="I8" s="64"/>
@@ -7300,7 +7274,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="2:15" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:15" ht="14.35" x14ac:dyDescent="0.5">
       <c r="B9" s="65" t="s">
         <v>178</v>
       </c>
@@ -7330,7 +7304,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:15" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:15" ht="14.35" x14ac:dyDescent="0.5">
       <c r="B10" s="65" t="s">
         <v>13</v>
       </c>
@@ -7357,7 +7331,7 @@
       <c r="K10" s="64"/>
       <c r="L10" s="64"/>
     </row>
-    <row r="11" spans="2:15" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:15" ht="14.35" x14ac:dyDescent="0.5">
       <c r="B11" s="66" t="s">
         <v>14</v>
       </c>
@@ -7384,7 +7358,7 @@
       <c r="K11" s="53"/>
       <c r="L11" s="53"/>
     </row>
-    <row r="12" spans="2:15" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:15" ht="14.35" x14ac:dyDescent="0.5">
       <c r="B12" s="67" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Added tests and finished Gantts
</commit_message>
<xml_diff>
--- a/383Game/Doc/Brain Stew Master Gantt Chart.xlsx
+++ b/383Game/Doc/Brain Stew Master Gantt Chart.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bidhi\OneDrive\Desktop\school\CS383\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clcla\Documents\bc\BcGitReop\CS383BrainstewGame\383Game\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DE2EE78-581D-4A47-AE04-EC930086EB2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8A474D5-B7B4-4C44-A2DC-3CB215E321DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Budget" sheetId="1" r:id="rId1"/>
@@ -1103,7 +1103,50 @@
     <xf numFmtId="0" fontId="2" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1127,64 +1170,21 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1452,597 +1452,650 @@
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="9" max="9" width="10.6328125" customWidth="1"/>
-    <col min="17" max="17" width="10.36328125" customWidth="1"/>
+    <col min="9" max="9" width="10.6640625" customWidth="1"/>
+    <col min="17" max="17" width="10.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C2" s="111" t="s">
+    <row r="2" spans="2:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C2" s="96" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="111"/>
-      <c r="E2" s="111"/>
-      <c r="F2" s="111"/>
-      <c r="G2" s="111"/>
-      <c r="H2" s="111"/>
-      <c r="K2" s="111" t="s">
+      <c r="D2" s="96"/>
+      <c r="E2" s="96"/>
+      <c r="F2" s="96"/>
+      <c r="G2" s="96"/>
+      <c r="H2" s="96"/>
+      <c r="K2" s="96" t="s">
         <v>1</v>
       </c>
-      <c r="L2" s="111"/>
-      <c r="M2" s="111"/>
-      <c r="N2" s="111"/>
-      <c r="O2" s="111"/>
-      <c r="P2" s="111"/>
-      <c r="S2" s="111" t="s">
+      <c r="L2" s="96"/>
+      <c r="M2" s="96"/>
+      <c r="N2" s="96"/>
+      <c r="O2" s="96"/>
+      <c r="P2" s="96"/>
+      <c r="S2" s="96" t="s">
         <v>2</v>
       </c>
-      <c r="T2" s="111"/>
-      <c r="U2" s="111"/>
-      <c r="V2" s="111"/>
-      <c r="W2" s="111"/>
-      <c r="X2" s="111"/>
-      <c r="AA2" s="111" t="s">
+      <c r="T2" s="96"/>
+      <c r="U2" s="96"/>
+      <c r="V2" s="96"/>
+      <c r="W2" s="96"/>
+      <c r="X2" s="96"/>
+      <c r="AA2" s="96" t="s">
         <v>3</v>
       </c>
-      <c r="AB2" s="111"/>
-      <c r="AC2" s="111"/>
-      <c r="AD2" s="111"/>
-      <c r="AE2" s="111"/>
-      <c r="AF2" s="111"/>
-    </row>
-    <row r="3" spans="2:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C3" s="112" t="s">
+      <c r="AB2" s="96"/>
+      <c r="AC2" s="96"/>
+      <c r="AD2" s="96"/>
+      <c r="AE2" s="96"/>
+      <c r="AF2" s="96"/>
+    </row>
+    <row r="3" spans="2:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C3" s="97" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="112"/>
-      <c r="E3" s="113" t="s">
+      <c r="D3" s="97"/>
+      <c r="E3" s="98" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="113"/>
-      <c r="G3" s="114" t="s">
+      <c r="F3" s="98"/>
+      <c r="G3" s="99" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="114"/>
-      <c r="K3" s="112" t="s">
+      <c r="H3" s="99"/>
+      <c r="K3" s="97" t="s">
         <v>4</v>
       </c>
-      <c r="L3" s="112"/>
-      <c r="M3" s="113" t="s">
+      <c r="L3" s="97"/>
+      <c r="M3" s="98" t="s">
         <v>5</v>
       </c>
-      <c r="N3" s="113"/>
-      <c r="O3" s="114" t="s">
+      <c r="N3" s="98"/>
+      <c r="O3" s="99" t="s">
         <v>6</v>
       </c>
-      <c r="P3" s="114"/>
-      <c r="S3" s="112" t="s">
+      <c r="P3" s="99"/>
+      <c r="S3" s="97" t="s">
         <v>4</v>
       </c>
-      <c r="T3" s="112"/>
-      <c r="U3" s="113" t="s">
+      <c r="T3" s="97"/>
+      <c r="U3" s="98" t="s">
         <v>5</v>
       </c>
-      <c r="V3" s="113"/>
-      <c r="W3" s="114" t="s">
+      <c r="V3" s="98"/>
+      <c r="W3" s="99" t="s">
         <v>6</v>
       </c>
-      <c r="X3" s="114"/>
-      <c r="AA3" s="112" t="s">
+      <c r="X3" s="99"/>
+      <c r="AA3" s="97" t="s">
         <v>4</v>
       </c>
-      <c r="AB3" s="112"/>
-      <c r="AC3" s="113" t="s">
+      <c r="AB3" s="97"/>
+      <c r="AC3" s="98" t="s">
         <v>5</v>
       </c>
-      <c r="AD3" s="113"/>
-      <c r="AE3" s="114" t="s">
+      <c r="AD3" s="98"/>
+      <c r="AE3" s="99" t="s">
         <v>6</v>
       </c>
-      <c r="AF3" s="114"/>
-    </row>
-    <row r="4" spans="2:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="AF3" s="99"/>
+    </row>
+    <row r="4" spans="2:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="100">
+      <c r="C4" s="93">
         <v>8200</v>
       </c>
-      <c r="D4" s="100"/>
-      <c r="E4" s="109">
+      <c r="D4" s="93"/>
+      <c r="E4" s="94">
         <v>2500</v>
       </c>
-      <c r="F4" s="109"/>
-      <c r="G4" s="108" t="s">
+      <c r="F4" s="94"/>
+      <c r="G4" s="95" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="108"/>
+      <c r="H4" s="95"/>
       <c r="J4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K4" s="110">
+      <c r="K4" s="107">
         <v>5200</v>
       </c>
-      <c r="L4" s="110"/>
-      <c r="M4" s="109">
+      <c r="L4" s="107"/>
+      <c r="M4" s="94">
         <v>1400</v>
       </c>
-      <c r="N4" s="109"/>
-      <c r="O4" s="108" t="s">
+      <c r="N4" s="94"/>
+      <c r="O4" s="95" t="s">
         <v>8</v>
       </c>
-      <c r="P4" s="108"/>
+      <c r="P4" s="95"/>
       <c r="R4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="S4" s="100">
+      <c r="S4" s="93">
         <v>3000</v>
       </c>
-      <c r="T4" s="100"/>
-      <c r="U4" s="109">
+      <c r="T4" s="93"/>
+      <c r="U4" s="94">
         <v>1100</v>
       </c>
-      <c r="V4" s="109"/>
-      <c r="W4" s="108" t="s">
+      <c r="V4" s="94"/>
+      <c r="W4" s="95" t="s">
         <v>8</v>
       </c>
-      <c r="X4" s="108"/>
+      <c r="X4" s="95"/>
       <c r="Z4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="AA4" s="106"/>
-      <c r="AB4" s="106"/>
-      <c r="AC4" s="107"/>
-      <c r="AD4" s="107"/>
-      <c r="AE4" s="108"/>
-      <c r="AF4" s="108"/>
-    </row>
-    <row r="5" spans="2:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="AA4" s="102"/>
+      <c r="AB4" s="102"/>
+      <c r="AC4" s="103"/>
+      <c r="AD4" s="103"/>
+      <c r="AE4" s="95"/>
+      <c r="AF4" s="95"/>
+    </row>
+    <row r="5" spans="2:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="100">
+      <c r="C5" s="93">
         <v>10200</v>
       </c>
-      <c r="D5" s="100"/>
-      <c r="E5" s="101">
+      <c r="D5" s="93"/>
+      <c r="E5" s="100">
         <v>3100</v>
       </c>
-      <c r="F5" s="101"/>
-      <c r="G5" s="102" t="s">
+      <c r="F5" s="100"/>
+      <c r="G5" s="101" t="s">
         <v>8</v>
       </c>
-      <c r="H5" s="102"/>
+      <c r="H5" s="101"/>
       <c r="J5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K5" s="105">
+      <c r="K5" s="104">
         <v>7200</v>
       </c>
-      <c r="L5" s="105"/>
-      <c r="M5" s="101">
+      <c r="L5" s="104"/>
+      <c r="M5" s="100">
         <v>1900</v>
       </c>
-      <c r="N5" s="101"/>
-      <c r="O5" s="102" t="s">
+      <c r="N5" s="100"/>
+      <c r="O5" s="101" t="s">
         <v>8</v>
       </c>
-      <c r="P5" s="102"/>
+      <c r="P5" s="101"/>
       <c r="R5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="S5" s="100">
+      <c r="S5" s="93">
         <v>3000</v>
       </c>
-      <c r="T5" s="100"/>
-      <c r="U5" s="101">
+      <c r="T5" s="93"/>
+      <c r="U5" s="100">
         <v>1200</v>
       </c>
-      <c r="V5" s="101"/>
-      <c r="W5" s="102" t="s">
+      <c r="V5" s="100"/>
+      <c r="W5" s="101" t="s">
         <v>8</v>
       </c>
-      <c r="X5" s="102"/>
+      <c r="X5" s="101"/>
       <c r="Z5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="AA5" s="104"/>
-      <c r="AB5" s="104"/>
-      <c r="AC5" s="92"/>
-      <c r="AD5" s="92"/>
-      <c r="AE5" s="102"/>
-      <c r="AF5" s="102"/>
-    </row>
-    <row r="6" spans="2:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="AA5" s="105"/>
+      <c r="AB5" s="105"/>
+      <c r="AC5" s="106"/>
+      <c r="AD5" s="106"/>
+      <c r="AE5" s="101"/>
+      <c r="AF5" s="101"/>
+    </row>
+    <row r="6" spans="2:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="100">
+      <c r="C6" s="93">
         <v>8300</v>
       </c>
-      <c r="D6" s="100"/>
-      <c r="E6" s="101">
+      <c r="D6" s="93"/>
+      <c r="E6" s="100">
         <v>1600</v>
       </c>
-      <c r="F6" s="101"/>
-      <c r="G6" s="102" t="s">
+      <c r="F6" s="100"/>
+      <c r="G6" s="101" t="s">
         <v>8</v>
       </c>
-      <c r="H6" s="102"/>
+      <c r="H6" s="101"/>
       <c r="J6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="K6" s="105">
+      <c r="K6" s="104">
         <v>5300</v>
       </c>
-      <c r="L6" s="105"/>
-      <c r="M6" s="101">
+      <c r="L6" s="104"/>
+      <c r="M6" s="100">
         <v>600</v>
       </c>
-      <c r="N6" s="101"/>
-      <c r="O6" s="102" t="s">
+      <c r="N6" s="100"/>
+      <c r="O6" s="101" t="s">
         <v>8</v>
       </c>
-      <c r="P6" s="102"/>
+      <c r="P6" s="101"/>
       <c r="R6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="S6" s="100">
+      <c r="S6" s="93">
         <v>3000</v>
       </c>
-      <c r="T6" s="100"/>
-      <c r="U6" s="101">
+      <c r="T6" s="93"/>
+      <c r="U6" s="100">
         <v>1000</v>
       </c>
-      <c r="V6" s="101"/>
-      <c r="W6" s="102" t="s">
+      <c r="V6" s="100"/>
+      <c r="W6" s="101" t="s">
         <v>8</v>
       </c>
-      <c r="X6" s="102"/>
+      <c r="X6" s="101"/>
       <c r="Z6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="AA6" s="104"/>
-      <c r="AB6" s="104"/>
-      <c r="AC6" s="92"/>
-      <c r="AD6" s="92"/>
-      <c r="AE6" s="102"/>
-      <c r="AF6" s="102"/>
-    </row>
-    <row r="7" spans="2:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="AA6" s="105"/>
+      <c r="AB6" s="105"/>
+      <c r="AC6" s="106"/>
+      <c r="AD6" s="106"/>
+      <c r="AE6" s="101"/>
+      <c r="AF6" s="101"/>
+    </row>
+    <row r="7" spans="2:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="100">
+      <c r="C7" s="93">
         <v>9000</v>
       </c>
-      <c r="D7" s="100"/>
-      <c r="E7" s="101">
+      <c r="D7" s="93"/>
+      <c r="E7" s="100">
         <v>1300</v>
       </c>
-      <c r="F7" s="101"/>
-      <c r="G7" s="102" t="s">
+      <c r="F7" s="100"/>
+      <c r="G7" s="101" t="s">
         <v>8</v>
       </c>
-      <c r="H7" s="102"/>
+      <c r="H7" s="101"/>
       <c r="J7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="K7" s="105">
+      <c r="K7" s="104">
         <v>6000</v>
       </c>
-      <c r="L7" s="105"/>
-      <c r="M7" s="101">
+      <c r="L7" s="104"/>
+      <c r="M7" s="100">
         <v>400</v>
       </c>
-      <c r="N7" s="101"/>
-      <c r="O7" s="102" t="s">
+      <c r="N7" s="100"/>
+      <c r="O7" s="101" t="s">
         <v>8</v>
       </c>
-      <c r="P7" s="102"/>
+      <c r="P7" s="101"/>
       <c r="R7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="S7" s="100">
+      <c r="S7" s="93">
         <v>3000</v>
       </c>
-      <c r="T7" s="100"/>
-      <c r="U7" s="101">
+      <c r="T7" s="93"/>
+      <c r="U7" s="100">
         <v>900</v>
       </c>
-      <c r="V7" s="101"/>
-      <c r="W7" s="102" t="s">
+      <c r="V7" s="100"/>
+      <c r="W7" s="101" t="s">
         <v>8</v>
       </c>
-      <c r="X7" s="102"/>
+      <c r="X7" s="101"/>
       <c r="Z7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="AA7" s="104"/>
-      <c r="AB7" s="104"/>
-      <c r="AC7" s="92"/>
-      <c r="AD7" s="92"/>
-      <c r="AE7" s="102"/>
-      <c r="AF7" s="102"/>
-    </row>
-    <row r="8" spans="2:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="AA7" s="105"/>
+      <c r="AB7" s="105"/>
+      <c r="AC7" s="106"/>
+      <c r="AD7" s="106"/>
+      <c r="AE7" s="101"/>
+      <c r="AF7" s="101"/>
+    </row>
+    <row r="8" spans="2:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="100">
+      <c r="C8" s="93">
         <v>9300</v>
       </c>
-      <c r="D8" s="100"/>
-      <c r="E8" s="101">
+      <c r="D8" s="93"/>
+      <c r="E8" s="100">
         <v>1900</v>
       </c>
-      <c r="F8" s="101"/>
-      <c r="G8" s="102" t="s">
+      <c r="F8" s="100"/>
+      <c r="G8" s="101" t="s">
         <v>8</v>
       </c>
-      <c r="H8" s="102"/>
+      <c r="H8" s="101"/>
       <c r="J8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="K8" s="105">
+      <c r="K8" s="104">
         <v>6300</v>
       </c>
-      <c r="L8" s="105"/>
-      <c r="M8" s="101">
+      <c r="L8" s="104"/>
+      <c r="M8" s="100">
         <v>600</v>
       </c>
-      <c r="N8" s="101"/>
-      <c r="O8" s="102" t="s">
+      <c r="N8" s="100"/>
+      <c r="O8" s="101" t="s">
         <v>8</v>
       </c>
-      <c r="P8" s="102"/>
+      <c r="P8" s="101"/>
       <c r="R8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="S8" s="100">
+      <c r="S8" s="93">
         <v>3000</v>
       </c>
-      <c r="T8" s="100"/>
-      <c r="U8" s="101">
+      <c r="T8" s="93"/>
+      <c r="U8" s="100">
         <v>1300</v>
       </c>
-      <c r="V8" s="101"/>
-      <c r="W8" s="102" t="s">
+      <c r="V8" s="100"/>
+      <c r="W8" s="101" t="s">
         <v>8</v>
       </c>
-      <c r="X8" s="102"/>
+      <c r="X8" s="101"/>
       <c r="Z8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="AA8" s="104"/>
-      <c r="AB8" s="104"/>
-      <c r="AC8" s="92"/>
-      <c r="AD8" s="92"/>
-      <c r="AE8" s="102"/>
-      <c r="AF8" s="102"/>
-    </row>
-    <row r="9" spans="2:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="AA8" s="105"/>
+      <c r="AB8" s="105"/>
+      <c r="AC8" s="106"/>
+      <c r="AD8" s="106"/>
+      <c r="AE8" s="101"/>
+      <c r="AF8" s="101"/>
+    </row>
+    <row r="9" spans="2:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="100">
+      <c r="C9" s="93">
         <v>8500</v>
       </c>
-      <c r="D9" s="100"/>
-      <c r="E9" s="101">
+      <c r="D9" s="93"/>
+      <c r="E9" s="100">
         <v>4400</v>
       </c>
-      <c r="F9" s="101"/>
-      <c r="G9" s="102" t="s">
+      <c r="F9" s="100"/>
+      <c r="G9" s="101" t="s">
         <v>8</v>
       </c>
-      <c r="H9" s="102"/>
+      <c r="H9" s="101"/>
       <c r="J9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="K9" s="105">
+      <c r="K9" s="104">
         <v>5500</v>
       </c>
-      <c r="L9" s="105"/>
-      <c r="M9" s="101">
+      <c r="L9" s="104"/>
+      <c r="M9" s="100">
         <v>2200</v>
       </c>
-      <c r="N9" s="101"/>
-      <c r="O9" s="102" t="s">
+      <c r="N9" s="100"/>
+      <c r="O9" s="101" t="s">
         <v>8</v>
       </c>
-      <c r="P9" s="102"/>
+      <c r="P9" s="101"/>
       <c r="R9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="S9" s="100">
+      <c r="S9" s="93">
         <v>3000</v>
       </c>
-      <c r="T9" s="100"/>
-      <c r="U9" s="101">
+      <c r="T9" s="93"/>
+      <c r="U9" s="100">
         <v>1200</v>
       </c>
-      <c r="V9" s="101"/>
-      <c r="W9" s="102" t="s">
+      <c r="V9" s="100"/>
+      <c r="W9" s="101" t="s">
         <v>8</v>
       </c>
-      <c r="X9" s="102"/>
+      <c r="X9" s="101"/>
       <c r="Z9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="AA9" s="104"/>
-      <c r="AB9" s="104"/>
-      <c r="AC9" s="92"/>
-      <c r="AD9" s="92"/>
-      <c r="AE9" s="102"/>
-      <c r="AF9" s="102"/>
-    </row>
-    <row r="10" spans="2:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="AA9" s="105"/>
+      <c r="AB9" s="105"/>
+      <c r="AC9" s="106"/>
+      <c r="AD9" s="106"/>
+      <c r="AE9" s="101"/>
+      <c r="AF9" s="101"/>
+    </row>
+    <row r="10" spans="2:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="100">
+      <c r="C10" s="93">
         <v>8800</v>
       </c>
-      <c r="D10" s="100"/>
-      <c r="E10" s="101">
+      <c r="D10" s="93"/>
+      <c r="E10" s="100">
         <v>3600</v>
       </c>
-      <c r="F10" s="101"/>
-      <c r="G10" s="102" t="s">
+      <c r="F10" s="100"/>
+      <c r="G10" s="101" t="s">
         <v>8</v>
       </c>
-      <c r="H10" s="102"/>
+      <c r="H10" s="101"/>
       <c r="J10" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="K10" s="99">
+      <c r="K10" s="114">
         <v>5800</v>
       </c>
-      <c r="L10" s="99"/>
-      <c r="M10" s="103">
+      <c r="L10" s="114"/>
+      <c r="M10" s="115">
         <v>2300</v>
       </c>
-      <c r="N10" s="103"/>
-      <c r="O10" s="95" t="s">
+      <c r="N10" s="115"/>
+      <c r="O10" s="110" t="s">
         <v>8</v>
       </c>
-      <c r="P10" s="95"/>
+      <c r="P10" s="110"/>
       <c r="R10" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="S10" s="100">
+      <c r="S10" s="93">
         <v>3000</v>
       </c>
-      <c r="T10" s="100"/>
-      <c r="U10" s="101">
+      <c r="T10" s="93"/>
+      <c r="U10" s="100">
         <v>1300</v>
       </c>
-      <c r="V10" s="101"/>
-      <c r="W10" s="102" t="s">
+      <c r="V10" s="100"/>
+      <c r="W10" s="101" t="s">
         <v>8</v>
       </c>
-      <c r="X10" s="102"/>
+      <c r="X10" s="101"/>
       <c r="Z10" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="AA10" s="93"/>
-      <c r="AB10" s="93"/>
-      <c r="AC10" s="94"/>
-      <c r="AD10" s="94"/>
-      <c r="AE10" s="95"/>
-      <c r="AF10" s="95"/>
-    </row>
-    <row r="11" spans="2:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="AA10" s="108"/>
+      <c r="AB10" s="108"/>
+      <c r="AC10" s="109"/>
+      <c r="AD10" s="109"/>
+      <c r="AE10" s="110"/>
+      <c r="AF10" s="110"/>
+    </row>
+    <row r="11" spans="2:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C11" s="96">
+      <c r="C11" s="111">
         <v>62300</v>
       </c>
-      <c r="D11" s="96"/>
-      <c r="E11" s="97">
+      <c r="D11" s="111"/>
+      <c r="E11" s="112">
         <v>17400</v>
       </c>
-      <c r="F11" s="97"/>
-      <c r="G11" s="98" t="s">
+      <c r="F11" s="112"/>
+      <c r="G11" s="113" t="s">
         <v>8</v>
       </c>
-      <c r="H11" s="98"/>
+      <c r="H11" s="113"/>
       <c r="J11" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="K11" s="99">
+      <c r="K11" s="114">
         <v>43100</v>
       </c>
-      <c r="L11" s="99"/>
-      <c r="M11" s="97">
+      <c r="L11" s="114"/>
+      <c r="M11" s="112">
         <v>9400</v>
       </c>
-      <c r="N11" s="97"/>
-      <c r="O11" s="98" t="s">
+      <c r="N11" s="112"/>
+      <c r="O11" s="113" t="s">
         <v>8</v>
       </c>
-      <c r="P11" s="98"/>
+      <c r="P11" s="113"/>
       <c r="R11" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="S11" s="96">
+      <c r="S11" s="111">
         <v>21000</v>
       </c>
-      <c r="T11" s="96"/>
-      <c r="U11" s="97">
+      <c r="T11" s="111"/>
+      <c r="U11" s="112">
         <v>8000</v>
       </c>
-      <c r="V11" s="97"/>
-      <c r="W11" s="98" t="s">
+      <c r="V11" s="112"/>
+      <c r="W11" s="113" t="s">
         <v>8</v>
       </c>
-      <c r="X11" s="98"/>
+      <c r="X11" s="113"/>
       <c r="Z11" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="AA11" s="93"/>
-      <c r="AB11" s="93"/>
-      <c r="AC11" s="94"/>
-      <c r="AD11" s="94"/>
-      <c r="AE11" s="95"/>
-      <c r="AF11" s="95"/>
-    </row>
-    <row r="12" spans="2:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="Y12" s="92"/>
-      <c r="Z12" s="92"/>
-      <c r="AA12" s="92"/>
-      <c r="AB12" s="92"/>
-      <c r="AC12" s="92"/>
-      <c r="AD12" s="92"/>
-    </row>
-    <row r="15" spans="2:32" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="AA11" s="108"/>
+      <c r="AB11" s="108"/>
+      <c r="AC11" s="109"/>
+      <c r="AD11" s="109"/>
+      <c r="AE11" s="110"/>
+      <c r="AF11" s="110"/>
+    </row>
+    <row r="12" spans="2:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Y12" s="106"/>
+      <c r="Z12" s="106"/>
+      <c r="AA12" s="106"/>
+      <c r="AB12" s="106"/>
+      <c r="AC12" s="106"/>
+      <c r="AD12" s="106"/>
+    </row>
+    <row r="15" spans="2:32" ht="14.4" x14ac:dyDescent="0.3">
       <c r="I15" s="5"/>
     </row>
-    <row r="16" spans="2:32" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:32" ht="14.4" x14ac:dyDescent="0.3">
       <c r="I16" s="5"/>
     </row>
-    <row r="17" spans="9:9" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="9:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="I17" s="5"/>
     </row>
-    <row r="18" spans="9:9" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="9:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="I18" s="5"/>
     </row>
-    <row r="19" spans="9:9" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="9:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="I19" s="5"/>
     </row>
-    <row r="20" spans="9:9" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="9:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="I20" s="5"/>
     </row>
-    <row r="21" spans="9:9" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="9:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="I21" s="5"/>
     </row>
-    <row r="22" spans="9:9" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="9:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="I22" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="115">
-    <mergeCell ref="S4:T4"/>
-    <mergeCell ref="U4:V4"/>
-    <mergeCell ref="W4:X4"/>
-    <mergeCell ref="C2:H2"/>
-    <mergeCell ref="K2:P2"/>
-    <mergeCell ref="S2:X2"/>
-    <mergeCell ref="AA2:AF2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="M3:N3"/>
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="S3:T3"/>
-    <mergeCell ref="U3:V3"/>
-    <mergeCell ref="W3:X3"/>
-    <mergeCell ref="AA3:AB3"/>
-    <mergeCell ref="AC3:AD3"/>
-    <mergeCell ref="AE3:AF3"/>
+    <mergeCell ref="Y12:Z12"/>
+    <mergeCell ref="AA12:AB12"/>
+    <mergeCell ref="AC12:AD12"/>
+    <mergeCell ref="AA10:AB10"/>
+    <mergeCell ref="AC10:AD10"/>
+    <mergeCell ref="AE10:AF10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="M11:N11"/>
+    <mergeCell ref="O11:P11"/>
+    <mergeCell ref="S11:T11"/>
+    <mergeCell ref="U11:V11"/>
+    <mergeCell ref="W11:X11"/>
+    <mergeCell ref="AA11:AB11"/>
+    <mergeCell ref="AC11:AD11"/>
+    <mergeCell ref="AE11:AF11"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="S10:T10"/>
+    <mergeCell ref="U10:V10"/>
+    <mergeCell ref="W10:X10"/>
+    <mergeCell ref="AA8:AB8"/>
+    <mergeCell ref="AC8:AD8"/>
+    <mergeCell ref="AE8:AF8"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="O9:P9"/>
+    <mergeCell ref="S9:T9"/>
+    <mergeCell ref="U9:V9"/>
+    <mergeCell ref="W9:X9"/>
+    <mergeCell ref="AA9:AB9"/>
+    <mergeCell ref="AC9:AD9"/>
+    <mergeCell ref="AE9:AF9"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="O8:P8"/>
+    <mergeCell ref="S8:T8"/>
+    <mergeCell ref="U8:V8"/>
+    <mergeCell ref="W8:X8"/>
+    <mergeCell ref="AA6:AB6"/>
+    <mergeCell ref="AC6:AD6"/>
+    <mergeCell ref="AE6:AF6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="M7:N7"/>
+    <mergeCell ref="O7:P7"/>
+    <mergeCell ref="S7:T7"/>
+    <mergeCell ref="U7:V7"/>
+    <mergeCell ref="W7:X7"/>
+    <mergeCell ref="AA7:AB7"/>
+    <mergeCell ref="AC7:AD7"/>
+    <mergeCell ref="AE7:AF7"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="O6:P6"/>
     <mergeCell ref="S6:T6"/>
     <mergeCell ref="U6:V6"/>
     <mergeCell ref="W6:X6"/>
@@ -2067,78 +2120,25 @@
     <mergeCell ref="K4:L4"/>
     <mergeCell ref="M4:N4"/>
     <mergeCell ref="O4:P4"/>
-    <mergeCell ref="S8:T8"/>
-    <mergeCell ref="U8:V8"/>
-    <mergeCell ref="W8:X8"/>
-    <mergeCell ref="AA6:AB6"/>
-    <mergeCell ref="AC6:AD6"/>
-    <mergeCell ref="AE6:AF6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="M7:N7"/>
-    <mergeCell ref="O7:P7"/>
-    <mergeCell ref="S7:T7"/>
-    <mergeCell ref="U7:V7"/>
-    <mergeCell ref="W7:X7"/>
-    <mergeCell ref="AA7:AB7"/>
-    <mergeCell ref="AC7:AD7"/>
-    <mergeCell ref="AE7:AF7"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="S10:T10"/>
-    <mergeCell ref="U10:V10"/>
-    <mergeCell ref="W10:X10"/>
-    <mergeCell ref="AA8:AB8"/>
-    <mergeCell ref="AC8:AD8"/>
-    <mergeCell ref="AE8:AF8"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="M9:N9"/>
-    <mergeCell ref="O9:P9"/>
-    <mergeCell ref="S9:T9"/>
-    <mergeCell ref="U9:V9"/>
-    <mergeCell ref="W9:X9"/>
-    <mergeCell ref="AA9:AB9"/>
-    <mergeCell ref="AC9:AD9"/>
-    <mergeCell ref="AE9:AF9"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="O8:P8"/>
-    <mergeCell ref="Y12:Z12"/>
-    <mergeCell ref="AA12:AB12"/>
-    <mergeCell ref="AC12:AD12"/>
-    <mergeCell ref="AA10:AB10"/>
-    <mergeCell ref="AC10:AD10"/>
-    <mergeCell ref="AE10:AF10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="M11:N11"/>
-    <mergeCell ref="O11:P11"/>
-    <mergeCell ref="S11:T11"/>
-    <mergeCell ref="U11:V11"/>
-    <mergeCell ref="W11:X11"/>
-    <mergeCell ref="AA11:AB11"/>
-    <mergeCell ref="AC11:AD11"/>
-    <mergeCell ref="AE11:AF11"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="M10:N10"/>
-    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="S4:T4"/>
+    <mergeCell ref="U4:V4"/>
+    <mergeCell ref="W4:X4"/>
+    <mergeCell ref="C2:H2"/>
+    <mergeCell ref="K2:P2"/>
+    <mergeCell ref="S2:X2"/>
+    <mergeCell ref="AA2:AF2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="S3:T3"/>
+    <mergeCell ref="U3:V3"/>
+    <mergeCell ref="W3:X3"/>
+    <mergeCell ref="AA3:AB3"/>
+    <mergeCell ref="AC3:AD3"/>
+    <mergeCell ref="AE3:AF3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -2149,23 +2149,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:CRC111"/>
   <sheetViews>
-    <sheetView topLeftCell="A48" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="R67" sqref="R67"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="AH20" sqref="AF20:AH20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="45.453125" style="7" customWidth="1"/>
-    <col min="2" max="2" width="26.54296875" style="7" customWidth="1"/>
-    <col min="3" max="3" width="19.08984375" style="7" customWidth="1"/>
-    <col min="4" max="4" width="17.6328125" style="7" customWidth="1"/>
-    <col min="5" max="5" width="17.6328125" style="8" customWidth="1"/>
-    <col min="6" max="7" width="8.6328125" style="7"/>
-    <col min="8" max="8" width="12.6328125" style="7" customWidth="1"/>
-    <col min="9" max="16384" width="8.6328125" style="7"/>
+    <col min="1" max="1" width="45.44140625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="26.5546875" style="7" customWidth="1"/>
+    <col min="3" max="3" width="19.109375" style="7" customWidth="1"/>
+    <col min="4" max="4" width="17.6640625" style="7" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" style="8" customWidth="1"/>
+    <col min="6" max="7" width="8.6640625" style="7"/>
+    <col min="8" max="8" width="12.6640625" style="7" customWidth="1"/>
+    <col min="9" max="16384" width="8.6640625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:65" s="9" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:65" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B1" s="9" t="s">
         <v>15</v>
       </c>
@@ -2191,11 +2191,11 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:65" s="14" customFormat="1" ht="21" x14ac:dyDescent="0.5">
-      <c r="A2" s="115" t="s">
+    <row r="2" spans="1:65" s="14" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+      <c r="A2" s="116" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="115"/>
+      <c r="B2" s="116"/>
       <c r="C2" s="79"/>
       <c r="E2" s="15"/>
       <c r="F2" s="14">
@@ -2379,7 +2379,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:65" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A3" s="16" t="s">
         <v>23</v>
       </c>
@@ -2396,7 +2396,7 @@
       <c r="H3" s="20"/>
       <c r="I3" s="20"/>
     </row>
-    <row r="4" spans="1:65" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A4" s="16" t="s">
         <v>25</v>
       </c>
@@ -2411,7 +2411,7 @@
       <c r="H4" s="19"/>
       <c r="I4" s="19"/>
     </row>
-    <row r="5" spans="1:65" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A5" s="16" t="s">
         <v>26</v>
       </c>
@@ -2422,13 +2422,13 @@
       <c r="D5" s="17">
         <v>1</v>
       </c>
-      <c r="E5" s="21"/>
-      <c r="H5" s="22"/>
-      <c r="I5" s="22"/>
-      <c r="J5" s="22"/>
-      <c r="K5" s="22"/>
-    </row>
-    <row r="6" spans="1:65" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="E5" s="18"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="19"/>
+      <c r="J5" s="19"/>
+      <c r="K5" s="19"/>
+    </row>
+    <row r="6" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A6" s="16" t="s">
         <v>27</v>
       </c>
@@ -2442,7 +2442,7 @@
       <c r="E6" s="18"/>
       <c r="J6" s="19"/>
     </row>
-    <row r="7" spans="1:65" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A7" s="16" t="s">
         <v>29</v>
       </c>
@@ -2457,7 +2457,7 @@
       <c r="J7" s="19"/>
       <c r="K7" s="19"/>
     </row>
-    <row r="8" spans="1:65" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A8" s="16" t="s">
         <v>30</v>
       </c>
@@ -2472,7 +2472,7 @@
       <c r="L8" s="19"/>
       <c r="M8" s="19"/>
     </row>
-    <row r="9" spans="1:65" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A9" s="16" t="s">
         <v>32</v>
       </c>
@@ -2487,7 +2487,7 @@
       <c r="N9" s="19"/>
       <c r="O9" s="19"/>
     </row>
-    <row r="10" spans="1:65" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A10" s="16" t="s">
         <v>34</v>
       </c>
@@ -2502,7 +2502,7 @@
       <c r="K10" s="19"/>
       <c r="L10" s="19"/>
     </row>
-    <row r="11" spans="1:65" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A11" s="16" t="s">
         <v>35</v>
       </c>
@@ -2513,13 +2513,13 @@
       <c r="D11" s="17">
         <v>3</v>
       </c>
-      <c r="E11" s="23"/>
-      <c r="L11" s="22"/>
-      <c r="M11" s="22"/>
-      <c r="N11" s="22"/>
-      <c r="O11" s="22"/>
-    </row>
-    <row r="12" spans="1:65" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="E11" s="18"/>
+      <c r="L11" s="19"/>
+      <c r="M11" s="19"/>
+      <c r="N11" s="19"/>
+      <c r="O11" s="19"/>
+    </row>
+    <row r="12" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A12" s="16" t="s">
         <v>36</v>
       </c>
@@ -2530,15 +2530,15 @@
       <c r="D12" s="17">
         <v>9</v>
       </c>
-      <c r="E12" s="23"/>
-      <c r="N12" s="24"/>
-      <c r="O12" s="24"/>
-      <c r="P12" s="24"/>
-      <c r="Q12" s="24"/>
-      <c r="R12" s="24"/>
-      <c r="S12" s="24"/>
-    </row>
-    <row r="13" spans="1:65" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="E12" s="18"/>
+      <c r="N12" s="19"/>
+      <c r="O12" s="19"/>
+      <c r="P12" s="19"/>
+      <c r="Q12" s="19"/>
+      <c r="R12" s="19"/>
+      <c r="S12" s="19"/>
+    </row>
+    <row r="13" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A13" s="16" t="s">
         <v>37</v>
       </c>
@@ -2549,12 +2549,12 @@
       <c r="D13" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="E13" s="21"/>
-      <c r="T13" s="22"/>
-      <c r="U13" s="22"/>
-      <c r="V13" s="22"/>
-    </row>
-    <row r="14" spans="1:65" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="E13" s="18"/>
+      <c r="T13" s="19"/>
+      <c r="U13" s="19"/>
+      <c r="V13" s="19"/>
+    </row>
+    <row r="14" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A14" s="16" t="s">
         <v>39</v>
       </c>
@@ -2565,11 +2565,11 @@
       <c r="D14" s="17">
         <v>8</v>
       </c>
-      <c r="E14" s="21"/>
-      <c r="M14" s="22"/>
-      <c r="N14" s="22"/>
-    </row>
-    <row r="15" spans="1:65" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="E14" s="18"/>
+      <c r="M14" s="19"/>
+      <c r="N14" s="19"/>
+    </row>
+    <row r="15" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A15" s="16" t="s">
         <v>40</v>
       </c>
@@ -2580,11 +2580,11 @@
       <c r="D15" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="E15" s="21"/>
+      <c r="E15" s="18"/>
       <c r="P15" s="19"/>
-      <c r="Q15" s="22"/>
-    </row>
-    <row r="16" spans="1:65" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="Q15" s="19"/>
+    </row>
+    <row r="16" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A16" s="16" t="s">
         <v>42</v>
       </c>
@@ -2595,11 +2595,11 @@
       <c r="D16" s="17">
         <v>12</v>
       </c>
-      <c r="E16" s="23"/>
-      <c r="O16" s="24"/>
-      <c r="P16" s="24"/>
-    </row>
-    <row r="17" spans="1:39" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="E16" s="18"/>
+      <c r="O16" s="19"/>
+      <c r="P16" s="19"/>
+    </row>
+    <row r="17" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A17" s="16" t="s">
         <v>43</v>
       </c>
@@ -2610,12 +2610,12 @@
       <c r="D17" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="E17" s="23"/>
-      <c r="W17" s="24"/>
-      <c r="X17" s="24"/>
-      <c r="Y17" s="24"/>
-    </row>
-    <row r="18" spans="1:39" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="E17" s="18"/>
+      <c r="W17" s="19"/>
+      <c r="X17" s="19"/>
+      <c r="Y17" s="19"/>
+    </row>
+    <row r="18" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A18" s="16" t="s">
         <v>45</v>
       </c>
@@ -2626,14 +2626,14 @@
       <c r="D18" s="17">
         <v>12</v>
       </c>
-      <c r="E18" s="23"/>
-      <c r="W18" s="24"/>
-      <c r="X18" s="24"/>
-      <c r="Y18" s="24"/>
-      <c r="Z18" s="24"/>
-      <c r="AA18" s="24"/>
-    </row>
-    <row r="19" spans="1:39" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="E18" s="18"/>
+      <c r="W18" s="19"/>
+      <c r="X18" s="19"/>
+      <c r="Y18" s="19"/>
+      <c r="Z18" s="19"/>
+      <c r="AA18" s="19"/>
+    </row>
+    <row r="19" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A19" s="16" t="s">
         <v>46</v>
       </c>
@@ -2644,13 +2644,13 @@
       <c r="D19" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="E19" s="23"/>
-      <c r="AB19" s="24"/>
-      <c r="AC19" s="24"/>
-      <c r="AD19" s="24"/>
-      <c r="AE19" s="24"/>
-    </row>
-    <row r="20" spans="1:39" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="E19" s="18"/>
+      <c r="AB19" s="19"/>
+      <c r="AC19" s="19"/>
+      <c r="AD19" s="19"/>
+      <c r="AE19" s="19"/>
+    </row>
+    <row r="20" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A20" s="16" t="s">
         <v>48</v>
       </c>
@@ -2661,12 +2661,12 @@
       <c r="D20" s="17">
         <v>17</v>
       </c>
-      <c r="E20" s="23"/>
-      <c r="AF20" s="24"/>
-      <c r="AG20" s="24"/>
-      <c r="AH20" s="24"/>
-    </row>
-    <row r="21" spans="1:39" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="E20" s="18"/>
+      <c r="AF20" s="19"/>
+      <c r="AG20" s="19"/>
+      <c r="AH20" s="19"/>
+    </row>
+    <row r="21" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A21" s="16" t="s">
         <v>49</v>
       </c>
@@ -2677,11 +2677,11 @@
       <c r="D21" s="17">
         <v>18</v>
       </c>
-      <c r="E21" s="23"/>
-      <c r="AI21" s="24"/>
-      <c r="AJ21" s="24"/>
-    </row>
-    <row r="22" spans="1:39" s="27" customFormat="1" ht="21" x14ac:dyDescent="0.5">
+      <c r="E21" s="18"/>
+      <c r="AI21" s="19"/>
+      <c r="AJ21" s="19"/>
+    </row>
+    <row r="22" spans="1:39" s="27" customFormat="1" ht="21" x14ac:dyDescent="0.4">
       <c r="A22" s="25" t="s">
         <v>50</v>
       </c>
@@ -2689,7 +2689,7 @@
       <c r="C22" s="26"/>
       <c r="E22" s="28"/>
     </row>
-    <row r="23" spans="1:39" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A23" s="16" t="s">
         <v>51</v>
       </c>
@@ -2704,7 +2704,7 @@
       <c r="F23" s="19"/>
       <c r="G23" s="19"/>
     </row>
-    <row r="24" spans="1:39" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A24" s="16" t="s">
         <v>52</v>
       </c>
@@ -2720,7 +2720,7 @@
       <c r="I24" s="19"/>
       <c r="J24" s="19"/>
     </row>
-    <row r="25" spans="1:39" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A25" s="16" t="s">
         <v>53</v>
       </c>
@@ -2737,7 +2737,7 @@
       <c r="M25" s="19"/>
       <c r="N25" s="19"/>
     </row>
-    <row r="26" spans="1:39" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A26" s="16" t="s">
         <v>54</v>
       </c>
@@ -2756,7 +2756,7 @@
       <c r="S26" s="19"/>
       <c r="T26" s="19"/>
     </row>
-    <row r="27" spans="1:39" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A27" s="16" t="s">
         <v>55</v>
       </c>
@@ -2772,7 +2772,7 @@
       <c r="V27" s="19"/>
       <c r="W27" s="19"/>
     </row>
-    <row r="28" spans="1:39" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A28" s="16" t="s">
         <v>57</v>
       </c>
@@ -2786,7 +2786,7 @@
       <c r="E28" s="18"/>
       <c r="X28" s="19"/>
     </row>
-    <row r="29" spans="1:39" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A29" s="16" t="s">
         <v>58</v>
       </c>
@@ -2804,7 +2804,7 @@
       <c r="AA29" s="19"/>
       <c r="AB29" s="19"/>
     </row>
-    <row r="30" spans="1:39" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A30" s="16" t="s">
         <v>59</v>
       </c>
@@ -2820,7 +2820,7 @@
       <c r="AD30" s="19"/>
       <c r="AE30" s="19"/>
     </row>
-    <row r="31" spans="1:39" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A31" s="16" t="s">
         <v>60</v>
       </c>
@@ -2839,7 +2839,7 @@
       <c r="AJ31" s="19"/>
       <c r="AK31" s="19"/>
     </row>
-    <row r="32" spans="1:39" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A32" s="16" t="s">
         <v>61</v>
       </c>
@@ -2854,7 +2854,7 @@
       <c r="AL32" s="22"/>
       <c r="AM32" s="22"/>
     </row>
-    <row r="33" spans="1:62" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:62" x14ac:dyDescent="0.35">
       <c r="A33" s="16" t="s">
         <v>62</v>
       </c>
@@ -2870,7 +2870,7 @@
       <c r="AD33" s="19"/>
       <c r="AE33" s="19"/>
     </row>
-    <row r="34" spans="1:62" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:62" x14ac:dyDescent="0.35">
       <c r="A34" s="16" t="s">
         <v>64</v>
       </c>
@@ -2889,7 +2889,7 @@
       <c r="AH34" s="80"/>
       <c r="AI34" s="80"/>
     </row>
-    <row r="35" spans="1:62" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:62" x14ac:dyDescent="0.35">
       <c r="A35" s="16" t="s">
         <v>65</v>
       </c>
@@ -2911,7 +2911,7 @@
       <c r="AS35" s="22"/>
       <c r="AT35" s="22"/>
     </row>
-    <row r="36" spans="1:62" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:62" x14ac:dyDescent="0.35">
       <c r="A36" s="16" t="s">
         <v>67</v>
       </c>
@@ -2928,7 +2928,7 @@
       <c r="AU36" s="83"/>
       <c r="AV36" s="83"/>
     </row>
-    <row r="37" spans="1:62" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:62" x14ac:dyDescent="0.35">
       <c r="A37" s="16" t="s">
         <v>68</v>
       </c>
@@ -2950,7 +2950,7 @@
       <c r="AK37" s="83"/>
       <c r="AL37" s="83"/>
     </row>
-    <row r="38" spans="1:62" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:62" x14ac:dyDescent="0.35">
       <c r="A38" s="16" t="s">
         <v>69</v>
       </c>
@@ -2973,7 +2973,7 @@
       <c r="BC38" s="83"/>
       <c r="BD38" s="83"/>
     </row>
-    <row r="39" spans="1:62" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:62" x14ac:dyDescent="0.35">
       <c r="A39" s="16" t="s">
         <v>70</v>
       </c>
@@ -2992,7 +2992,7 @@
       <c r="BI39" s="24"/>
       <c r="BJ39" s="24"/>
     </row>
-    <row r="40" spans="1:62" s="27" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="40" spans="1:62" s="27" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A40" s="25" t="s">
         <v>71</v>
       </c>
@@ -3000,7 +3000,7 @@
       <c r="C40" s="26"/>
       <c r="E40" s="28"/>
     </row>
-    <row r="41" spans="1:62" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:62" x14ac:dyDescent="0.35">
       <c r="A41" s="16" t="s">
         <v>72</v>
       </c>
@@ -3017,7 +3017,7 @@
       <c r="F41" s="19"/>
       <c r="G41" s="19"/>
     </row>
-    <row r="42" spans="1:62" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:62" x14ac:dyDescent="0.35">
       <c r="A42" s="16" t="s">
         <v>73</v>
       </c>
@@ -3034,7 +3034,7 @@
       <c r="H42" s="19"/>
       <c r="I42" s="19"/>
     </row>
-    <row r="43" spans="1:62" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:62" x14ac:dyDescent="0.35">
       <c r="A43" s="16" t="s">
         <v>74</v>
       </c>
@@ -3050,7 +3050,7 @@
       </c>
       <c r="J43" s="22"/>
     </row>
-    <row r="44" spans="1:62" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:62" x14ac:dyDescent="0.35">
       <c r="A44" s="16" t="s">
         <v>76</v>
       </c>
@@ -3069,7 +3069,7 @@
       <c r="L44" s="22"/>
       <c r="M44" s="22"/>
     </row>
-    <row r="45" spans="1:62" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:62" x14ac:dyDescent="0.35">
       <c r="A45" s="16" t="s">
         <v>78</v>
       </c>
@@ -3088,7 +3088,7 @@
       <c r="P45" s="22"/>
       <c r="Q45" s="22"/>
     </row>
-    <row r="46" spans="1:62" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:62" x14ac:dyDescent="0.35">
       <c r="A46" s="16" t="s">
         <v>81</v>
       </c>
@@ -3105,7 +3105,7 @@
       <c r="R46" s="22"/>
       <c r="S46" s="22"/>
     </row>
-    <row r="47" spans="1:62" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:62" x14ac:dyDescent="0.35">
       <c r="A47" s="16" t="s">
         <v>83</v>
       </c>
@@ -3122,7 +3122,7 @@
       <c r="T47" s="24"/>
       <c r="U47" s="24"/>
     </row>
-    <row r="48" spans="1:62" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:62" x14ac:dyDescent="0.35">
       <c r="A48" s="16" t="s">
         <v>84</v>
       </c>
@@ -3137,7 +3137,7 @@
       <c r="V48" s="24"/>
       <c r="W48" s="24"/>
     </row>
-    <row r="49" spans="1:50" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A49" s="16" t="s">
         <v>85</v>
       </c>
@@ -3152,7 +3152,7 @@
       <c r="X49" s="24"/>
       <c r="Y49" s="24"/>
     </row>
-    <row r="50" spans="1:50" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A50" s="16" t="s">
         <v>86</v>
       </c>
@@ -3166,7 +3166,7 @@
       <c r="E50" s="30"/>
       <c r="Z50" s="24"/>
     </row>
-    <row r="51" spans="1:50" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A51" s="16" t="s">
         <v>87</v>
       </c>
@@ -3183,7 +3183,7 @@
       <c r="AB51" s="24"/>
       <c r="AC51" s="24"/>
     </row>
-    <row r="52" spans="1:50" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A52" s="16" t="s">
         <v>88</v>
       </c>
@@ -3200,7 +3200,7 @@
       <c r="AF52" s="24"/>
       <c r="AG52" s="24"/>
     </row>
-    <row r="53" spans="1:50" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A53" s="16" t="s">
         <v>90</v>
       </c>
@@ -3215,7 +3215,7 @@
       <c r="AH53" s="24"/>
       <c r="AI53" s="24"/>
     </row>
-    <row r="54" spans="1:50" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A54" s="16" t="s">
         <v>92</v>
       </c>
@@ -3232,7 +3232,7 @@
       <c r="AJ54" s="24"/>
       <c r="AK54" s="24"/>
     </row>
-    <row r="55" spans="1:50" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A55" s="16" t="s">
         <v>93</v>
       </c>
@@ -3247,7 +3247,7 @@
       <c r="AL55" s="24"/>
       <c r="AM55" s="24"/>
     </row>
-    <row r="56" spans="1:50" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A56" s="16" t="s">
         <v>94</v>
       </c>
@@ -3262,7 +3262,7 @@
       <c r="AN56" s="24"/>
       <c r="AO56" s="24"/>
     </row>
-    <row r="57" spans="1:50" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A57" s="16" t="s">
         <v>95</v>
       </c>
@@ -3276,7 +3276,7 @@
       <c r="E57" s="30"/>
       <c r="AP57" s="24"/>
     </row>
-    <row r="58" spans="1:50" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A58" s="16" t="s">
         <v>96</v>
       </c>
@@ -3293,7 +3293,7 @@
       <c r="AS58" s="24"/>
       <c r="AT58" s="24"/>
     </row>
-    <row r="59" spans="1:50" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A59" s="16" t="s">
         <v>98</v>
       </c>
@@ -3308,7 +3308,7 @@
       <c r="AU59" s="24"/>
       <c r="AV59" s="24"/>
     </row>
-    <row r="60" spans="1:50" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A60" s="16" t="s">
         <v>100</v>
       </c>
@@ -3325,7 +3325,7 @@
       <c r="AW60" s="24"/>
       <c r="AX60" s="24"/>
     </row>
-    <row r="61" spans="1:50" s="27" customFormat="1" ht="21" x14ac:dyDescent="0.5">
+    <row r="61" spans="1:50" s="27" customFormat="1" ht="21" x14ac:dyDescent="0.4">
       <c r="A61" s="25" t="s">
         <v>101</v>
       </c>
@@ -3333,7 +3333,7 @@
       <c r="C61" s="26"/>
       <c r="E61" s="28"/>
     </row>
-    <row r="62" spans="1:50" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A62" s="7" t="s">
         <v>102</v>
       </c>
@@ -3350,7 +3350,7 @@
       <c r="H62" s="32"/>
       <c r="I62" s="32"/>
     </row>
-    <row r="63" spans="1:50" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A63" s="7" t="s">
         <v>103</v>
       </c>
@@ -3362,14 +3362,14 @@
         <v>1</v>
       </c>
       <c r="E63" s="30"/>
-      <c r="J63" s="119"/>
-      <c r="K63" s="119"/>
-      <c r="L63" s="119"/>
-      <c r="M63" s="119"/>
-      <c r="N63" s="119"/>
-      <c r="O63" s="119"/>
-    </row>
-    <row r="64" spans="1:50" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="J63" s="92"/>
+      <c r="K63" s="92"/>
+      <c r="L63" s="92"/>
+      <c r="M63" s="92"/>
+      <c r="N63" s="92"/>
+      <c r="O63" s="92"/>
+    </row>
+    <row r="64" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A64" s="7" t="s">
         <v>104</v>
       </c>
@@ -3381,16 +3381,16 @@
         <v>1</v>
       </c>
       <c r="E64" s="30"/>
-      <c r="J64" s="119"/>
-      <c r="K64" s="119"/>
-      <c r="L64" s="119"/>
-      <c r="M64" s="119"/>
-      <c r="N64" s="119"/>
-      <c r="O64" s="119"/>
-      <c r="P64" s="119"/>
-      <c r="Q64" s="119"/>
-    </row>
-    <row r="65" spans="1:43" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="J64" s="92"/>
+      <c r="K64" s="92"/>
+      <c r="L64" s="92"/>
+      <c r="M64" s="92"/>
+      <c r="N64" s="92"/>
+      <c r="O64" s="92"/>
+      <c r="P64" s="92"/>
+      <c r="Q64" s="92"/>
+    </row>
+    <row r="65" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A65" s="7" t="s">
         <v>105</v>
       </c>
@@ -3411,7 +3411,7 @@
       <c r="X65" s="77"/>
       <c r="Y65" s="77"/>
     </row>
-    <row r="66" spans="1:43" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A66" s="7" t="s">
         <v>106</v>
       </c>
@@ -3428,7 +3428,7 @@
       <c r="T66" s="77"/>
       <c r="U66" s="77"/>
     </row>
-    <row r="67" spans="1:43" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A67" s="7" t="s">
         <v>108</v>
       </c>
@@ -3449,7 +3449,7 @@
       <c r="X67" s="33"/>
       <c r="Y67" s="33"/>
     </row>
-    <row r="68" spans="1:43" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:43" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A68" s="7" t="s">
         <v>109</v>
       </c>
@@ -3466,7 +3466,7 @@
       <c r="AB68" s="33"/>
       <c r="AC68" s="33"/>
     </row>
-    <row r="69" spans="1:43" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A69" s="7" t="s">
         <v>111</v>
       </c>
@@ -3483,7 +3483,7 @@
       <c r="AB69" s="77"/>
       <c r="AC69" s="77"/>
     </row>
-    <row r="70" spans="1:43" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A70" s="7" t="s">
         <v>112</v>
       </c>
@@ -3499,7 +3499,7 @@
       <c r="AE70" s="77"/>
       <c r="AF70" s="77"/>
     </row>
-    <row r="71" spans="1:43" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A71" s="7" t="s">
         <v>113</v>
       </c>
@@ -3515,7 +3515,7 @@
       <c r="AH71" s="33"/>
       <c r="AI71" s="33"/>
     </row>
-    <row r="72" spans="1:43" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A72" s="7" t="s">
         <v>115</v>
       </c>
@@ -3532,7 +3532,7 @@
       <c r="AL72" s="33"/>
       <c r="AM72" s="33"/>
     </row>
-    <row r="73" spans="1:43" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A73" s="7" t="s">
         <v>116</v>
       </c>
@@ -3549,7 +3549,7 @@
       <c r="AP73" s="33"/>
       <c r="AQ73" s="33"/>
     </row>
-    <row r="74" spans="1:43" s="27" customFormat="1" ht="21" x14ac:dyDescent="0.5">
+    <row r="74" spans="1:43" s="27" customFormat="1" ht="21" x14ac:dyDescent="0.4">
       <c r="A74" s="25" t="s">
         <v>117</v>
       </c>
@@ -3557,7 +3557,7 @@
       <c r="C74" s="34"/>
       <c r="E74" s="28"/>
     </row>
-    <row r="75" spans="1:43" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A75" s="16" t="s">
         <v>118</v>
       </c>
@@ -3579,7 +3579,7 @@
       <c r="K75" s="19"/>
       <c r="L75" s="80"/>
     </row>
-    <row r="76" spans="1:43" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A76" s="16" t="s">
         <v>119</v>
       </c>
@@ -3599,7 +3599,7 @@
       <c r="R76" s="80"/>
       <c r="S76" s="22"/>
     </row>
-    <row r="77" spans="1:43" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A77" s="16" t="s">
         <v>120</v>
       </c>
@@ -3623,7 +3623,7 @@
       <c r="T77" s="80"/>
       <c r="U77" s="89"/>
     </row>
-    <row r="78" spans="1:43" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A78" s="16" t="s">
         <v>121</v>
       </c>
@@ -3642,7 +3642,7 @@
       <c r="V78" s="86"/>
       <c r="W78" s="86"/>
     </row>
-    <row r="79" spans="1:43" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A79" s="16" t="s">
         <v>123</v>
       </c>
@@ -3664,7 +3664,7 @@
       <c r="AC79" s="86"/>
       <c r="AD79" s="89"/>
     </row>
-    <row r="80" spans="1:43" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A80" s="16" t="s">
         <v>124</v>
       </c>
@@ -3683,7 +3683,7 @@
       <c r="AB80" s="83"/>
       <c r="AC80" s="83"/>
     </row>
-    <row r="81" spans="1:46" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A81" s="16" t="s">
         <v>125</v>
       </c>
@@ -3701,7 +3701,7 @@
       <c r="AH81" s="90"/>
       <c r="AI81" s="91"/>
     </row>
-    <row r="82" spans="1:46" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A82" s="16" t="s">
         <v>127</v>
       </c>
@@ -3720,7 +3720,7 @@
       <c r="AN82" s="90"/>
       <c r="AO82" s="91"/>
     </row>
-    <row r="83" spans="1:46" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A83" s="16" t="s">
         <v>128</v>
       </c>
@@ -3739,7 +3739,7 @@
       <c r="AP83" s="90"/>
       <c r="AQ83" s="91"/>
     </row>
-    <row r="84" spans="1:46" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A84" s="16" t="s">
         <v>129</v>
       </c>
@@ -3791,7 +3791,7 @@
       <c r="AO84" s="36"/>
       <c r="AP84" s="36"/>
     </row>
-    <row r="85" spans="1:46" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A85" s="16" t="s">
         <v>130</v>
       </c>
@@ -3807,7 +3807,7 @@
       <c r="AS85" s="90"/>
       <c r="AT85" s="91"/>
     </row>
-    <row r="86" spans="1:46" s="27" customFormat="1" ht="21" x14ac:dyDescent="0.5">
+    <row r="86" spans="1:46" s="27" customFormat="1" ht="21" x14ac:dyDescent="0.4">
       <c r="A86" s="25" t="s">
         <v>132</v>
       </c>
@@ -3815,7 +3815,7 @@
       <c r="C86" s="26"/>
       <c r="E86" s="28"/>
     </row>
-    <row r="87" spans="1:46" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A87" s="16" t="s">
         <v>133</v>
       </c>
@@ -3851,7 +3851,7 @@
       <c r="AA87" s="39"/>
       <c r="AB87" s="39"/>
     </row>
-    <row r="88" spans="1:46" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A88" s="16" t="s">
         <v>134</v>
       </c>
@@ -3887,7 +3887,7 @@
       <c r="AA88" s="39"/>
       <c r="AB88" s="39"/>
     </row>
-    <row r="89" spans="1:46" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A89" s="16" t="s">
         <v>135</v>
       </c>
@@ -3923,7 +3923,7 @@
       <c r="AA89" s="39"/>
       <c r="AB89" s="39"/>
     </row>
-    <row r="90" spans="1:46" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A90" s="16" t="s">
         <v>136</v>
       </c>
@@ -3959,7 +3959,7 @@
       <c r="AA90" s="39"/>
       <c r="AB90" s="39"/>
     </row>
-    <row r="91" spans="1:46" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A91" s="16" t="s">
         <v>137</v>
       </c>
@@ -3995,7 +3995,7 @@
       <c r="AA91" s="39"/>
       <c r="AB91" s="39"/>
     </row>
-    <row r="92" spans="1:46" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A92" s="16" t="s">
         <v>139</v>
       </c>
@@ -4029,7 +4029,7 @@
       <c r="AA92" s="39"/>
       <c r="AB92" s="39"/>
     </row>
-    <row r="93" spans="1:46" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A93" s="16" t="s">
         <v>141</v>
       </c>
@@ -4063,7 +4063,7 @@
       <c r="AA93" s="39"/>
       <c r="AB93" s="39"/>
     </row>
-    <row r="94" spans="1:46" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A94" s="16" t="s">
         <v>142</v>
       </c>
@@ -4099,7 +4099,7 @@
       <c r="AA94" s="39"/>
       <c r="AB94" s="39"/>
     </row>
-    <row r="95" spans="1:46" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A95" s="16" t="s">
         <v>144</v>
       </c>
@@ -4135,7 +4135,7 @@
       <c r="Y95" s="76"/>
       <c r="Z95" s="76"/>
     </row>
-    <row r="96" spans="1:46" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A96" s="16" t="s">
         <v>145</v>
       </c>
@@ -4150,7 +4150,7 @@
       <c r="Y96" s="77"/>
       <c r="Z96" s="77"/>
     </row>
-    <row r="97" spans="1:2499" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:2499" x14ac:dyDescent="0.35">
       <c r="A97" s="16" t="s">
         <v>146</v>
       </c>
@@ -4173,7 +4173,7 @@
       <c r="AI97" s="78"/>
       <c r="AJ97" s="78"/>
     </row>
-    <row r="98" spans="1:2499" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:2499" x14ac:dyDescent="0.35">
       <c r="A98" s="7" t="s">
         <v>147</v>
       </c>
@@ -4187,7 +4187,7 @@
       <c r="E98" s="41"/>
       <c r="AJ98" s="78"/>
     </row>
-    <row r="99" spans="1:2499" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:2499" x14ac:dyDescent="0.35">
       <c r="A99" s="7" t="s">
         <v>148</v>
       </c>
@@ -4205,7 +4205,7 @@
       <c r="AN99" s="33"/>
       <c r="AO99" s="33"/>
     </row>
-    <row r="100" spans="1:2499" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:2499" x14ac:dyDescent="0.35">
       <c r="A100" s="7" t="s">
         <v>149</v>
       </c>
@@ -4220,7 +4220,7 @@
       <c r="AP100" s="33"/>
       <c r="AQ100" s="33"/>
     </row>
-    <row r="101" spans="1:2499" s="42" customFormat="1" ht="21" x14ac:dyDescent="0.5">
+    <row r="101" spans="1:2499" s="42" customFormat="1" ht="21" x14ac:dyDescent="0.4">
       <c r="A101" s="25" t="s">
         <v>150</v>
       </c>
@@ -6723,7 +6723,7 @@
       <c r="CRB101" s="27"/>
       <c r="CRC101" s="27"/>
     </row>
-    <row r="102" spans="1:2499" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:2499" x14ac:dyDescent="0.35">
       <c r="A102" s="43" t="s">
         <v>151</v>
       </c>
@@ -6738,7 +6738,7 @@
       <c r="F102" s="19"/>
       <c r="G102" s="19"/>
     </row>
-    <row r="103" spans="1:2499" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:2499" x14ac:dyDescent="0.35">
       <c r="A103" s="43" t="s">
         <v>152</v>
       </c>
@@ -6756,7 +6756,7 @@
       <c r="K103" s="19"/>
       <c r="L103" s="19"/>
     </row>
-    <row r="104" spans="1:2499" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:2499" x14ac:dyDescent="0.35">
       <c r="A104" s="43" t="s">
         <v>153</v>
       </c>
@@ -6774,7 +6774,7 @@
       <c r="K104" s="19"/>
       <c r="L104" s="19"/>
     </row>
-    <row r="105" spans="1:2499" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:2499" x14ac:dyDescent="0.35">
       <c r="A105" s="43" t="s">
         <v>154</v>
       </c>
@@ -6792,7 +6792,7 @@
       <c r="K105" s="19"/>
       <c r="L105" s="19"/>
     </row>
-    <row r="106" spans="1:2499" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:2499" x14ac:dyDescent="0.35">
       <c r="A106" s="43" t="s">
         <v>155</v>
       </c>
@@ -6818,7 +6818,7 @@
       <c r="S106" s="19"/>
       <c r="T106" s="19"/>
     </row>
-    <row r="107" spans="1:2499" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:2499" x14ac:dyDescent="0.35">
       <c r="A107" s="43" t="s">
         <v>156</v>
       </c>
@@ -6836,7 +6836,7 @@
       <c r="X107" s="24"/>
       <c r="Y107" s="24"/>
     </row>
-    <row r="108" spans="1:2499" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:2499" x14ac:dyDescent="0.35">
       <c r="A108" s="43" t="s">
         <v>158</v>
       </c>
@@ -6854,7 +6854,7 @@
       <c r="AC108" s="24"/>
       <c r="AD108" s="24"/>
     </row>
-    <row r="109" spans="1:2499" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:2499" x14ac:dyDescent="0.35">
       <c r="A109" s="43" t="s">
         <v>159</v>
       </c>
@@ -6873,7 +6873,7 @@
       <c r="AI109" s="24"/>
       <c r="AJ109" s="24"/>
     </row>
-    <row r="110" spans="1:2499" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:2499" x14ac:dyDescent="0.35">
       <c r="A110" s="43" t="s">
         <v>160</v>
       </c>
@@ -6892,7 +6892,7 @@
       <c r="AO110" s="24"/>
       <c r="AP110" s="24"/>
     </row>
-    <row r="111" spans="1:2499" s="42" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:2499" s="42" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A111" s="45" t="s">
         <v>162</v>
       </c>
@@ -6926,294 +6926,294 @@
       <selection activeCell="E2" sqref="E2:G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="118" t="s">
+    <row r="2" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="117" t="s">
         <v>163</v>
       </c>
-      <c r="C2" s="118"/>
-      <c r="D2" s="118"/>
-      <c r="E2" s="118" t="s">
+      <c r="C2" s="117"/>
+      <c r="D2" s="117"/>
+      <c r="E2" s="117" t="s">
         <v>164</v>
       </c>
-      <c r="F2" s="118"/>
-      <c r="G2" s="118"/>
-      <c r="H2" s="118" t="s">
+      <c r="F2" s="117"/>
+      <c r="G2" s="117"/>
+      <c r="H2" s="117" t="s">
         <v>165</v>
       </c>
-      <c r="I2" s="118"/>
-      <c r="J2" s="118"/>
-      <c r="K2" s="118" t="s">
+      <c r="I2" s="117"/>
+      <c r="J2" s="117"/>
+      <c r="K2" s="117" t="s">
         <v>166</v>
       </c>
-      <c r="L2" s="118"/>
-      <c r="M2" s="118"/>
-      <c r="N2" s="118" t="s">
+      <c r="L2" s="117"/>
+      <c r="M2" s="117"/>
+      <c r="N2" s="117" t="s">
         <v>167</v>
       </c>
-      <c r="O2" s="118"/>
-      <c r="P2" s="118"/>
-      <c r="Q2" s="118" t="s">
+      <c r="O2" s="117"/>
+      <c r="P2" s="117"/>
+      <c r="Q2" s="117" t="s">
         <v>168</v>
       </c>
-      <c r="R2" s="118"/>
-      <c r="S2" s="118"/>
-    </row>
-    <row r="3" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="117" t="s">
+      <c r="R2" s="117"/>
+      <c r="S2" s="117"/>
+    </row>
+    <row r="3" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="118" t="s">
         <v>169</v>
       </c>
-      <c r="C3" s="117"/>
-      <c r="D3" s="117"/>
-      <c r="E3" s="117" t="s">
+      <c r="C3" s="118"/>
+      <c r="D3" s="118"/>
+      <c r="E3" s="118" t="s">
         <v>169</v>
       </c>
-      <c r="F3" s="117"/>
-      <c r="G3" s="117"/>
-      <c r="H3" s="117" t="s">
+      <c r="F3" s="118"/>
+      <c r="G3" s="118"/>
+      <c r="H3" s="118" t="s">
         <v>169</v>
       </c>
-      <c r="I3" s="117"/>
-      <c r="J3" s="117"/>
-      <c r="K3" s="117" t="s">
+      <c r="I3" s="118"/>
+      <c r="J3" s="118"/>
+      <c r="K3" s="118" t="s">
         <v>169</v>
       </c>
-      <c r="L3" s="117"/>
-      <c r="M3" s="117"/>
-      <c r="N3" s="117" t="s">
+      <c r="L3" s="118"/>
+      <c r="M3" s="118"/>
+      <c r="N3" s="118" t="s">
         <v>169</v>
       </c>
-      <c r="O3" s="117"/>
-      <c r="P3" s="117"/>
-      <c r="Q3" s="117" t="s">
+      <c r="O3" s="118"/>
+      <c r="P3" s="118"/>
+      <c r="Q3" s="118" t="s">
         <v>169</v>
       </c>
-      <c r="R3" s="117"/>
-      <c r="S3" s="117"/>
-    </row>
-    <row r="4" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="116"/>
-      <c r="C4" s="116"/>
-      <c r="D4" s="116"/>
-      <c r="E4" s="116"/>
-      <c r="F4" s="116"/>
-      <c r="G4" s="116"/>
-      <c r="H4" s="116"/>
-      <c r="I4" s="116"/>
-      <c r="J4" s="116"/>
-      <c r="K4" s="116"/>
-      <c r="L4" s="116"/>
-      <c r="M4" s="116"/>
-      <c r="N4" s="116"/>
-      <c r="O4" s="116"/>
-      <c r="P4" s="116"/>
-      <c r="Q4" s="116"/>
-      <c r="R4" s="116"/>
-      <c r="S4" s="116"/>
-    </row>
-    <row r="5" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="116"/>
-      <c r="C5" s="116"/>
-      <c r="D5" s="116"/>
-      <c r="E5" s="116"/>
-      <c r="F5" s="116"/>
-      <c r="G5" s="116"/>
-      <c r="H5" s="116"/>
-      <c r="I5" s="116"/>
-      <c r="J5" s="116"/>
-      <c r="K5" s="116"/>
-      <c r="L5" s="116"/>
-      <c r="M5" s="116"/>
-      <c r="N5" s="116"/>
-      <c r="O5" s="116"/>
-      <c r="P5" s="116"/>
-      <c r="Q5" s="116"/>
-      <c r="R5" s="116"/>
-      <c r="S5" s="116"/>
-    </row>
-    <row r="6" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="116"/>
-      <c r="C6" s="116"/>
-      <c r="D6" s="116"/>
-      <c r="E6" s="116"/>
-      <c r="F6" s="116"/>
-      <c r="G6" s="116"/>
-      <c r="H6" s="116"/>
-      <c r="I6" s="116"/>
-      <c r="J6" s="116"/>
-      <c r="K6" s="116"/>
-      <c r="L6" s="116"/>
-      <c r="M6" s="116"/>
-      <c r="N6" s="116"/>
-      <c r="O6" s="116"/>
-      <c r="P6" s="116"/>
-      <c r="Q6" s="116"/>
-      <c r="R6" s="116"/>
-      <c r="S6" s="116"/>
-    </row>
-    <row r="7" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="116"/>
-      <c r="C7" s="116"/>
-      <c r="D7" s="116"/>
-      <c r="E7" s="116"/>
-      <c r="F7" s="116"/>
-      <c r="G7" s="116"/>
-      <c r="H7" s="116"/>
-      <c r="I7" s="116"/>
-      <c r="J7" s="116"/>
-      <c r="K7" s="116"/>
-      <c r="L7" s="116"/>
-      <c r="M7" s="116"/>
-      <c r="N7" s="116"/>
-      <c r="O7" s="116"/>
-      <c r="P7" s="116"/>
-      <c r="Q7" s="116"/>
-      <c r="R7" s="116"/>
-      <c r="S7" s="116"/>
-    </row>
-    <row r="8" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="116"/>
-      <c r="C8" s="116"/>
-      <c r="D8" s="116"/>
-      <c r="E8" s="116"/>
-      <c r="F8" s="116"/>
-      <c r="G8" s="116"/>
-      <c r="H8" s="116"/>
-      <c r="I8" s="116"/>
-      <c r="J8" s="116"/>
-      <c r="K8" s="116"/>
-      <c r="L8" s="116"/>
-      <c r="M8" s="116"/>
-      <c r="N8" s="116"/>
-      <c r="O8" s="116"/>
-      <c r="P8" s="116"/>
-      <c r="Q8" s="116"/>
-      <c r="R8" s="116"/>
-      <c r="S8" s="116"/>
-    </row>
-    <row r="9" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="116"/>
-      <c r="C9" s="116"/>
-      <c r="D9" s="116"/>
-      <c r="E9" s="116"/>
-      <c r="F9" s="116"/>
-      <c r="G9" s="116"/>
-      <c r="H9" s="116"/>
-      <c r="I9" s="116"/>
-      <c r="J9" s="116"/>
-      <c r="K9" s="116"/>
-      <c r="L9" s="116"/>
-      <c r="M9" s="116"/>
-      <c r="N9" s="116"/>
-      <c r="O9" s="116"/>
-      <c r="P9" s="116"/>
-      <c r="Q9" s="116"/>
-      <c r="R9" s="116"/>
-      <c r="S9" s="116"/>
-    </row>
-    <row r="10" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="116"/>
-      <c r="C10" s="116"/>
-      <c r="D10" s="116"/>
-      <c r="E10" s="116"/>
-      <c r="F10" s="116"/>
-      <c r="G10" s="116"/>
-      <c r="H10" s="116"/>
-      <c r="I10" s="116"/>
-      <c r="J10" s="116"/>
-      <c r="K10" s="116"/>
-      <c r="L10" s="116"/>
-      <c r="M10" s="116"/>
-      <c r="N10" s="116"/>
-      <c r="O10" s="116"/>
-      <c r="P10" s="116"/>
-      <c r="Q10" s="116"/>
-      <c r="R10" s="116"/>
-      <c r="S10" s="116"/>
-    </row>
-    <row r="11" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="116"/>
-      <c r="C11" s="116"/>
-      <c r="D11" s="116"/>
-      <c r="E11" s="116"/>
-      <c r="F11" s="116"/>
-      <c r="G11" s="116"/>
-      <c r="H11" s="116"/>
-      <c r="I11" s="116"/>
-      <c r="J11" s="116"/>
-      <c r="K11" s="116"/>
-      <c r="L11" s="116"/>
-      <c r="M11" s="116"/>
-      <c r="N11" s="116"/>
-      <c r="O11" s="116"/>
-      <c r="P11" s="116"/>
-      <c r="Q11" s="116"/>
-      <c r="R11" s="116"/>
-      <c r="S11" s="116"/>
-    </row>
-    <row r="12" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="116"/>
-      <c r="C12" s="116"/>
-      <c r="D12" s="116"/>
-      <c r="E12" s="116"/>
-      <c r="F12" s="116"/>
-      <c r="G12" s="116"/>
-      <c r="H12" s="116"/>
-      <c r="I12" s="116"/>
-      <c r="J12" s="116"/>
-      <c r="K12" s="116"/>
-      <c r="L12" s="116"/>
-      <c r="M12" s="116"/>
-      <c r="N12" s="116"/>
-      <c r="O12" s="116"/>
-      <c r="P12" s="116"/>
-      <c r="Q12" s="116"/>
-      <c r="R12" s="116"/>
-      <c r="S12" s="116"/>
-    </row>
-    <row r="13" spans="1:19" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="B13" s="116"/>
-      <c r="C13" s="116"/>
-      <c r="D13" s="116"/>
-      <c r="E13" s="116"/>
-      <c r="F13" s="116"/>
-      <c r="G13" s="116"/>
-      <c r="H13" s="116"/>
-      <c r="I13" s="116"/>
-      <c r="J13" s="116"/>
-      <c r="K13" s="116"/>
-      <c r="L13" s="116"/>
-      <c r="M13" s="116"/>
-      <c r="N13" s="116"/>
-      <c r="O13" s="116"/>
-      <c r="P13" s="116"/>
-      <c r="Q13" s="116"/>
-      <c r="R13" s="116"/>
-      <c r="S13" s="116"/>
-    </row>
-    <row r="14" spans="1:19" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="R3" s="118"/>
+      <c r="S3" s="118"/>
+    </row>
+    <row r="4" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="119"/>
+      <c r="C4" s="119"/>
+      <c r="D4" s="119"/>
+      <c r="E4" s="119"/>
+      <c r="F4" s="119"/>
+      <c r="G4" s="119"/>
+      <c r="H4" s="119"/>
+      <c r="I4" s="119"/>
+      <c r="J4" s="119"/>
+      <c r="K4" s="119"/>
+      <c r="L4" s="119"/>
+      <c r="M4" s="119"/>
+      <c r="N4" s="119"/>
+      <c r="O4" s="119"/>
+      <c r="P4" s="119"/>
+      <c r="Q4" s="119"/>
+      <c r="R4" s="119"/>
+      <c r="S4" s="119"/>
+    </row>
+    <row r="5" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="119"/>
+      <c r="C5" s="119"/>
+      <c r="D5" s="119"/>
+      <c r="E5" s="119"/>
+      <c r="F5" s="119"/>
+      <c r="G5" s="119"/>
+      <c r="H5" s="119"/>
+      <c r="I5" s="119"/>
+      <c r="J5" s="119"/>
+      <c r="K5" s="119"/>
+      <c r="L5" s="119"/>
+      <c r="M5" s="119"/>
+      <c r="N5" s="119"/>
+      <c r="O5" s="119"/>
+      <c r="P5" s="119"/>
+      <c r="Q5" s="119"/>
+      <c r="R5" s="119"/>
+      <c r="S5" s="119"/>
+    </row>
+    <row r="6" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="119"/>
+      <c r="C6" s="119"/>
+      <c r="D6" s="119"/>
+      <c r="E6" s="119"/>
+      <c r="F6" s="119"/>
+      <c r="G6" s="119"/>
+      <c r="H6" s="119"/>
+      <c r="I6" s="119"/>
+      <c r="J6" s="119"/>
+      <c r="K6" s="119"/>
+      <c r="L6" s="119"/>
+      <c r="M6" s="119"/>
+      <c r="N6" s="119"/>
+      <c r="O6" s="119"/>
+      <c r="P6" s="119"/>
+      <c r="Q6" s="119"/>
+      <c r="R6" s="119"/>
+      <c r="S6" s="119"/>
+    </row>
+    <row r="7" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="119"/>
+      <c r="C7" s="119"/>
+      <c r="D7" s="119"/>
+      <c r="E7" s="119"/>
+      <c r="F7" s="119"/>
+      <c r="G7" s="119"/>
+      <c r="H7" s="119"/>
+      <c r="I7" s="119"/>
+      <c r="J7" s="119"/>
+      <c r="K7" s="119"/>
+      <c r="L7" s="119"/>
+      <c r="M7" s="119"/>
+      <c r="N7" s="119"/>
+      <c r="O7" s="119"/>
+      <c r="P7" s="119"/>
+      <c r="Q7" s="119"/>
+      <c r="R7" s="119"/>
+      <c r="S7" s="119"/>
+    </row>
+    <row r="8" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="119"/>
+      <c r="C8" s="119"/>
+      <c r="D8" s="119"/>
+      <c r="E8" s="119"/>
+      <c r="F8" s="119"/>
+      <c r="G8" s="119"/>
+      <c r="H8" s="119"/>
+      <c r="I8" s="119"/>
+      <c r="J8" s="119"/>
+      <c r="K8" s="119"/>
+      <c r="L8" s="119"/>
+      <c r="M8" s="119"/>
+      <c r="N8" s="119"/>
+      <c r="O8" s="119"/>
+      <c r="P8" s="119"/>
+      <c r="Q8" s="119"/>
+      <c r="R8" s="119"/>
+      <c r="S8" s="119"/>
+    </row>
+    <row r="9" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="119"/>
+      <c r="C9" s="119"/>
+      <c r="D9" s="119"/>
+      <c r="E9" s="119"/>
+      <c r="F9" s="119"/>
+      <c r="G9" s="119"/>
+      <c r="H9" s="119"/>
+      <c r="I9" s="119"/>
+      <c r="J9" s="119"/>
+      <c r="K9" s="119"/>
+      <c r="L9" s="119"/>
+      <c r="M9" s="119"/>
+      <c r="N9" s="119"/>
+      <c r="O9" s="119"/>
+      <c r="P9" s="119"/>
+      <c r="Q9" s="119"/>
+      <c r="R9" s="119"/>
+      <c r="S9" s="119"/>
+    </row>
+    <row r="10" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="119"/>
+      <c r="C10" s="119"/>
+      <c r="D10" s="119"/>
+      <c r="E10" s="119"/>
+      <c r="F10" s="119"/>
+      <c r="G10" s="119"/>
+      <c r="H10" s="119"/>
+      <c r="I10" s="119"/>
+      <c r="J10" s="119"/>
+      <c r="K10" s="119"/>
+      <c r="L10" s="119"/>
+      <c r="M10" s="119"/>
+      <c r="N10" s="119"/>
+      <c r="O10" s="119"/>
+      <c r="P10" s="119"/>
+      <c r="Q10" s="119"/>
+      <c r="R10" s="119"/>
+      <c r="S10" s="119"/>
+    </row>
+    <row r="11" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="119"/>
+      <c r="C11" s="119"/>
+      <c r="D11" s="119"/>
+      <c r="E11" s="119"/>
+      <c r="F11" s="119"/>
+      <c r="G11" s="119"/>
+      <c r="H11" s="119"/>
+      <c r="I11" s="119"/>
+      <c r="J11" s="119"/>
+      <c r="K11" s="119"/>
+      <c r="L11" s="119"/>
+      <c r="M11" s="119"/>
+      <c r="N11" s="119"/>
+      <c r="O11" s="119"/>
+      <c r="P11" s="119"/>
+      <c r="Q11" s="119"/>
+      <c r="R11" s="119"/>
+      <c r="S11" s="119"/>
+    </row>
+    <row r="12" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="119"/>
+      <c r="C12" s="119"/>
+      <c r="D12" s="119"/>
+      <c r="E12" s="119"/>
+      <c r="F12" s="119"/>
+      <c r="G12" s="119"/>
+      <c r="H12" s="119"/>
+      <c r="I12" s="119"/>
+      <c r="J12" s="119"/>
+      <c r="K12" s="119"/>
+      <c r="L12" s="119"/>
+      <c r="M12" s="119"/>
+      <c r="N12" s="119"/>
+      <c r="O12" s="119"/>
+      <c r="P12" s="119"/>
+      <c r="Q12" s="119"/>
+      <c r="R12" s="119"/>
+      <c r="S12" s="119"/>
+    </row>
+    <row r="13" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="B13" s="119"/>
+      <c r="C13" s="119"/>
+      <c r="D13" s="119"/>
+      <c r="E13" s="119"/>
+      <c r="F13" s="119"/>
+      <c r="G13" s="119"/>
+      <c r="H13" s="119"/>
+      <c r="I13" s="119"/>
+      <c r="J13" s="119"/>
+      <c r="K13" s="119"/>
+      <c r="L13" s="119"/>
+      <c r="M13" s="119"/>
+      <c r="N13" s="119"/>
+      <c r="O13" s="119"/>
+      <c r="P13" s="119"/>
+      <c r="Q13" s="119"/>
+      <c r="R13" s="119"/>
+      <c r="S13" s="119"/>
+    </row>
+    <row r="14" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A14" s="49"/>
-      <c r="B14" s="117"/>
-      <c r="C14" s="117"/>
-      <c r="D14" s="117"/>
-      <c r="E14" s="117"/>
-      <c r="F14" s="117"/>
-      <c r="G14" s="117"/>
-      <c r="H14" s="117"/>
-      <c r="I14" s="117"/>
-      <c r="J14" s="117"/>
-      <c r="K14" s="117"/>
-      <c r="L14" s="117"/>
-      <c r="M14" s="117"/>
-      <c r="N14" s="117"/>
-      <c r="O14" s="117"/>
-      <c r="P14" s="117"/>
-      <c r="Q14" s="117"/>
-      <c r="R14" s="117"/>
-      <c r="S14" s="117"/>
-    </row>
-    <row r="15" spans="1:19" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B14" s="118"/>
+      <c r="C14" s="118"/>
+      <c r="D14" s="118"/>
+      <c r="E14" s="118"/>
+      <c r="F14" s="118"/>
+      <c r="G14" s="118"/>
+      <c r="H14" s="118"/>
+      <c r="I14" s="118"/>
+      <c r="J14" s="118"/>
+      <c r="K14" s="118"/>
+      <c r="L14" s="118"/>
+      <c r="M14" s="118"/>
+      <c r="N14" s="118"/>
+      <c r="O14" s="118"/>
+      <c r="P14" s="118"/>
+      <c r="Q14" s="118"/>
+      <c r="R14" s="118"/>
+      <c r="S14" s="118"/>
+    </row>
+    <row r="15" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B15" s="50" t="s">
         <v>170</v>
       </c>
@@ -7228,6 +7228,18 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="Q4:S13"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="H14:J14"/>
+    <mergeCell ref="K14:M14"/>
+    <mergeCell ref="N14:P14"/>
+    <mergeCell ref="Q14:S14"/>
+    <mergeCell ref="B4:D13"/>
+    <mergeCell ref="E4:G13"/>
+    <mergeCell ref="H4:J13"/>
+    <mergeCell ref="K4:M13"/>
+    <mergeCell ref="N4:P13"/>
     <mergeCell ref="Q2:S2"/>
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="E3:G3"/>
@@ -7240,18 +7252,6 @@
     <mergeCell ref="H2:J2"/>
     <mergeCell ref="K2:M2"/>
     <mergeCell ref="N2:P2"/>
-    <mergeCell ref="Q4:S13"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="H14:J14"/>
-    <mergeCell ref="K14:M14"/>
-    <mergeCell ref="N14:P14"/>
-    <mergeCell ref="Q14:S14"/>
-    <mergeCell ref="B4:D13"/>
-    <mergeCell ref="E4:G13"/>
-    <mergeCell ref="H4:J13"/>
-    <mergeCell ref="K4:M13"/>
-    <mergeCell ref="N4:P13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -7262,16 +7262,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B2:O12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="6" max="6" width="11.6328125" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:15" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:15" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B2" s="52"/>
       <c r="C2" s="53" t="s">
         <v>171</v>
@@ -7296,7 +7296,7 @@
       <c r="K2" s="54"/>
       <c r="L2" s="57"/>
     </row>
-    <row r="3" spans="2:15" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:15" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B3" s="52"/>
       <c r="C3" s="58" t="s">
         <v>177</v>
@@ -7321,7 +7321,7 @@
       <c r="K3" s="59"/>
       <c r="L3" s="60"/>
     </row>
-    <row r="4" spans="2:15" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:15" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B4" s="52" t="s">
         <v>181</v>
       </c>
@@ -7348,7 +7348,7 @@
       <c r="K4" s="62"/>
       <c r="L4" s="63"/>
     </row>
-    <row r="5" spans="2:15" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:15" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B5" s="64" t="s">
         <v>7</v>
       </c>
@@ -7375,7 +7375,7 @@
       <c r="K5" s="65"/>
       <c r="L5" s="65"/>
     </row>
-    <row r="6" spans="2:15" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:15" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B6" s="66" t="s">
         <v>9</v>
       </c>
@@ -7405,7 +7405,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="2:15" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:15" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B7" s="66" t="s">
         <v>183</v>
       </c>
@@ -7435,7 +7435,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="2:15" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:15" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B8" s="66" t="s">
         <v>11</v>
       </c>
@@ -7465,7 +7465,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="2:15" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:15" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B9" s="66" t="s">
         <v>184</v>
       </c>
@@ -7495,7 +7495,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:15" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:15" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B10" s="66" t="s">
         <v>13</v>
       </c>
@@ -7522,7 +7522,7 @@
       <c r="K10" s="65"/>
       <c r="L10" s="65"/>
     </row>
-    <row r="11" spans="2:15" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:15" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B11" s="68" t="s">
         <v>14</v>
       </c>
@@ -7549,7 +7549,7 @@
       <c r="K11" s="52"/>
       <c r="L11" s="52"/>
     </row>
-    <row r="12" spans="2:15" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:15" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B12" s="69" t="s">
         <v>0</v>
       </c>

</xml_diff>